<commit_message>
Az oldal eszközfüggetlenné tétele
</commit_message>
<xml_diff>
--- a/egyebek/WebprogramozásBeadandóHtmlCssBootstrap.xlsx
+++ b/egyebek/WebprogramozásBeadandóHtmlCssBootstrap.xlsx
@@ -1,16 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28623"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="H:\9.osztály\Programozás\Webprogramozás\Beadandó\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Latitude\OneDrive\Dokumentumok\Suli\Közgáz\Programozás\Webprogramozás\Beadandó\egyebek\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{596C2795-AD96-4370-95AB-6176D5585F2B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Fedőlap" sheetId="2" r:id="rId1"/>
@@ -21,7 +20,7 @@
     <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">Irányelvek!$A$1:$L$39</definedName>
     <definedName name="nem_modosithato2">Irányelvek!$J:$J,Irányelvek!$I:$I,Irányelvek!$H$1,Irányelvek!$G:$G,Irányelvek!$H:$H,Irányelvek!$F:$F,Irányelvek!$C:$C,Irányelvek!$B:$B,Irányelvek!$A:$A</definedName>
   </definedNames>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
@@ -307,11 +306,11 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <numFmts count="3">
-    <numFmt numFmtId="164" formatCode="_-* #,##0.00\ _F_t_-;\-* #,##0.00\ _F_t_-;_-* &quot;-&quot;??\ _F_t_-;_-@_-"/>
-    <numFmt numFmtId="165" formatCode=";;;"/>
-    <numFmt numFmtId="166" formatCode="#,##0_ ;\-#,##0\ "/>
+    <numFmt numFmtId="43" formatCode="_-* #,##0.00\ _F_t_-;\-* #,##0.00\ _F_t_-;_-* &quot;-&quot;??\ _F_t_-;_-@_-"/>
+    <numFmt numFmtId="164" formatCode=";;;"/>
+    <numFmt numFmtId="165" formatCode="#,##0_ ;\-#,##0\ "/>
   </numFmts>
   <fonts count="22" x14ac:knownFonts="1">
     <font>
@@ -1008,7 +1007,7 @@
   </borders>
   <cellStyleXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="top"/>
       <protection locked="0"/>
@@ -1024,38 +1023,38 @@
       <alignment horizontal="right" vertical="top"/>
     </xf>
     <xf numFmtId="9" fontId="7" fillId="0" borderId="0" xfId="3" applyFont="1"/>
-    <xf numFmtId="165" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
     <xf numFmtId="9" fontId="7" fillId="0" borderId="1" xfId="3" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="166" fontId="7" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="7" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="4" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
-    <xf numFmtId="165" fontId="5" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="164" fontId="5" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="right" vertical="top"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="165" fontId="7" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="164" fontId="7" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment wrapText="1"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="165" fontId="4" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment wrapText="1"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="165" fontId="7" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="164" fontId="7" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment wrapText="1"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyProtection="1">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyProtection="1">
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1" applyProtection="1">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1" applyProtection="1">
       <protection locked="0"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyProtection="1">
@@ -1099,7 +1098,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="165" fontId="5" fillId="3" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="164" fontId="5" fillId="3" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="right" vertical="top"/>
       <protection locked="0"/>
     </xf>
@@ -1110,11 +1109,11 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="165" fontId="4" fillId="0" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment wrapText="1"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="165" fontId="7" fillId="0" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="164" fontId="7" fillId="0" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment wrapText="1"/>
       <protection locked="0"/>
     </xf>
@@ -1141,21 +1140,21 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="165" fontId="4" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment wrapText="1"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="165" fontId="7" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="164" fontId="7" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment wrapText="1"/>
       <protection locked="0"/>
     </xf>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="17" xfId="0" applyNumberFormat="1" applyBorder="1" applyProtection="1">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="17" xfId="0" applyNumberFormat="1" applyBorder="1" applyProtection="1">
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyBorder="1" applyProtection="1">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyBorder="1" applyProtection="1">
       <protection locked="0"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyBorder="1"/>
@@ -1188,13 +1187,25 @@
     <xf numFmtId="0" fontId="4" fillId="7" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="7" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="7" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="165" fontId="2" fillId="0" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="164" fontId="2" fillId="0" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment wrapText="1"/>
       <protection locked="0"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="11" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="21" fillId="11" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1240,18 +1251,6 @@
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="17" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
   </cellXfs>
   <cellStyles count="4">
     <cellStyle name="Ezres" xfId="1" builtinId="3"/>
@@ -1304,19 +1303,19 @@
 </file>
 
 <file path=xl/ctrlProps/ctrlProp10.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" fmlaLink="D11" lockText="1" noThreeD="1"/>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" checked="Checked" fmlaLink="D11" lockText="1" noThreeD="1"/>
 </file>
 
 <file path=xl/ctrlProps/ctrlProp11.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" fmlaLink="D12" lockText="1" noThreeD="1"/>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" checked="Checked" fmlaLink="D12" lockText="1" noThreeD="1"/>
 </file>
 
 <file path=xl/ctrlProps/ctrlProp12.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" fmlaLink="D13" lockText="1" noThreeD="1"/>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" checked="Checked" fmlaLink="D13" lockText="1" noThreeD="1"/>
 </file>
 
 <file path=xl/ctrlProps/ctrlProp13.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" fmlaLink="D14" lockText="1" noThreeD="1"/>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" checked="Checked" fmlaLink="D14" lockText="1" noThreeD="1"/>
 </file>
 
 <file path=xl/ctrlProps/ctrlProp14.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1332,11 +1331,11 @@
 </file>
 
 <file path=xl/ctrlProps/ctrlProp17.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" fmlaLink="D18" lockText="1" noThreeD="1"/>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" checked="Checked" fmlaLink="D18" lockText="1" noThreeD="1"/>
 </file>
 
 <file path=xl/ctrlProps/ctrlProp18.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" fmlaLink="D19" lockText="1" noThreeD="1"/>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" checked="Checked" fmlaLink="D19" lockText="1" noThreeD="1"/>
 </file>
 
 <file path=xl/ctrlProps/ctrlProp19.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1344,19 +1343,19 @@
 </file>
 
 <file path=xl/ctrlProps/ctrlProp2.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" fmlaLink="D3" lockText="1" noThreeD="1"/>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" checked="Checked" fmlaLink="D3" lockText="1" noThreeD="1"/>
 </file>
 
 <file path=xl/ctrlProps/ctrlProp20.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" fmlaLink="D21" lockText="1" noThreeD="1"/>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" checked="Checked" fmlaLink="D21" lockText="1" noThreeD="1"/>
 </file>
 
 <file path=xl/ctrlProps/ctrlProp21.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" fmlaLink="D22" lockText="1" noThreeD="1"/>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" checked="Checked" fmlaLink="D22" lockText="1" noThreeD="1"/>
 </file>
 
 <file path=xl/ctrlProps/ctrlProp22.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" fmlaLink="D23" lockText="1" noThreeD="1"/>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" checked="Checked" fmlaLink="D23" lockText="1" noThreeD="1"/>
 </file>
 
 <file path=xl/ctrlProps/ctrlProp23.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1364,7 +1363,7 @@
 </file>
 
 <file path=xl/ctrlProps/ctrlProp24.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" fmlaLink="D25" lockText="1" noThreeD="1"/>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" checked="Checked" fmlaLink="D25" lockText="1" noThreeD="1"/>
 </file>
 
 <file path=xl/ctrlProps/ctrlProp25.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1372,19 +1371,19 @@
 </file>
 
 <file path=xl/ctrlProps/ctrlProp26.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" fmlaLink="D27" lockText="1" noThreeD="1"/>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" checked="Checked" fmlaLink="D27" lockText="1" noThreeD="1"/>
 </file>
 
 <file path=xl/ctrlProps/ctrlProp27.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" fmlaLink="D28" lockText="1" noThreeD="1"/>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" checked="Checked" fmlaLink="D28" lockText="1" noThreeD="1"/>
 </file>
 
 <file path=xl/ctrlProps/ctrlProp28.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" fmlaLink="D29" lockText="1" noThreeD="1"/>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" checked="Checked" fmlaLink="D29" lockText="1" noThreeD="1"/>
 </file>
 
 <file path=xl/ctrlProps/ctrlProp29.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" fmlaLink="D30" lockText="1" noThreeD="1"/>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" checked="Checked" fmlaLink="D30" lockText="1" noThreeD="1"/>
 </file>
 
 <file path=xl/ctrlProps/ctrlProp3.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1392,7 +1391,7 @@
 </file>
 
 <file path=xl/ctrlProps/ctrlProp30.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" fmlaLink="D31" lockText="1" noThreeD="1"/>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" checked="Checked" fmlaLink="D31" lockText="1" noThreeD="1"/>
 </file>
 
 <file path=xl/ctrlProps/ctrlProp31.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1400,11 +1399,11 @@
 </file>
 
 <file path=xl/ctrlProps/ctrlProp32.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" fmlaLink="D33" lockText="1" noThreeD="1"/>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" checked="Checked" fmlaLink="D33" lockText="1" noThreeD="1"/>
 </file>
 
 <file path=xl/ctrlProps/ctrlProp33.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" fmlaLink="D34" lockText="1" noThreeD="1"/>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" checked="Checked" fmlaLink="D34" lockText="1" noThreeD="1"/>
 </file>
 
 <file path=xl/ctrlProps/ctrlProp34.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1596,11 +1595,11 @@
 </file>
 
 <file path=xl/ctrlProps/ctrlProp8.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" fmlaLink="D9" lockText="1" noThreeD="1"/>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" checked="Checked" fmlaLink="D9" lockText="1" noThreeD="1"/>
 </file>
 
 <file path=xl/ctrlProps/ctrlProp9.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" fmlaLink="D10" lockText="1" noThreeD="1"/>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" checked="Checked" fmlaLink="D10" lockText="1" noThreeD="1"/>
 </file>
 
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1691,7 +1690,7 @@
         </xdr:from>
         <xdr:to>
           <xdr:col>4</xdr:col>
-          <xdr:colOff>104775</xdr:colOff>
+          <xdr:colOff>107950</xdr:colOff>
           <xdr:row>1</xdr:row>
           <xdr:rowOff>209550</xdr:rowOff>
         </xdr:to>
@@ -1742,7 +1741,7 @@
             </a:extLst>
           </xdr:spPr>
           <xdr:txBody>
-            <a:bodyPr vertOverflow="clip" wrap="square" lIns="27432" tIns="18288" rIns="0" bIns="18288" anchor="ctr" upright="1"/>
+            <a:bodyPr vertOverflow="clip" wrap="square" lIns="36576" tIns="22860" rIns="0" bIns="22860" anchor="ctr" upright="1"/>
             <a:lstStyle/>
             <a:p>
               <a:pPr algn="l" rtl="0">
@@ -1778,7 +1777,7 @@
         </xdr:from>
         <xdr:to>
           <xdr:col>4</xdr:col>
-          <xdr:colOff>104775</xdr:colOff>
+          <xdr:colOff>107950</xdr:colOff>
           <xdr:row>2</xdr:row>
           <xdr:rowOff>209550</xdr:rowOff>
         </xdr:to>
@@ -1829,7 +1828,7 @@
             </a:extLst>
           </xdr:spPr>
           <xdr:txBody>
-            <a:bodyPr vertOverflow="clip" wrap="square" lIns="27432" tIns="18288" rIns="0" bIns="18288" anchor="ctr" upright="1"/>
+            <a:bodyPr vertOverflow="clip" wrap="square" lIns="36576" tIns="22860" rIns="0" bIns="22860" anchor="ctr" upright="1"/>
             <a:lstStyle/>
             <a:p>
               <a:pPr algn="l" rtl="0">
@@ -1865,7 +1864,7 @@
         </xdr:from>
         <xdr:to>
           <xdr:col>4</xdr:col>
-          <xdr:colOff>104775</xdr:colOff>
+          <xdr:colOff>107950</xdr:colOff>
           <xdr:row>3</xdr:row>
           <xdr:rowOff>381000</xdr:rowOff>
         </xdr:to>
@@ -1916,7 +1915,7 @@
             </a:extLst>
           </xdr:spPr>
           <xdr:txBody>
-            <a:bodyPr vertOverflow="clip" wrap="square" lIns="27432" tIns="18288" rIns="0" bIns="18288" anchor="ctr" upright="1"/>
+            <a:bodyPr vertOverflow="clip" wrap="square" lIns="36576" tIns="22860" rIns="0" bIns="22860" anchor="ctr" upright="1"/>
             <a:lstStyle/>
             <a:p>
               <a:pPr algn="l" rtl="0">
@@ -1952,9 +1951,9 @@
         </xdr:from>
         <xdr:to>
           <xdr:col>4</xdr:col>
-          <xdr:colOff>104775</xdr:colOff>
+          <xdr:colOff>107950</xdr:colOff>
           <xdr:row>4</xdr:row>
-          <xdr:rowOff>714375</xdr:rowOff>
+          <xdr:rowOff>717550</xdr:rowOff>
         </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
@@ -2003,7 +2002,7 @@
             </a:extLst>
           </xdr:spPr>
           <xdr:txBody>
-            <a:bodyPr vertOverflow="clip" wrap="square" lIns="27432" tIns="18288" rIns="0" bIns="18288" anchor="ctr" upright="1"/>
+            <a:bodyPr vertOverflow="clip" wrap="square" lIns="36576" tIns="22860" rIns="0" bIns="22860" anchor="ctr" upright="1"/>
             <a:lstStyle/>
             <a:p>
               <a:pPr algn="l" rtl="0">
@@ -2033,7 +2032,7 @@
       <xdr:twoCellAnchor editAs="oneCell">
         <xdr:from>
           <xdr:col>3</xdr:col>
-          <xdr:colOff>28575</xdr:colOff>
+          <xdr:colOff>31750</xdr:colOff>
           <xdr:row>5</xdr:row>
           <xdr:rowOff>19050</xdr:rowOff>
         </xdr:from>
@@ -2090,7 +2089,7 @@
             </a:extLst>
           </xdr:spPr>
           <xdr:txBody>
-            <a:bodyPr vertOverflow="clip" wrap="square" lIns="27432" tIns="18288" rIns="0" bIns="18288" anchor="ctr" upright="1"/>
+            <a:bodyPr vertOverflow="clip" wrap="square" lIns="36576" tIns="22860" rIns="0" bIns="22860" anchor="ctr" upright="1"/>
             <a:lstStyle/>
             <a:p>
               <a:pPr algn="l" rtl="0">
@@ -2126,9 +2125,9 @@
         </xdr:from>
         <xdr:to>
           <xdr:col>4</xdr:col>
-          <xdr:colOff>104775</xdr:colOff>
+          <xdr:colOff>107950</xdr:colOff>
           <xdr:row>7</xdr:row>
-          <xdr:rowOff>66675</xdr:rowOff>
+          <xdr:rowOff>69850</xdr:rowOff>
         </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
@@ -2177,7 +2176,7 @@
             </a:extLst>
           </xdr:spPr>
           <xdr:txBody>
-            <a:bodyPr vertOverflow="clip" wrap="square" lIns="27432" tIns="18288" rIns="0" bIns="18288" anchor="ctr" upright="1"/>
+            <a:bodyPr vertOverflow="clip" wrap="square" lIns="36576" tIns="22860" rIns="0" bIns="22860" anchor="ctr" upright="1"/>
             <a:lstStyle/>
             <a:p>
               <a:pPr algn="l" rtl="0">
@@ -2213,7 +2212,7 @@
         </xdr:from>
         <xdr:to>
           <xdr:col>4</xdr:col>
-          <xdr:colOff>104775</xdr:colOff>
+          <xdr:colOff>107950</xdr:colOff>
           <xdr:row>7</xdr:row>
           <xdr:rowOff>209550</xdr:rowOff>
         </xdr:to>
@@ -2264,7 +2263,7 @@
             </a:extLst>
           </xdr:spPr>
           <xdr:txBody>
-            <a:bodyPr vertOverflow="clip" wrap="square" lIns="27432" tIns="18288" rIns="0" bIns="18288" anchor="ctr" upright="1"/>
+            <a:bodyPr vertOverflow="clip" wrap="square" lIns="36576" tIns="22860" rIns="0" bIns="22860" anchor="ctr" upright="1"/>
             <a:lstStyle/>
             <a:p>
               <a:pPr algn="l" rtl="0">
@@ -2300,9 +2299,9 @@
         </xdr:from>
         <xdr:to>
           <xdr:col>4</xdr:col>
-          <xdr:colOff>104775</xdr:colOff>
+          <xdr:colOff>107950</xdr:colOff>
           <xdr:row>8</xdr:row>
-          <xdr:rowOff>123825</xdr:rowOff>
+          <xdr:rowOff>127000</xdr:rowOff>
         </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
@@ -2351,7 +2350,7 @@
             </a:extLst>
           </xdr:spPr>
           <xdr:txBody>
-            <a:bodyPr vertOverflow="clip" wrap="square" lIns="27432" tIns="18288" rIns="0" bIns="18288" anchor="ctr" upright="1"/>
+            <a:bodyPr vertOverflow="clip" wrap="square" lIns="36576" tIns="22860" rIns="0" bIns="22860" anchor="ctr" upright="1"/>
             <a:lstStyle/>
             <a:p>
               <a:pPr algn="l" rtl="0">
@@ -2387,7 +2386,7 @@
         </xdr:from>
         <xdr:to>
           <xdr:col>4</xdr:col>
-          <xdr:colOff>104775</xdr:colOff>
+          <xdr:colOff>107950</xdr:colOff>
           <xdr:row>10</xdr:row>
           <xdr:rowOff>0</xdr:rowOff>
         </xdr:to>
@@ -2438,7 +2437,7 @@
             </a:extLst>
           </xdr:spPr>
           <xdr:txBody>
-            <a:bodyPr vertOverflow="clip" wrap="square" lIns="27432" tIns="18288" rIns="0" bIns="18288" anchor="ctr" upright="1"/>
+            <a:bodyPr vertOverflow="clip" wrap="square" lIns="36576" tIns="22860" rIns="0" bIns="22860" anchor="ctr" upright="1"/>
             <a:lstStyle/>
             <a:p>
               <a:pPr algn="l" rtl="0">
@@ -2474,7 +2473,7 @@
         </xdr:from>
         <xdr:to>
           <xdr:col>4</xdr:col>
-          <xdr:colOff>104775</xdr:colOff>
+          <xdr:colOff>107950</xdr:colOff>
           <xdr:row>11</xdr:row>
           <xdr:rowOff>0</xdr:rowOff>
         </xdr:to>
@@ -2525,7 +2524,7 @@
             </a:extLst>
           </xdr:spPr>
           <xdr:txBody>
-            <a:bodyPr vertOverflow="clip" wrap="square" lIns="27432" tIns="18288" rIns="0" bIns="18288" anchor="ctr" upright="1"/>
+            <a:bodyPr vertOverflow="clip" wrap="square" lIns="36576" tIns="22860" rIns="0" bIns="22860" anchor="ctr" upright="1"/>
             <a:lstStyle/>
             <a:p>
               <a:pPr algn="l" rtl="0">
@@ -2561,7 +2560,7 @@
         </xdr:from>
         <xdr:to>
           <xdr:col>4</xdr:col>
-          <xdr:colOff>104775</xdr:colOff>
+          <xdr:colOff>107950</xdr:colOff>
           <xdr:row>11</xdr:row>
           <xdr:rowOff>209550</xdr:rowOff>
         </xdr:to>
@@ -2612,7 +2611,7 @@
             </a:extLst>
           </xdr:spPr>
           <xdr:txBody>
-            <a:bodyPr vertOverflow="clip" wrap="square" lIns="27432" tIns="18288" rIns="0" bIns="18288" anchor="ctr" upright="1"/>
+            <a:bodyPr vertOverflow="clip" wrap="square" lIns="36576" tIns="22860" rIns="0" bIns="22860" anchor="ctr" upright="1"/>
             <a:lstStyle/>
             <a:p>
               <a:pPr algn="l" rtl="0">
@@ -2648,7 +2647,7 @@
         </xdr:from>
         <xdr:to>
           <xdr:col>3</xdr:col>
-          <xdr:colOff>657225</xdr:colOff>
+          <xdr:colOff>660400</xdr:colOff>
           <xdr:row>12</xdr:row>
           <xdr:rowOff>571500</xdr:rowOff>
         </xdr:to>
@@ -2699,7 +2698,7 @@
             </a:extLst>
           </xdr:spPr>
           <xdr:txBody>
-            <a:bodyPr vertOverflow="clip" wrap="square" lIns="27432" tIns="18288" rIns="0" bIns="18288" anchor="ctr" upright="1"/>
+            <a:bodyPr vertOverflow="clip" wrap="square" lIns="36576" tIns="22860" rIns="0" bIns="22860" anchor="ctr" upright="1"/>
             <a:lstStyle/>
             <a:p>
               <a:pPr algn="l" rtl="0">
@@ -2735,7 +2734,7 @@
         </xdr:from>
         <xdr:to>
           <xdr:col>4</xdr:col>
-          <xdr:colOff>104775</xdr:colOff>
+          <xdr:colOff>107950</xdr:colOff>
           <xdr:row>13</xdr:row>
           <xdr:rowOff>381000</xdr:rowOff>
         </xdr:to>
@@ -2786,7 +2785,7 @@
             </a:extLst>
           </xdr:spPr>
           <xdr:txBody>
-            <a:bodyPr vertOverflow="clip" wrap="square" lIns="27432" tIns="18288" rIns="0" bIns="18288" anchor="ctr" upright="1"/>
+            <a:bodyPr vertOverflow="clip" wrap="square" lIns="36576" tIns="22860" rIns="0" bIns="22860" anchor="ctr" upright="1"/>
             <a:lstStyle/>
             <a:p>
               <a:pPr algn="l" rtl="0">
@@ -2822,7 +2821,7 @@
         </xdr:from>
         <xdr:to>
           <xdr:col>4</xdr:col>
-          <xdr:colOff>104775</xdr:colOff>
+          <xdr:colOff>107950</xdr:colOff>
           <xdr:row>14</xdr:row>
           <xdr:rowOff>209550</xdr:rowOff>
         </xdr:to>
@@ -2873,7 +2872,7 @@
             </a:extLst>
           </xdr:spPr>
           <xdr:txBody>
-            <a:bodyPr vertOverflow="clip" wrap="square" lIns="27432" tIns="18288" rIns="0" bIns="18288" anchor="ctr" upright="1"/>
+            <a:bodyPr vertOverflow="clip" wrap="square" lIns="36576" tIns="22860" rIns="0" bIns="22860" anchor="ctr" upright="1"/>
             <a:lstStyle/>
             <a:p>
               <a:pPr algn="l" rtl="0">
@@ -2909,9 +2908,9 @@
         </xdr:from>
         <xdr:to>
           <xdr:col>4</xdr:col>
-          <xdr:colOff>104775</xdr:colOff>
+          <xdr:colOff>107950</xdr:colOff>
           <xdr:row>15</xdr:row>
-          <xdr:rowOff>333375</xdr:rowOff>
+          <xdr:rowOff>336550</xdr:rowOff>
         </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
@@ -2960,7 +2959,7 @@
             </a:extLst>
           </xdr:spPr>
           <xdr:txBody>
-            <a:bodyPr vertOverflow="clip" wrap="square" lIns="27432" tIns="18288" rIns="0" bIns="18288" anchor="ctr" upright="1"/>
+            <a:bodyPr vertOverflow="clip" wrap="square" lIns="36576" tIns="22860" rIns="0" bIns="22860" anchor="ctr" upright="1"/>
             <a:lstStyle/>
             <a:p>
               <a:pPr algn="l" rtl="0">
@@ -2996,7 +2995,7 @@
         </xdr:from>
         <xdr:to>
           <xdr:col>4</xdr:col>
-          <xdr:colOff>104775</xdr:colOff>
+          <xdr:colOff>107950</xdr:colOff>
           <xdr:row>17</xdr:row>
           <xdr:rowOff>0</xdr:rowOff>
         </xdr:to>
@@ -3047,7 +3046,7 @@
             </a:extLst>
           </xdr:spPr>
           <xdr:txBody>
-            <a:bodyPr vertOverflow="clip" wrap="square" lIns="27432" tIns="18288" rIns="0" bIns="18288" anchor="ctr" upright="1"/>
+            <a:bodyPr vertOverflow="clip" wrap="square" lIns="36576" tIns="22860" rIns="0" bIns="22860" anchor="ctr" upright="1"/>
             <a:lstStyle/>
             <a:p>
               <a:pPr algn="l" rtl="0">
@@ -3083,9 +3082,9 @@
         </xdr:from>
         <xdr:to>
           <xdr:col>4</xdr:col>
-          <xdr:colOff>104775</xdr:colOff>
+          <xdr:colOff>107950</xdr:colOff>
           <xdr:row>17</xdr:row>
-          <xdr:rowOff>123825</xdr:rowOff>
+          <xdr:rowOff>127000</xdr:rowOff>
         </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
@@ -3134,7 +3133,7 @@
             </a:extLst>
           </xdr:spPr>
           <xdr:txBody>
-            <a:bodyPr vertOverflow="clip" wrap="square" lIns="27432" tIns="18288" rIns="0" bIns="18288" anchor="ctr" upright="1"/>
+            <a:bodyPr vertOverflow="clip" wrap="square" lIns="36576" tIns="22860" rIns="0" bIns="22860" anchor="ctr" upright="1"/>
             <a:lstStyle/>
             <a:p>
               <a:pPr algn="l" rtl="0">
@@ -3170,7 +3169,7 @@
         </xdr:from>
         <xdr:to>
           <xdr:col>4</xdr:col>
-          <xdr:colOff>104775</xdr:colOff>
+          <xdr:colOff>107950</xdr:colOff>
           <xdr:row>18</xdr:row>
           <xdr:rowOff>133350</xdr:rowOff>
         </xdr:to>
@@ -3221,7 +3220,7 @@
             </a:extLst>
           </xdr:spPr>
           <xdr:txBody>
-            <a:bodyPr vertOverflow="clip" wrap="square" lIns="27432" tIns="18288" rIns="0" bIns="18288" anchor="ctr" upright="1"/>
+            <a:bodyPr vertOverflow="clip" wrap="square" lIns="36576" tIns="22860" rIns="0" bIns="22860" anchor="ctr" upright="1"/>
             <a:lstStyle/>
             <a:p>
               <a:pPr algn="l" rtl="0">
@@ -3257,7 +3256,7 @@
         </xdr:from>
         <xdr:to>
           <xdr:col>4</xdr:col>
-          <xdr:colOff>104775</xdr:colOff>
+          <xdr:colOff>107950</xdr:colOff>
           <xdr:row>20</xdr:row>
           <xdr:rowOff>0</xdr:rowOff>
         </xdr:to>
@@ -3308,7 +3307,7 @@
             </a:extLst>
           </xdr:spPr>
           <xdr:txBody>
-            <a:bodyPr vertOverflow="clip" wrap="square" lIns="27432" tIns="18288" rIns="0" bIns="18288" anchor="ctr" upright="1"/>
+            <a:bodyPr vertOverflow="clip" wrap="square" lIns="36576" tIns="22860" rIns="0" bIns="22860" anchor="ctr" upright="1"/>
             <a:lstStyle/>
             <a:p>
               <a:pPr algn="l" rtl="0">
@@ -3344,7 +3343,7 @@
         </xdr:from>
         <xdr:to>
           <xdr:col>4</xdr:col>
-          <xdr:colOff>104775</xdr:colOff>
+          <xdr:colOff>107950</xdr:colOff>
           <xdr:row>20</xdr:row>
           <xdr:rowOff>209550</xdr:rowOff>
         </xdr:to>
@@ -3395,7 +3394,7 @@
             </a:extLst>
           </xdr:spPr>
           <xdr:txBody>
-            <a:bodyPr vertOverflow="clip" wrap="square" lIns="27432" tIns="18288" rIns="0" bIns="18288" anchor="ctr" upright="1"/>
+            <a:bodyPr vertOverflow="clip" wrap="square" lIns="36576" tIns="22860" rIns="0" bIns="22860" anchor="ctr" upright="1"/>
             <a:lstStyle/>
             <a:p>
               <a:pPr algn="l" rtl="0">
@@ -3431,7 +3430,7 @@
         </xdr:from>
         <xdr:to>
           <xdr:col>4</xdr:col>
-          <xdr:colOff>104775</xdr:colOff>
+          <xdr:colOff>107950</xdr:colOff>
           <xdr:row>22</xdr:row>
           <xdr:rowOff>0</xdr:rowOff>
         </xdr:to>
@@ -3482,7 +3481,7 @@
             </a:extLst>
           </xdr:spPr>
           <xdr:txBody>
-            <a:bodyPr vertOverflow="clip" wrap="square" lIns="27432" tIns="18288" rIns="0" bIns="18288" anchor="ctr" upright="1"/>
+            <a:bodyPr vertOverflow="clip" wrap="square" lIns="36576" tIns="22860" rIns="0" bIns="22860" anchor="ctr" upright="1"/>
             <a:lstStyle/>
             <a:p>
               <a:pPr algn="l" rtl="0">
@@ -3518,7 +3517,7 @@
         </xdr:from>
         <xdr:to>
           <xdr:col>4</xdr:col>
-          <xdr:colOff>104775</xdr:colOff>
+          <xdr:colOff>107950</xdr:colOff>
           <xdr:row>22</xdr:row>
           <xdr:rowOff>209550</xdr:rowOff>
         </xdr:to>
@@ -3569,7 +3568,7 @@
             </a:extLst>
           </xdr:spPr>
           <xdr:txBody>
-            <a:bodyPr vertOverflow="clip" wrap="square" lIns="27432" tIns="18288" rIns="0" bIns="18288" anchor="ctr" upright="1"/>
+            <a:bodyPr vertOverflow="clip" wrap="square" lIns="36576" tIns="22860" rIns="0" bIns="22860" anchor="ctr" upright="1"/>
             <a:lstStyle/>
             <a:p>
               <a:pPr algn="l" rtl="0">
@@ -3605,7 +3604,7 @@
         </xdr:from>
         <xdr:to>
           <xdr:col>4</xdr:col>
-          <xdr:colOff>104775</xdr:colOff>
+          <xdr:colOff>107950</xdr:colOff>
           <xdr:row>23</xdr:row>
           <xdr:rowOff>209550</xdr:rowOff>
         </xdr:to>
@@ -3656,7 +3655,7 @@
             </a:extLst>
           </xdr:spPr>
           <xdr:txBody>
-            <a:bodyPr vertOverflow="clip" wrap="square" lIns="27432" tIns="18288" rIns="0" bIns="18288" anchor="ctr" upright="1"/>
+            <a:bodyPr vertOverflow="clip" wrap="square" lIns="36576" tIns="22860" rIns="0" bIns="22860" anchor="ctr" upright="1"/>
             <a:lstStyle/>
             <a:p>
               <a:pPr algn="l" rtl="0">
@@ -3692,9 +3691,9 @@
         </xdr:from>
         <xdr:to>
           <xdr:col>4</xdr:col>
-          <xdr:colOff>104775</xdr:colOff>
+          <xdr:colOff>107950</xdr:colOff>
           <xdr:row>24</xdr:row>
-          <xdr:rowOff>123825</xdr:rowOff>
+          <xdr:rowOff>127000</xdr:rowOff>
         </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
@@ -3743,7 +3742,7 @@
             </a:extLst>
           </xdr:spPr>
           <xdr:txBody>
-            <a:bodyPr vertOverflow="clip" wrap="square" lIns="27432" tIns="18288" rIns="0" bIns="18288" anchor="ctr" upright="1"/>
+            <a:bodyPr vertOverflow="clip" wrap="square" lIns="36576" tIns="22860" rIns="0" bIns="22860" anchor="ctr" upright="1"/>
             <a:lstStyle/>
             <a:p>
               <a:pPr algn="l" rtl="0">
@@ -3779,7 +3778,7 @@
         </xdr:from>
         <xdr:to>
           <xdr:col>4</xdr:col>
-          <xdr:colOff>104775</xdr:colOff>
+          <xdr:colOff>107950</xdr:colOff>
           <xdr:row>26</xdr:row>
           <xdr:rowOff>0</xdr:rowOff>
         </xdr:to>
@@ -3830,7 +3829,7 @@
             </a:extLst>
           </xdr:spPr>
           <xdr:txBody>
-            <a:bodyPr vertOverflow="clip" wrap="square" lIns="27432" tIns="18288" rIns="0" bIns="18288" anchor="ctr" upright="1"/>
+            <a:bodyPr vertOverflow="clip" wrap="square" lIns="36576" tIns="22860" rIns="0" bIns="22860" anchor="ctr" upright="1"/>
             <a:lstStyle/>
             <a:p>
               <a:pPr algn="l" rtl="0">
@@ -3866,7 +3865,7 @@
         </xdr:from>
         <xdr:to>
           <xdr:col>4</xdr:col>
-          <xdr:colOff>104775</xdr:colOff>
+          <xdr:colOff>107950</xdr:colOff>
           <xdr:row>27</xdr:row>
           <xdr:rowOff>0</xdr:rowOff>
         </xdr:to>
@@ -3917,7 +3916,7 @@
             </a:extLst>
           </xdr:spPr>
           <xdr:txBody>
-            <a:bodyPr vertOverflow="clip" wrap="square" lIns="27432" tIns="18288" rIns="0" bIns="18288" anchor="ctr" upright="1"/>
+            <a:bodyPr vertOverflow="clip" wrap="square" lIns="36576" tIns="22860" rIns="0" bIns="22860" anchor="ctr" upright="1"/>
             <a:lstStyle/>
             <a:p>
               <a:pPr algn="l" rtl="0">
@@ -3953,7 +3952,7 @@
         </xdr:from>
         <xdr:to>
           <xdr:col>4</xdr:col>
-          <xdr:colOff>104775</xdr:colOff>
+          <xdr:colOff>107950</xdr:colOff>
           <xdr:row>27</xdr:row>
           <xdr:rowOff>209550</xdr:rowOff>
         </xdr:to>
@@ -4004,7 +4003,7 @@
             </a:extLst>
           </xdr:spPr>
           <xdr:txBody>
-            <a:bodyPr vertOverflow="clip" wrap="square" lIns="27432" tIns="18288" rIns="0" bIns="18288" anchor="ctr" upright="1"/>
+            <a:bodyPr vertOverflow="clip" wrap="square" lIns="36576" tIns="22860" rIns="0" bIns="22860" anchor="ctr" upright="1"/>
             <a:lstStyle/>
             <a:p>
               <a:pPr algn="l" rtl="0">
@@ -4040,9 +4039,9 @@
         </xdr:from>
         <xdr:to>
           <xdr:col>4</xdr:col>
-          <xdr:colOff>104775</xdr:colOff>
+          <xdr:colOff>107950</xdr:colOff>
           <xdr:row>28</xdr:row>
-          <xdr:rowOff>352425</xdr:rowOff>
+          <xdr:rowOff>355600</xdr:rowOff>
         </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
@@ -4091,7 +4090,7 @@
             </a:extLst>
           </xdr:spPr>
           <xdr:txBody>
-            <a:bodyPr vertOverflow="clip" wrap="square" lIns="27432" tIns="18288" rIns="0" bIns="18288" anchor="ctr" upright="1"/>
+            <a:bodyPr vertOverflow="clip" wrap="square" lIns="36576" tIns="22860" rIns="0" bIns="22860" anchor="ctr" upright="1"/>
             <a:lstStyle/>
             <a:p>
               <a:pPr algn="l" rtl="0">
@@ -4127,7 +4126,7 @@
         </xdr:from>
         <xdr:to>
           <xdr:col>4</xdr:col>
-          <xdr:colOff>104775</xdr:colOff>
+          <xdr:colOff>107950</xdr:colOff>
           <xdr:row>30</xdr:row>
           <xdr:rowOff>0</xdr:rowOff>
         </xdr:to>
@@ -4178,7 +4177,7 @@
             </a:extLst>
           </xdr:spPr>
           <xdr:txBody>
-            <a:bodyPr vertOverflow="clip" wrap="square" lIns="27432" tIns="18288" rIns="0" bIns="18288" anchor="ctr" upright="1"/>
+            <a:bodyPr vertOverflow="clip" wrap="square" lIns="36576" tIns="22860" rIns="0" bIns="22860" anchor="ctr" upright="1"/>
             <a:lstStyle/>
             <a:p>
               <a:pPr algn="l" rtl="0">
@@ -4214,7 +4213,7 @@
         </xdr:from>
         <xdr:to>
           <xdr:col>4</xdr:col>
-          <xdr:colOff>104775</xdr:colOff>
+          <xdr:colOff>107950</xdr:colOff>
           <xdr:row>30</xdr:row>
           <xdr:rowOff>209550</xdr:rowOff>
         </xdr:to>
@@ -4265,7 +4264,7 @@
             </a:extLst>
           </xdr:spPr>
           <xdr:txBody>
-            <a:bodyPr vertOverflow="clip" wrap="square" lIns="27432" tIns="18288" rIns="0" bIns="18288" anchor="ctr" upright="1"/>
+            <a:bodyPr vertOverflow="clip" wrap="square" lIns="36576" tIns="22860" rIns="0" bIns="22860" anchor="ctr" upright="1"/>
             <a:lstStyle/>
             <a:p>
               <a:pPr algn="l" rtl="0">
@@ -4301,7 +4300,7 @@
         </xdr:from>
         <xdr:to>
           <xdr:col>4</xdr:col>
-          <xdr:colOff>104775</xdr:colOff>
+          <xdr:colOff>107950</xdr:colOff>
           <xdr:row>32</xdr:row>
           <xdr:rowOff>0</xdr:rowOff>
         </xdr:to>
@@ -4352,7 +4351,7 @@
             </a:extLst>
           </xdr:spPr>
           <xdr:txBody>
-            <a:bodyPr vertOverflow="clip" wrap="square" lIns="27432" tIns="18288" rIns="0" bIns="18288" anchor="ctr" upright="1"/>
+            <a:bodyPr vertOverflow="clip" wrap="square" lIns="36576" tIns="22860" rIns="0" bIns="22860" anchor="ctr" upright="1"/>
             <a:lstStyle/>
             <a:p>
               <a:pPr algn="l" rtl="0">
@@ -4388,7 +4387,7 @@
         </xdr:from>
         <xdr:to>
           <xdr:col>4</xdr:col>
-          <xdr:colOff>104775</xdr:colOff>
+          <xdr:colOff>107950</xdr:colOff>
           <xdr:row>32</xdr:row>
           <xdr:rowOff>209550</xdr:rowOff>
         </xdr:to>
@@ -4439,7 +4438,7 @@
             </a:extLst>
           </xdr:spPr>
           <xdr:txBody>
-            <a:bodyPr vertOverflow="clip" wrap="square" lIns="27432" tIns="18288" rIns="0" bIns="18288" anchor="ctr" upright="1"/>
+            <a:bodyPr vertOverflow="clip" wrap="square" lIns="36576" tIns="22860" rIns="0" bIns="22860" anchor="ctr" upright="1"/>
             <a:lstStyle/>
             <a:p>
               <a:pPr algn="l" rtl="0">
@@ -4475,9 +4474,9 @@
         </xdr:from>
         <xdr:to>
           <xdr:col>4</xdr:col>
-          <xdr:colOff>104775</xdr:colOff>
+          <xdr:colOff>107950</xdr:colOff>
           <xdr:row>33</xdr:row>
-          <xdr:rowOff>180975</xdr:rowOff>
+          <xdr:rowOff>184150</xdr:rowOff>
         </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
@@ -4526,7 +4525,7 @@
             </a:extLst>
           </xdr:spPr>
           <xdr:txBody>
-            <a:bodyPr vertOverflow="clip" wrap="square" lIns="27432" tIns="18288" rIns="0" bIns="18288" anchor="ctr" upright="1"/>
+            <a:bodyPr vertOverflow="clip" wrap="square" lIns="36576" tIns="22860" rIns="0" bIns="22860" anchor="ctr" upright="1"/>
             <a:lstStyle/>
             <a:p>
               <a:pPr algn="l" rtl="0">
@@ -4562,9 +4561,9 @@
         </xdr:from>
         <xdr:to>
           <xdr:col>4</xdr:col>
-          <xdr:colOff>104775</xdr:colOff>
+          <xdr:colOff>107950</xdr:colOff>
           <xdr:row>35</xdr:row>
-          <xdr:rowOff>9525</xdr:rowOff>
+          <xdr:rowOff>12700</xdr:rowOff>
         </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
@@ -4613,7 +4612,7 @@
             </a:extLst>
           </xdr:spPr>
           <xdr:txBody>
-            <a:bodyPr vertOverflow="clip" wrap="square" lIns="27432" tIns="18288" rIns="0" bIns="18288" anchor="ctr" upright="1"/>
+            <a:bodyPr vertOverflow="clip" wrap="square" lIns="36576" tIns="22860" rIns="0" bIns="22860" anchor="ctr" upright="1"/>
             <a:lstStyle/>
             <a:p>
               <a:pPr algn="l" rtl="0">
@@ -4649,7 +4648,7 @@
         </xdr:from>
         <xdr:to>
           <xdr:col>4</xdr:col>
-          <xdr:colOff>104775</xdr:colOff>
+          <xdr:colOff>107950</xdr:colOff>
           <xdr:row>35</xdr:row>
           <xdr:rowOff>209550</xdr:rowOff>
         </xdr:to>
@@ -4700,7 +4699,7 @@
             </a:extLst>
           </xdr:spPr>
           <xdr:txBody>
-            <a:bodyPr vertOverflow="clip" wrap="square" lIns="27432" tIns="18288" rIns="0" bIns="18288" anchor="ctr" upright="1"/>
+            <a:bodyPr vertOverflow="clip" wrap="square" lIns="36576" tIns="22860" rIns="0" bIns="22860" anchor="ctr" upright="1"/>
             <a:lstStyle/>
             <a:p>
               <a:pPr algn="l" rtl="0">
@@ -4736,9 +4735,9 @@
         </xdr:from>
         <xdr:to>
           <xdr:col>4</xdr:col>
-          <xdr:colOff>104775</xdr:colOff>
+          <xdr:colOff>107950</xdr:colOff>
           <xdr:row>36</xdr:row>
-          <xdr:rowOff>371475</xdr:rowOff>
+          <xdr:rowOff>374650</xdr:rowOff>
         </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
@@ -4787,7 +4786,7 @@
             </a:extLst>
           </xdr:spPr>
           <xdr:txBody>
-            <a:bodyPr vertOverflow="clip" wrap="square" lIns="27432" tIns="18288" rIns="0" bIns="18288" anchor="ctr" upright="1"/>
+            <a:bodyPr vertOverflow="clip" wrap="square" lIns="36576" tIns="22860" rIns="0" bIns="22860" anchor="ctr" upright="1"/>
             <a:lstStyle/>
             <a:p>
               <a:pPr algn="l" rtl="0">
@@ -4823,7 +4822,7 @@
         </xdr:from>
         <xdr:to>
           <xdr:col>4</xdr:col>
-          <xdr:colOff>104775</xdr:colOff>
+          <xdr:colOff>107950</xdr:colOff>
           <xdr:row>37</xdr:row>
           <xdr:rowOff>323850</xdr:rowOff>
         </xdr:to>
@@ -4874,7 +4873,7 @@
             </a:extLst>
           </xdr:spPr>
           <xdr:txBody>
-            <a:bodyPr vertOverflow="clip" wrap="square" lIns="27432" tIns="18288" rIns="0" bIns="18288" anchor="ctr" upright="1"/>
+            <a:bodyPr vertOverflow="clip" wrap="square" lIns="36576" tIns="22860" rIns="0" bIns="22860" anchor="ctr" upright="1"/>
             <a:lstStyle/>
             <a:p>
               <a:pPr algn="l" rtl="0">
@@ -4910,7 +4909,7 @@
         </xdr:from>
         <xdr:to>
           <xdr:col>4</xdr:col>
-          <xdr:colOff>104775</xdr:colOff>
+          <xdr:colOff>107950</xdr:colOff>
           <xdr:row>38</xdr:row>
           <xdr:rowOff>381000</xdr:rowOff>
         </xdr:to>
@@ -4961,7 +4960,7 @@
             </a:extLst>
           </xdr:spPr>
           <xdr:txBody>
-            <a:bodyPr vertOverflow="clip" wrap="square" lIns="27432" tIns="18288" rIns="0" bIns="18288" anchor="ctr" upright="1"/>
+            <a:bodyPr vertOverflow="clip" wrap="square" lIns="36576" tIns="22860" rIns="0" bIns="22860" anchor="ctr" upright="1"/>
             <a:lstStyle/>
             <a:p>
               <a:pPr algn="l" rtl="0">
@@ -5048,7 +5047,7 @@
             </a:extLst>
           </xdr:spPr>
           <xdr:txBody>
-            <a:bodyPr vertOverflow="clip" wrap="square" lIns="27432" tIns="18288" rIns="0" bIns="18288" anchor="ctr" upright="1"/>
+            <a:bodyPr vertOverflow="clip" wrap="square" lIns="36576" tIns="22860" rIns="0" bIns="22860" anchor="ctr" upright="1"/>
             <a:lstStyle/>
             <a:p>
               <a:pPr algn="l" rtl="0">
@@ -5135,7 +5134,7 @@
             </a:extLst>
           </xdr:spPr>
           <xdr:txBody>
-            <a:bodyPr vertOverflow="clip" wrap="square" lIns="27432" tIns="18288" rIns="0" bIns="18288" anchor="ctr" upright="1"/>
+            <a:bodyPr vertOverflow="clip" wrap="square" lIns="36576" tIns="22860" rIns="0" bIns="22860" anchor="ctr" upright="1"/>
             <a:lstStyle/>
             <a:p>
               <a:pPr algn="l" rtl="0">
@@ -5222,7 +5221,7 @@
             </a:extLst>
           </xdr:spPr>
           <xdr:txBody>
-            <a:bodyPr vertOverflow="clip" wrap="square" lIns="27432" tIns="18288" rIns="0" bIns="18288" anchor="ctr" upright="1"/>
+            <a:bodyPr vertOverflow="clip" wrap="square" lIns="36576" tIns="22860" rIns="0" bIns="22860" anchor="ctr" upright="1"/>
             <a:lstStyle/>
             <a:p>
               <a:pPr algn="l" rtl="0">
@@ -5260,7 +5259,7 @@
           <xdr:col>5</xdr:col>
           <xdr:colOff>152400</xdr:colOff>
           <xdr:row>4</xdr:row>
-          <xdr:rowOff>714375</xdr:rowOff>
+          <xdr:rowOff>717550</xdr:rowOff>
         </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
@@ -5309,7 +5308,7 @@
             </a:extLst>
           </xdr:spPr>
           <xdr:txBody>
-            <a:bodyPr vertOverflow="clip" wrap="square" lIns="27432" tIns="18288" rIns="0" bIns="18288" anchor="ctr" upright="1"/>
+            <a:bodyPr vertOverflow="clip" wrap="square" lIns="36576" tIns="22860" rIns="0" bIns="22860" anchor="ctr" upright="1"/>
             <a:lstStyle/>
             <a:p>
               <a:pPr algn="l" rtl="0">
@@ -5341,7 +5340,7 @@
           <xdr:col>4</xdr:col>
           <xdr:colOff>0</xdr:colOff>
           <xdr:row>5</xdr:row>
-          <xdr:rowOff>9525</xdr:rowOff>
+          <xdr:rowOff>12700</xdr:rowOff>
         </xdr:from>
         <xdr:to>
           <xdr:col>4</xdr:col>
@@ -5396,7 +5395,7 @@
             </a:extLst>
           </xdr:spPr>
           <xdr:txBody>
-            <a:bodyPr vertOverflow="clip" wrap="square" lIns="27432" tIns="18288" rIns="0" bIns="18288" anchor="ctr" upright="1"/>
+            <a:bodyPr vertOverflow="clip" wrap="square" lIns="36576" tIns="22860" rIns="0" bIns="22860" anchor="ctr" upright="1"/>
             <a:lstStyle/>
             <a:p>
               <a:pPr algn="l" rtl="0">
@@ -5434,7 +5433,7 @@
           <xdr:col>5</xdr:col>
           <xdr:colOff>152400</xdr:colOff>
           <xdr:row>7</xdr:row>
-          <xdr:rowOff>66675</xdr:rowOff>
+          <xdr:rowOff>69850</xdr:rowOff>
         </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
@@ -5483,7 +5482,7 @@
             </a:extLst>
           </xdr:spPr>
           <xdr:txBody>
-            <a:bodyPr vertOverflow="clip" wrap="square" lIns="27432" tIns="18288" rIns="0" bIns="18288" anchor="ctr" upright="1"/>
+            <a:bodyPr vertOverflow="clip" wrap="square" lIns="36576" tIns="22860" rIns="0" bIns="22860" anchor="ctr" upright="1"/>
             <a:lstStyle/>
             <a:p>
               <a:pPr algn="l" rtl="0">
@@ -5570,7 +5569,7 @@
             </a:extLst>
           </xdr:spPr>
           <xdr:txBody>
-            <a:bodyPr vertOverflow="clip" wrap="square" lIns="27432" tIns="18288" rIns="0" bIns="18288" anchor="ctr" upright="1"/>
+            <a:bodyPr vertOverflow="clip" wrap="square" lIns="36576" tIns="22860" rIns="0" bIns="22860" anchor="ctr" upright="1"/>
             <a:lstStyle/>
             <a:p>
               <a:pPr algn="l" rtl="0">
@@ -5608,7 +5607,7 @@
           <xdr:col>5</xdr:col>
           <xdr:colOff>152400</xdr:colOff>
           <xdr:row>8</xdr:row>
-          <xdr:rowOff>123825</xdr:rowOff>
+          <xdr:rowOff>127000</xdr:rowOff>
         </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
@@ -5657,7 +5656,7 @@
             </a:extLst>
           </xdr:spPr>
           <xdr:txBody>
-            <a:bodyPr vertOverflow="clip" wrap="square" lIns="27432" tIns="18288" rIns="0" bIns="18288" anchor="ctr" upright="1"/>
+            <a:bodyPr vertOverflow="clip" wrap="square" lIns="36576" tIns="22860" rIns="0" bIns="22860" anchor="ctr" upright="1"/>
             <a:lstStyle/>
             <a:p>
               <a:pPr algn="l" rtl="0">
@@ -5744,7 +5743,7 @@
             </a:extLst>
           </xdr:spPr>
           <xdr:txBody>
-            <a:bodyPr vertOverflow="clip" wrap="square" lIns="27432" tIns="18288" rIns="0" bIns="18288" anchor="ctr" upright="1"/>
+            <a:bodyPr vertOverflow="clip" wrap="square" lIns="36576" tIns="22860" rIns="0" bIns="22860" anchor="ctr" upright="1"/>
             <a:lstStyle/>
             <a:p>
               <a:pPr algn="l" rtl="0">
@@ -5831,7 +5830,7 @@
             </a:extLst>
           </xdr:spPr>
           <xdr:txBody>
-            <a:bodyPr vertOverflow="clip" wrap="square" lIns="27432" tIns="18288" rIns="0" bIns="18288" anchor="ctr" upright="1"/>
+            <a:bodyPr vertOverflow="clip" wrap="square" lIns="36576" tIns="22860" rIns="0" bIns="22860" anchor="ctr" upright="1"/>
             <a:lstStyle/>
             <a:p>
               <a:pPr algn="l" rtl="0">
@@ -5918,7 +5917,7 @@
             </a:extLst>
           </xdr:spPr>
           <xdr:txBody>
-            <a:bodyPr vertOverflow="clip" wrap="square" lIns="27432" tIns="18288" rIns="0" bIns="18288" anchor="ctr" upright="1"/>
+            <a:bodyPr vertOverflow="clip" wrap="square" lIns="36576" tIns="22860" rIns="0" bIns="22860" anchor="ctr" upright="1"/>
             <a:lstStyle/>
             <a:p>
               <a:pPr algn="l" rtl="0">
@@ -5954,7 +5953,7 @@
         </xdr:from>
         <xdr:to>
           <xdr:col>4</xdr:col>
-          <xdr:colOff>695325</xdr:colOff>
+          <xdr:colOff>698500</xdr:colOff>
           <xdr:row>12</xdr:row>
           <xdr:rowOff>571500</xdr:rowOff>
         </xdr:to>
@@ -6005,7 +6004,7 @@
             </a:extLst>
           </xdr:spPr>
           <xdr:txBody>
-            <a:bodyPr vertOverflow="clip" wrap="square" lIns="27432" tIns="18288" rIns="0" bIns="18288" anchor="ctr" upright="1"/>
+            <a:bodyPr vertOverflow="clip" wrap="square" lIns="36576" tIns="22860" rIns="0" bIns="22860" anchor="ctr" upright="1"/>
             <a:lstStyle/>
             <a:p>
               <a:pPr algn="l" rtl="0">
@@ -6092,7 +6091,7 @@
             </a:extLst>
           </xdr:spPr>
           <xdr:txBody>
-            <a:bodyPr vertOverflow="clip" wrap="square" lIns="27432" tIns="18288" rIns="0" bIns="18288" anchor="ctr" upright="1"/>
+            <a:bodyPr vertOverflow="clip" wrap="square" lIns="36576" tIns="22860" rIns="0" bIns="22860" anchor="ctr" upright="1"/>
             <a:lstStyle/>
             <a:p>
               <a:pPr algn="l" rtl="0">
@@ -6179,7 +6178,7 @@
             </a:extLst>
           </xdr:spPr>
           <xdr:txBody>
-            <a:bodyPr vertOverflow="clip" wrap="square" lIns="27432" tIns="18288" rIns="0" bIns="18288" anchor="ctr" upright="1"/>
+            <a:bodyPr vertOverflow="clip" wrap="square" lIns="36576" tIns="22860" rIns="0" bIns="22860" anchor="ctr" upright="1"/>
             <a:lstStyle/>
             <a:p>
               <a:pPr algn="l" rtl="0">
@@ -6217,7 +6216,7 @@
           <xdr:col>5</xdr:col>
           <xdr:colOff>152400</xdr:colOff>
           <xdr:row>15</xdr:row>
-          <xdr:rowOff>333375</xdr:rowOff>
+          <xdr:rowOff>336550</xdr:rowOff>
         </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
@@ -6266,7 +6265,7 @@
             </a:extLst>
           </xdr:spPr>
           <xdr:txBody>
-            <a:bodyPr vertOverflow="clip" wrap="square" lIns="27432" tIns="18288" rIns="0" bIns="18288" anchor="ctr" upright="1"/>
+            <a:bodyPr vertOverflow="clip" wrap="square" lIns="36576" tIns="22860" rIns="0" bIns="22860" anchor="ctr" upright="1"/>
             <a:lstStyle/>
             <a:p>
               <a:pPr algn="l" rtl="0">
@@ -6353,7 +6352,7 @@
             </a:extLst>
           </xdr:spPr>
           <xdr:txBody>
-            <a:bodyPr vertOverflow="clip" wrap="square" lIns="27432" tIns="18288" rIns="0" bIns="18288" anchor="ctr" upright="1"/>
+            <a:bodyPr vertOverflow="clip" wrap="square" lIns="36576" tIns="22860" rIns="0" bIns="22860" anchor="ctr" upright="1"/>
             <a:lstStyle/>
             <a:p>
               <a:pPr algn="l" rtl="0">
@@ -6391,7 +6390,7 @@
           <xdr:col>5</xdr:col>
           <xdr:colOff>152400</xdr:colOff>
           <xdr:row>17</xdr:row>
-          <xdr:rowOff>123825</xdr:rowOff>
+          <xdr:rowOff>127000</xdr:rowOff>
         </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
@@ -6440,7 +6439,7 @@
             </a:extLst>
           </xdr:spPr>
           <xdr:txBody>
-            <a:bodyPr vertOverflow="clip" wrap="square" lIns="27432" tIns="18288" rIns="0" bIns="18288" anchor="ctr" upright="1"/>
+            <a:bodyPr vertOverflow="clip" wrap="square" lIns="36576" tIns="22860" rIns="0" bIns="22860" anchor="ctr" upright="1"/>
             <a:lstStyle/>
             <a:p>
               <a:pPr algn="l" rtl="0">
@@ -6527,7 +6526,7 @@
             </a:extLst>
           </xdr:spPr>
           <xdr:txBody>
-            <a:bodyPr vertOverflow="clip" wrap="square" lIns="27432" tIns="18288" rIns="0" bIns="18288" anchor="ctr" upright="1"/>
+            <a:bodyPr vertOverflow="clip" wrap="square" lIns="36576" tIns="22860" rIns="0" bIns="22860" anchor="ctr" upright="1"/>
             <a:lstStyle/>
             <a:p>
               <a:pPr algn="l" rtl="0">
@@ -6614,7 +6613,7 @@
             </a:extLst>
           </xdr:spPr>
           <xdr:txBody>
-            <a:bodyPr vertOverflow="clip" wrap="square" lIns="27432" tIns="18288" rIns="0" bIns="18288" anchor="ctr" upright="1"/>
+            <a:bodyPr vertOverflow="clip" wrap="square" lIns="36576" tIns="22860" rIns="0" bIns="22860" anchor="ctr" upright="1"/>
             <a:lstStyle/>
             <a:p>
               <a:pPr algn="l" rtl="0">
@@ -6701,7 +6700,7 @@
             </a:extLst>
           </xdr:spPr>
           <xdr:txBody>
-            <a:bodyPr vertOverflow="clip" wrap="square" lIns="27432" tIns="18288" rIns="0" bIns="18288" anchor="ctr" upright="1"/>
+            <a:bodyPr vertOverflow="clip" wrap="square" lIns="36576" tIns="22860" rIns="0" bIns="22860" anchor="ctr" upright="1"/>
             <a:lstStyle/>
             <a:p>
               <a:pPr algn="l" rtl="0">
@@ -6788,7 +6787,7 @@
             </a:extLst>
           </xdr:spPr>
           <xdr:txBody>
-            <a:bodyPr vertOverflow="clip" wrap="square" lIns="27432" tIns="18288" rIns="0" bIns="18288" anchor="ctr" upright="1"/>
+            <a:bodyPr vertOverflow="clip" wrap="square" lIns="36576" tIns="22860" rIns="0" bIns="22860" anchor="ctr" upright="1"/>
             <a:lstStyle/>
             <a:p>
               <a:pPr algn="l" rtl="0">
@@ -6875,7 +6874,7 @@
             </a:extLst>
           </xdr:spPr>
           <xdr:txBody>
-            <a:bodyPr vertOverflow="clip" wrap="square" lIns="27432" tIns="18288" rIns="0" bIns="18288" anchor="ctr" upright="1"/>
+            <a:bodyPr vertOverflow="clip" wrap="square" lIns="36576" tIns="22860" rIns="0" bIns="22860" anchor="ctr" upright="1"/>
             <a:lstStyle/>
             <a:p>
               <a:pPr algn="l" rtl="0">
@@ -6962,7 +6961,7 @@
             </a:extLst>
           </xdr:spPr>
           <xdr:txBody>
-            <a:bodyPr vertOverflow="clip" wrap="square" lIns="27432" tIns="18288" rIns="0" bIns="18288" anchor="ctr" upright="1"/>
+            <a:bodyPr vertOverflow="clip" wrap="square" lIns="36576" tIns="22860" rIns="0" bIns="22860" anchor="ctr" upright="1"/>
             <a:lstStyle/>
             <a:p>
               <a:pPr algn="l" rtl="0">
@@ -7000,7 +6999,7 @@
           <xdr:col>5</xdr:col>
           <xdr:colOff>152400</xdr:colOff>
           <xdr:row>24</xdr:row>
-          <xdr:rowOff>123825</xdr:rowOff>
+          <xdr:rowOff>127000</xdr:rowOff>
         </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
@@ -7049,7 +7048,7 @@
             </a:extLst>
           </xdr:spPr>
           <xdr:txBody>
-            <a:bodyPr vertOverflow="clip" wrap="square" lIns="27432" tIns="18288" rIns="0" bIns="18288" anchor="ctr" upright="1"/>
+            <a:bodyPr vertOverflow="clip" wrap="square" lIns="36576" tIns="22860" rIns="0" bIns="22860" anchor="ctr" upright="1"/>
             <a:lstStyle/>
             <a:p>
               <a:pPr algn="l" rtl="0">
@@ -7136,7 +7135,7 @@
             </a:extLst>
           </xdr:spPr>
           <xdr:txBody>
-            <a:bodyPr vertOverflow="clip" wrap="square" lIns="27432" tIns="18288" rIns="0" bIns="18288" anchor="ctr" upright="1"/>
+            <a:bodyPr vertOverflow="clip" wrap="square" lIns="36576" tIns="22860" rIns="0" bIns="22860" anchor="ctr" upright="1"/>
             <a:lstStyle/>
             <a:p>
               <a:pPr algn="l" rtl="0">
@@ -7223,7 +7222,7 @@
             </a:extLst>
           </xdr:spPr>
           <xdr:txBody>
-            <a:bodyPr vertOverflow="clip" wrap="square" lIns="27432" tIns="18288" rIns="0" bIns="18288" anchor="ctr" upright="1"/>
+            <a:bodyPr vertOverflow="clip" wrap="square" lIns="36576" tIns="22860" rIns="0" bIns="22860" anchor="ctr" upright="1"/>
             <a:lstStyle/>
             <a:p>
               <a:pPr algn="l" rtl="0">
@@ -7310,7 +7309,7 @@
             </a:extLst>
           </xdr:spPr>
           <xdr:txBody>
-            <a:bodyPr vertOverflow="clip" wrap="square" lIns="27432" tIns="18288" rIns="0" bIns="18288" anchor="ctr" upright="1"/>
+            <a:bodyPr vertOverflow="clip" wrap="square" lIns="36576" tIns="22860" rIns="0" bIns="22860" anchor="ctr" upright="1"/>
             <a:lstStyle/>
             <a:p>
               <a:pPr algn="l" rtl="0">
@@ -7397,7 +7396,7 @@
             </a:extLst>
           </xdr:spPr>
           <xdr:txBody>
-            <a:bodyPr vertOverflow="clip" wrap="square" lIns="27432" tIns="18288" rIns="0" bIns="18288" anchor="ctr" upright="1"/>
+            <a:bodyPr vertOverflow="clip" wrap="square" lIns="36576" tIns="22860" rIns="0" bIns="22860" anchor="ctr" upright="1"/>
             <a:lstStyle/>
             <a:p>
               <a:pPr algn="l" rtl="0">
@@ -7484,7 +7483,7 @@
             </a:extLst>
           </xdr:spPr>
           <xdr:txBody>
-            <a:bodyPr vertOverflow="clip" wrap="square" lIns="27432" tIns="18288" rIns="0" bIns="18288" anchor="ctr" upright="1"/>
+            <a:bodyPr vertOverflow="clip" wrap="square" lIns="36576" tIns="22860" rIns="0" bIns="22860" anchor="ctr" upright="1"/>
             <a:lstStyle/>
             <a:p>
               <a:pPr algn="l" rtl="0">
@@ -7571,7 +7570,7 @@
             </a:extLst>
           </xdr:spPr>
           <xdr:txBody>
-            <a:bodyPr vertOverflow="clip" wrap="square" lIns="27432" tIns="18288" rIns="0" bIns="18288" anchor="ctr" upright="1"/>
+            <a:bodyPr vertOverflow="clip" wrap="square" lIns="36576" tIns="22860" rIns="0" bIns="22860" anchor="ctr" upright="1"/>
             <a:lstStyle/>
             <a:p>
               <a:pPr algn="l" rtl="0">
@@ -7658,7 +7657,7 @@
             </a:extLst>
           </xdr:spPr>
           <xdr:txBody>
-            <a:bodyPr vertOverflow="clip" wrap="square" lIns="27432" tIns="18288" rIns="0" bIns="18288" anchor="ctr" upright="1"/>
+            <a:bodyPr vertOverflow="clip" wrap="square" lIns="36576" tIns="22860" rIns="0" bIns="22860" anchor="ctr" upright="1"/>
             <a:lstStyle/>
             <a:p>
               <a:pPr algn="l" rtl="0">
@@ -7745,7 +7744,7 @@
             </a:extLst>
           </xdr:spPr>
           <xdr:txBody>
-            <a:bodyPr vertOverflow="clip" wrap="square" lIns="27432" tIns="18288" rIns="0" bIns="18288" anchor="ctr" upright="1"/>
+            <a:bodyPr vertOverflow="clip" wrap="square" lIns="36576" tIns="22860" rIns="0" bIns="22860" anchor="ctr" upright="1"/>
             <a:lstStyle/>
             <a:p>
               <a:pPr algn="l" rtl="0">
@@ -7783,7 +7782,7 @@
           <xdr:col>5</xdr:col>
           <xdr:colOff>152400</xdr:colOff>
           <xdr:row>34</xdr:row>
-          <xdr:rowOff>28575</xdr:rowOff>
+          <xdr:rowOff>31750</xdr:rowOff>
         </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
@@ -7832,7 +7831,7 @@
             </a:extLst>
           </xdr:spPr>
           <xdr:txBody>
-            <a:bodyPr vertOverflow="clip" wrap="square" lIns="27432" tIns="18288" rIns="0" bIns="18288" anchor="ctr" upright="1"/>
+            <a:bodyPr vertOverflow="clip" wrap="square" lIns="36576" tIns="22860" rIns="0" bIns="22860" anchor="ctr" upright="1"/>
             <a:lstStyle/>
             <a:p>
               <a:pPr algn="l" rtl="0">
@@ -7870,7 +7869,7 @@
           <xdr:col>5</xdr:col>
           <xdr:colOff>152400</xdr:colOff>
           <xdr:row>35</xdr:row>
-          <xdr:rowOff>9525</xdr:rowOff>
+          <xdr:rowOff>12700</xdr:rowOff>
         </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
@@ -7919,7 +7918,7 @@
             </a:extLst>
           </xdr:spPr>
           <xdr:txBody>
-            <a:bodyPr vertOverflow="clip" wrap="square" lIns="27432" tIns="18288" rIns="0" bIns="18288" anchor="ctr" upright="1"/>
+            <a:bodyPr vertOverflow="clip" wrap="square" lIns="36576" tIns="22860" rIns="0" bIns="22860" anchor="ctr" upright="1"/>
             <a:lstStyle/>
             <a:p>
               <a:pPr algn="l" rtl="0">
@@ -8006,7 +8005,7 @@
             </a:extLst>
           </xdr:spPr>
           <xdr:txBody>
-            <a:bodyPr vertOverflow="clip" wrap="square" lIns="27432" tIns="18288" rIns="0" bIns="18288" anchor="ctr" upright="1"/>
+            <a:bodyPr vertOverflow="clip" wrap="square" lIns="36576" tIns="22860" rIns="0" bIns="22860" anchor="ctr" upright="1"/>
             <a:lstStyle/>
             <a:p>
               <a:pPr algn="l" rtl="0">
@@ -8093,7 +8092,7 @@
             </a:extLst>
           </xdr:spPr>
           <xdr:txBody>
-            <a:bodyPr vertOverflow="clip" wrap="square" lIns="27432" tIns="18288" rIns="0" bIns="18288" anchor="ctr" upright="1"/>
+            <a:bodyPr vertOverflow="clip" wrap="square" lIns="36576" tIns="22860" rIns="0" bIns="22860" anchor="ctr" upright="1"/>
             <a:lstStyle/>
             <a:p>
               <a:pPr algn="l" rtl="0">
@@ -8125,13 +8124,13 @@
           <xdr:col>4</xdr:col>
           <xdr:colOff>19050</xdr:colOff>
           <xdr:row>37</xdr:row>
-          <xdr:rowOff>85725</xdr:rowOff>
+          <xdr:rowOff>88900</xdr:rowOff>
         </xdr:from>
         <xdr:to>
           <xdr:col>5</xdr:col>
           <xdr:colOff>171450</xdr:colOff>
           <xdr:row>37</xdr:row>
-          <xdr:rowOff>295275</xdr:rowOff>
+          <xdr:rowOff>298450</xdr:rowOff>
         </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
@@ -8180,7 +8179,7 @@
             </a:extLst>
           </xdr:spPr>
           <xdr:txBody>
-            <a:bodyPr vertOverflow="clip" wrap="square" lIns="27432" tIns="18288" rIns="0" bIns="18288" anchor="ctr" upright="1"/>
+            <a:bodyPr vertOverflow="clip" wrap="square" lIns="36576" tIns="22860" rIns="0" bIns="22860" anchor="ctr" upright="1"/>
             <a:lstStyle/>
             <a:p>
               <a:pPr algn="l" rtl="0">
@@ -8267,7 +8266,7 @@
             </a:extLst>
           </xdr:spPr>
           <xdr:txBody>
-            <a:bodyPr vertOverflow="clip" wrap="square" lIns="27432" tIns="18288" rIns="0" bIns="18288" anchor="ctr" upright="1"/>
+            <a:bodyPr vertOverflow="clip" wrap="square" lIns="36576" tIns="22860" rIns="0" bIns="22860" anchor="ctr" upright="1"/>
             <a:lstStyle/>
             <a:p>
               <a:pPr algn="l" rtl="0">
@@ -8296,9 +8295,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme 2007 - 2010">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office-téma">
   <a:themeElements>
-    <a:clrScheme name="Office 2007 - 2010">
+    <a:clrScheme name="Office">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -8336,9 +8335,9 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office 2007 - 2010">
+    <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -8373,7 +8372,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -8408,7 +8407,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office 2007 - 2010">
+    <a:fmtScheme name="Office">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -8581,85 +8580,85 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Munka1"/>
-  <dimension ref="A1:J464"/>
+  <dimension ref="A1:J21"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="4.28515625" customWidth="1"/>
-    <col min="2" max="2" width="26.85546875" customWidth="1"/>
-    <col min="3" max="3" width="39.85546875" customWidth="1"/>
-    <col min="4" max="4" width="14.85546875" customWidth="1"/>
-    <col min="5" max="5" width="4.140625" customWidth="1"/>
-    <col min="6" max="6" width="40.7109375" customWidth="1"/>
-    <col min="8" max="8" width="6.140625" customWidth="1"/>
-    <col min="9" max="9" width="2.42578125" customWidth="1"/>
-    <col min="10" max="10" width="2.7109375" customWidth="1"/>
-    <col min="13" max="13" width="15.28515625" customWidth="1"/>
+    <col min="1" max="1" width="4.26953125" customWidth="1"/>
+    <col min="2" max="2" width="26.81640625" customWidth="1"/>
+    <col min="3" max="3" width="39.81640625" customWidth="1"/>
+    <col min="4" max="4" width="14.81640625" customWidth="1"/>
+    <col min="5" max="5" width="4.1796875" customWidth="1"/>
+    <col min="6" max="6" width="40.7265625" customWidth="1"/>
+    <col min="8" max="8" width="6.1796875" customWidth="1"/>
+    <col min="9" max="9" width="2.453125" customWidth="1"/>
+    <col min="10" max="10" width="2.7265625" customWidth="1"/>
+    <col min="13" max="13" width="15.26953125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:10" ht="32.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A1" s="31"/>
-      <c r="B1" s="96" t="s">
+      <c r="B1" s="81" t="s">
         <v>45</v>
       </c>
-      <c r="C1" s="97"/>
-      <c r="D1" s="97"/>
-      <c r="E1" s="97"/>
-      <c r="F1" s="97"/>
-      <c r="G1" s="97"/>
-      <c r="H1" s="97"/>
+      <c r="C1" s="82"/>
+      <c r="D1" s="82"/>
+      <c r="E1" s="82"/>
+      <c r="F1" s="82"/>
+      <c r="G1" s="82"/>
+      <c r="H1" s="82"/>
       <c r="I1" s="31"/>
       <c r="J1" s="31"/>
     </row>
-    <row r="2" spans="1:10" ht="23.25" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:10" ht="23.5" x14ac:dyDescent="0.55000000000000004">
       <c r="A2" s="31"/>
       <c r="B2" s="34" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="82"/>
-      <c r="D2" s="83"/>
-      <c r="E2" s="83"/>
-      <c r="F2" s="83"/>
-      <c r="G2" s="83"/>
-      <c r="H2" s="83"/>
+      <c r="C2" s="86"/>
+      <c r="D2" s="87"/>
+      <c r="E2" s="87"/>
+      <c r="F2" s="87"/>
+      <c r="G2" s="87"/>
+      <c r="H2" s="87"/>
       <c r="I2" s="31"/>
       <c r="J2" s="31"/>
     </row>
-    <row r="3" spans="1:10" ht="23.25" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:10" ht="23.5" x14ac:dyDescent="0.55000000000000004">
       <c r="A3" s="31"/>
       <c r="B3" s="34" t="s">
         <v>1</v>
       </c>
-      <c r="C3" s="84"/>
-      <c r="D3" s="83"/>
-      <c r="E3" s="83"/>
-      <c r="F3" s="83"/>
-      <c r="G3" s="83"/>
-      <c r="H3" s="83"/>
+      <c r="C3" s="88"/>
+      <c r="D3" s="87"/>
+      <c r="E3" s="87"/>
+      <c r="F3" s="87"/>
+      <c r="G3" s="87"/>
+      <c r="H3" s="87"/>
       <c r="I3" s="31"/>
       <c r="J3" s="31"/>
     </row>
-    <row r="4" spans="1:10" ht="23.25" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:10" ht="22.5" x14ac:dyDescent="0.45">
       <c r="A4" s="31"/>
       <c r="B4" s="34" t="s">
         <v>3</v>
       </c>
-      <c r="C4" s="82"/>
-      <c r="D4" s="88"/>
-      <c r="E4" s="88"/>
-      <c r="F4" s="88"/>
-      <c r="G4" s="88"/>
-      <c r="H4" s="89"/>
+      <c r="C4" s="86"/>
+      <c r="D4" s="92"/>
+      <c r="E4" s="92"/>
+      <c r="F4" s="92"/>
+      <c r="G4" s="92"/>
+      <c r="H4" s="93"/>
       <c r="I4" s="31"/>
       <c r="J4" s="31"/>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A5" s="31"/>
       <c r="B5" s="31"/>
       <c r="C5" s="31"/>
@@ -8671,36 +8670,36 @@
       <c r="I5" s="31"/>
       <c r="J5" s="31"/>
     </row>
-    <row r="6" spans="1:10" ht="49.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:10" ht="49.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A6" s="31"/>
-      <c r="B6" s="87" t="s">
+      <c r="B6" s="91" t="s">
         <v>2</v>
       </c>
-      <c r="C6" s="87"/>
-      <c r="D6" s="87"/>
-      <c r="E6" s="87"/>
-      <c r="F6" s="87"/>
-      <c r="G6" s="87"/>
-      <c r="H6" s="87"/>
+      <c r="C6" s="91"/>
+      <c r="D6" s="91"/>
+      <c r="E6" s="91"/>
+      <c r="F6" s="91"/>
+      <c r="G6" s="91"/>
+      <c r="H6" s="91"/>
       <c r="I6" s="31"/>
       <c r="J6" s="31"/>
     </row>
-    <row r="7" spans="1:10" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:10" ht="37.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A7" s="31"/>
-      <c r="B7" s="90" t="str">
+      <c r="B7" s="94" t="str">
         <f>CONCATENATE("Az irányelvek között vannak kiemelt (sárga háttérszínnel és félkövér kiemeléssel jelölt) elvek , amelyek betartására kiemelten figyelni kell! Az elégséges szinthez legalább ",D11," pontot el kell érni. A tanulói és tanári értékelés tekintetében, maximum 10 darab irányelvben lehet eltérés.")</f>
         <v>Az irányelvek között vannak kiemelt (sárga háttérszínnel és félkövér kiemeléssel jelölt) elvek , amelyek betartására kiemelten figyelni kell! Az elégséges szinthez legalább 20 pontot el kell érni. A tanulói és tanári értékelés tekintetében, maximum 10 darab irányelvben lehet eltérés.</v>
       </c>
-      <c r="C7" s="90"/>
-      <c r="D7" s="90"/>
-      <c r="E7" s="90"/>
-      <c r="F7" s="90"/>
-      <c r="G7" s="90"/>
-      <c r="H7" s="90"/>
+      <c r="C7" s="94"/>
+      <c r="D7" s="94"/>
+      <c r="E7" s="94"/>
+      <c r="F7" s="94"/>
+      <c r="G7" s="94"/>
+      <c r="H7" s="94"/>
       <c r="I7" s="31"/>
       <c r="J7" s="31"/>
     </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A8" s="31"/>
       <c r="B8" s="31"/>
       <c r="C8" s="31"/>
@@ -8712,7 +8711,7 @@
       <c r="I8" s="31"/>
       <c r="J8" s="31"/>
     </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A9" s="31"/>
       <c r="B9" s="32" t="s">
         <v>33</v>
@@ -8726,86 +8725,86 @@
       <c r="I9" s="31"/>
       <c r="J9" s="31"/>
     </row>
-    <row r="10" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A10" s="31"/>
-      <c r="B10" s="85" t="s">
+      <c r="B10" s="89" t="s">
         <v>30</v>
       </c>
-      <c r="C10" s="86"/>
+      <c r="C10" s="90"/>
       <c r="D10" s="78">
         <f>SUM(Irányelvek!G:G)</f>
         <v>80</v>
       </c>
       <c r="E10" s="31"/>
-      <c r="F10" s="94" t="s">
+      <c r="F10" s="98" t="s">
         <v>46</v>
       </c>
-      <c r="G10" s="94"/>
-      <c r="H10" s="94"/>
+      <c r="G10" s="98"/>
+      <c r="H10" s="98"/>
       <c r="I10" s="31"/>
       <c r="J10" s="31"/>
     </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A11" s="31"/>
-      <c r="B11" s="98" t="s">
+      <c r="B11" s="83" t="s">
         <v>36</v>
       </c>
-      <c r="C11" s="99"/>
+      <c r="C11" s="84"/>
       <c r="D11" s="79">
         <v>20</v>
       </c>
       <c r="E11" s="31"/>
-      <c r="F11" s="95"/>
-      <c r="G11" s="95"/>
-      <c r="H11" s="95"/>
+      <c r="F11" s="99"/>
+      <c r="G11" s="99"/>
+      <c r="H11" s="99"/>
       <c r="I11" s="31"/>
       <c r="J11" s="31"/>
     </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A12" s="31"/>
-      <c r="B12" s="85" t="s">
+      <c r="B12" s="89" t="s">
         <v>58</v>
       </c>
-      <c r="C12" s="86"/>
+      <c r="C12" s="90"/>
       <c r="D12" s="78">
         <v>20</v>
       </c>
       <c r="E12" s="31"/>
-      <c r="F12" s="95"/>
-      <c r="G12" s="95"/>
-      <c r="H12" s="95"/>
+      <c r="F12" s="99"/>
+      <c r="G12" s="99"/>
+      <c r="H12" s="99"/>
       <c r="I12" s="31"/>
       <c r="J12" s="31"/>
     </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A13" s="31"/>
-      <c r="B13" s="85" t="s">
+      <c r="B13" s="89" t="s">
         <v>59</v>
       </c>
-      <c r="C13" s="86"/>
+      <c r="C13" s="90"/>
       <c r="D13" s="78">
         <v>40</v>
       </c>
       <c r="E13" s="31"/>
-      <c r="F13" s="95"/>
-      <c r="G13" s="95"/>
-      <c r="H13" s="95"/>
+      <c r="F13" s="99"/>
+      <c r="G13" s="99"/>
+      <c r="H13" s="99"/>
       <c r="I13" s="31"/>
       <c r="J13" s="31"/>
     </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A14" s="31"/>
       <c r="B14" s="31"/>
       <c r="C14" s="31"/>
       <c r="D14" s="31"/>
       <c r="E14" s="31"/>
-      <c r="F14" s="95"/>
-      <c r="G14" s="95"/>
-      <c r="H14" s="95"/>
+      <c r="F14" s="99"/>
+      <c r="G14" s="99"/>
+      <c r="H14" s="99"/>
       <c r="I14" s="31"/>
       <c r="J14" s="31"/>
     </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A15" s="31"/>
       <c r="B15" s="32" t="s">
         <v>57</v>
@@ -8819,12 +8818,12 @@
       <c r="I15" s="31"/>
       <c r="J15" s="31"/>
     </row>
-    <row r="16" spans="1:10" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:10" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A16" s="31"/>
-      <c r="B16" s="85" t="s">
+      <c r="B16" s="89" t="s">
         <v>39</v>
       </c>
-      <c r="C16" s="86"/>
+      <c r="C16" s="90"/>
       <c r="D16" s="30" t="b">
         <f t="array" ref="D16">IF(COUNTIFS(Irányelvek!D2:D39,"=hamis",Irányelvek!F2:F39,"=Igaz")=0,TRUE,FALSE)</f>
         <v>0</v>
@@ -8836,80 +8835,80 @@
       <c r="I16" s="31"/>
       <c r="J16" s="31"/>
     </row>
-    <row r="17" spans="1:10" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:10" ht="31.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A17" s="31"/>
-      <c r="B17" s="85" t="s">
+      <c r="B17" s="89" t="s">
         <v>32</v>
       </c>
-      <c r="C17" s="86"/>
+      <c r="C17" s="90"/>
       <c r="D17" s="33">
         <f>SUM(Irányelvek!H2:H39)</f>
-        <v>-41</v>
+        <v>22</v>
       </c>
       <c r="E17" s="31"/>
-      <c r="F17" s="93" t="str">
+      <c r="F17" s="97" t="str">
         <f>VLOOKUP(D20,Ponthatárok!$C$3:$D$7,2,TRUE)</f>
-        <v>Elégtelen (1)</v>
-      </c>
-      <c r="G17" s="93"/>
-      <c r="H17" s="93"/>
+        <v>Elégséges (2)</v>
+      </c>
+      <c r="G17" s="97"/>
+      <c r="H17" s="97"/>
       <c r="I17" s="31"/>
       <c r="J17" s="31"/>
     </row>
-    <row r="18" spans="1:10" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:10" ht="31.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A18" s="31"/>
-      <c r="B18" s="91" t="s">
+      <c r="B18" s="95" t="s">
         <v>60</v>
       </c>
-      <c r="C18" s="92"/>
+      <c r="C18" s="96"/>
       <c r="D18" s="36">
         <f>IF(D17&gt;D11,VLOOKUP(SUM(Irányelvek!J2:J39),Ponthatárok!G2:H12,2,TRUE),0)</f>
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="E18" s="31"/>
-      <c r="F18" s="93"/>
-      <c r="G18" s="93"/>
-      <c r="H18" s="93"/>
+      <c r="F18" s="97"/>
+      <c r="G18" s="97"/>
+      <c r="H18" s="97"/>
       <c r="I18" s="31"/>
       <c r="J18" s="31"/>
     </row>
-    <row r="19" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A19" s="31"/>
-      <c r="B19" s="85" t="s">
+      <c r="B19" s="89" t="s">
         <v>61</v>
       </c>
-      <c r="C19" s="86"/>
+      <c r="C19" s="90"/>
       <c r="D19" s="80">
         <v>40</v>
       </c>
       <c r="E19" s="31"/>
-      <c r="F19" s="93"/>
-      <c r="G19" s="93"/>
-      <c r="H19" s="93"/>
+      <c r="F19" s="97"/>
+      <c r="G19" s="97"/>
+      <c r="H19" s="97"/>
       <c r="I19" s="31"/>
       <c r="J19" s="31"/>
     </row>
-    <row r="20" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A20" s="31"/>
-      <c r="B20" s="85" t="s">
+      <c r="B20" s="89" t="s">
         <v>62</v>
       </c>
-      <c r="C20" s="86"/>
+      <c r="C20" s="90"/>
       <c r="D20" s="33">
         <f>SUM(D17:D19)</f>
-        <v>-1</v>
+        <v>66</v>
       </c>
       <c r="E20" s="31"/>
-      <c r="F20" s="81" t="str">
+      <c r="F20" s="85" t="str">
         <f>CONCATENATE("Az önértékelés alapján ",VLOOKUP(D20,Ponthatárok!$C$3:$D$7,2,TRUE), "  érdemjegyet kapnál rá.")</f>
-        <v>Az önértékelés alapján Elégtelen (1)  érdemjegyet kapnál rá.</v>
-      </c>
-      <c r="G20" s="81"/>
-      <c r="H20" s="81"/>
+        <v>Az önértékelés alapján Elégséges (2)  érdemjegyet kapnál rá.</v>
+      </c>
+      <c r="G20" s="85"/>
+      <c r="H20" s="85"/>
       <c r="I20" s="31"/>
       <c r="J20" s="31"/>
     </row>
-    <row r="21" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A21" s="31"/>
       <c r="B21" s="35"/>
       <c r="C21" s="35"/>
@@ -8921,441 +8920,11 @@
       <c r="I21" s="31"/>
       <c r="J21" s="31"/>
     </row>
-    <row r="33" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="34" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="35" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="36" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="37" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="38" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="39" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="40" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="41" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="42" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="43" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="44" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="45" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="46" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="47" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="48" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="49" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="50" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="51" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="52" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="53" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="54" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="55" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="56" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="57" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="58" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="59" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="60" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="61" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="62" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="63" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="64" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="65" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="66" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="67" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="68" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="69" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="70" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="71" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="72" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="73" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="74" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="75" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="76" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="77" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="78" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="79" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="80" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="81" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="82" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="83" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="84" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="85" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="86" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="87" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="88" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="89" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="90" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="91" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="92" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="93" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="94" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="95" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="96" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="97" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="98" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="99" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="100" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="101" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="102" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="103" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="104" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="105" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="106" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="107" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="108" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="109" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="110" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="111" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="112" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="113" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="114" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="115" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="116" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="117" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="118" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="119" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="120" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="121" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="122" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="123" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="124" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="125" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="126" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="127" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="128" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="129" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="130" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="131" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="132" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="133" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="134" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="135" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="136" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="137" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="138" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="139" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="140" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="141" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="142" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="143" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="144" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="145" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="146" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="147" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="148" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="149" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="150" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="151" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="152" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="153" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="154" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="155" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="156" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="157" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="158" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="159" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="160" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="161" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="162" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="163" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="164" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="165" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="166" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="167" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="168" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="169" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="170" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="171" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="172" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="173" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="174" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="175" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="176" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="177" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="178" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="179" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="180" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="181" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="182" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="183" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="184" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="185" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="186" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="187" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="188" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="189" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="190" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="191" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="192" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="193" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="194" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="195" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="196" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="197" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="198" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="199" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="200" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="201" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="202" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="203" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="204" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="205" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="206" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="207" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="208" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="209" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="210" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="211" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="212" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="213" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="214" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="215" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="216" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="217" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="218" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="219" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="220" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="221" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="222" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="223" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="224" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="225" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="226" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="227" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="228" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="229" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="230" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="231" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="232" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="233" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="234" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="235" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="236" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="237" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="238" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="239" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="240" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="241" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="242" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="243" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="244" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="245" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="246" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="247" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="248" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="249" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="250" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="251" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="252" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="253" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="254" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="255" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="256" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="257" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="258" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="259" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="260" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="261" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="262" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="263" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="264" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="265" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="266" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="267" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="268" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="269" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="270" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="271" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="272" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="273" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="274" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="275" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="276" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="277" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="278" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="279" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="280" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="281" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="282" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="283" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="284" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="285" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="286" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="287" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="288" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="289" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="290" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="291" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="292" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="293" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="294" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="295" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="296" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="297" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="298" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="299" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="300" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="301" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="302" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="303" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="304" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="305" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="306" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="307" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="308" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="309" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="310" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="311" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="312" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="313" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="314" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="315" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="316" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="317" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="318" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="319" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="320" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="321" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="322" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="323" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="324" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="325" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="326" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="327" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="328" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="329" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="330" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="331" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="332" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="333" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="334" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="335" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="336" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="337" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="338" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="339" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="340" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="341" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="342" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="343" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="344" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="345" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="346" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="347" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="348" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="349" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="350" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="351" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="352" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="353" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="354" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="355" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="356" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="357" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="358" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="359" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="360" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="361" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="362" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="363" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="364" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="365" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="366" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="367" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="368" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="369" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="370" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="371" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="372" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="373" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="374" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="375" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="376" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="377" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="378" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="379" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="380" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="381" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="382" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="383" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="384" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="385" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="386" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="387" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="388" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="389" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="390" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="391" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="392" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="393" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="394" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="395" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="396" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="397" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="398" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="399" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="400" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="401" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="402" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="403" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="404" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="405" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="406" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="407" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="408" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="409" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="410" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="411" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="412" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="413" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="414" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="415" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="416" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="417" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="418" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="419" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="420" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="421" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="422" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="423" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="424" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="425" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="426" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="427" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="428" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="429" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="430" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="431" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="432" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="433" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="434" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="435" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="436" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="437" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="438" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="439" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="440" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="441" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="442" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="443" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="444" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="445" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="446" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="447" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="448" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="449" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="450" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="451" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="452" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="453" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="454" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="455" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="456" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="457" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="458" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="459" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="460" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="461" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="462" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="463" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="464" customFormat="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <sheetProtection algorithmName="SHA-512" hashValue="Pt2r10NfCQvSDRx8qMjGYxYpEYBoOyIK56jWLg5u88pMtB0yZv+L45h/PZkvP5rgD0XQukcG0FY9SUv/PUWVng==" saltValue="OS0FMTO/1nXUT8EsxtE52w==" spinCount="100000" sheet="1" objects="1" scenarios="1"/>
   <mergeCells count="18">
+    <mergeCell ref="B10:C10"/>
+    <mergeCell ref="B16:C16"/>
     <mergeCell ref="B1:H1"/>
     <mergeCell ref="B11:C11"/>
     <mergeCell ref="F20:H20"/>
@@ -9372,8 +8941,6 @@
     <mergeCell ref="B18:C18"/>
     <mergeCell ref="F17:H19"/>
     <mergeCell ref="F10:H14"/>
-    <mergeCell ref="B10:C10"/>
-    <mergeCell ref="B16:C16"/>
   </mergeCells>
   <conditionalFormatting sqref="D17:D20">
     <cfRule type="expression" dxfId="2" priority="1" stopIfTrue="1">
@@ -9381,8 +8948,8 @@
     </cfRule>
   </conditionalFormatting>
   <hyperlinks>
-    <hyperlink ref="B6" location="Irányelvek!A1" display="Az irányelvek megtekintése és az adatlap kitöltése" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
-    <hyperlink ref="B6:H6" location="Irányelvek!A1" display="Az irányelvek megtekintése és az adatlap kitöltése" xr:uid="{00000000-0004-0000-0000-000001000000}"/>
+    <hyperlink ref="B6" location="Irányelvek!A1" display="Az irányelvek megtekintése és az adatlap kitöltése"/>
+    <hyperlink ref="B6:H6" location="Irányelvek!A1" display="Az irányelvek megtekintése és az adatlap kitöltése"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>
@@ -9390,31 +8957,31 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Munka2"/>
   <dimension ref="A1:L39"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="1" topLeftCell="A32" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="C36" sqref="C36"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="3.140625" customWidth="1"/>
-    <col min="2" max="2" width="15.85546875" style="28" customWidth="1"/>
-    <col min="3" max="3" width="54.140625" style="29" customWidth="1"/>
-    <col min="4" max="4" width="10.5703125" style="22" customWidth="1"/>
-    <col min="5" max="5" width="10.5703125" style="23" customWidth="1"/>
-    <col min="6" max="6" width="9.85546875" customWidth="1"/>
+    <col min="1" max="1" width="3.1796875" customWidth="1"/>
+    <col min="2" max="2" width="15.81640625" style="28" customWidth="1"/>
+    <col min="3" max="3" width="54.1796875" style="29" customWidth="1"/>
+    <col min="4" max="4" width="10.54296875" style="22" customWidth="1"/>
+    <col min="5" max="5" width="10.54296875" style="23" customWidth="1"/>
+    <col min="6" max="6" width="9.81640625" customWidth="1"/>
     <col min="8" max="8" width="13" customWidth="1"/>
     <col min="9" max="9" width="16" customWidth="1"/>
-    <col min="10" max="10" width="10.85546875" customWidth="1"/>
-    <col min="11" max="11" width="11.7109375" customWidth="1"/>
-    <col min="12" max="12" width="9.7109375" customWidth="1"/>
+    <col min="10" max="10" width="10.81640625" customWidth="1"/>
+    <col min="11" max="11" width="11.7265625" customWidth="1"/>
+    <col min="12" max="12" width="9.7265625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" s="3" customFormat="1" ht="39" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:12" s="3" customFormat="1" ht="39.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1" s="71"/>
       <c r="B1" s="64" t="s">
         <v>5</v>
@@ -9445,7 +9012,7 @@
       </c>
       <c r="L1" s="4"/>
     </row>
-    <row r="2" spans="1:12" s="1" customFormat="1" ht="24.75" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:12" s="1" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A2" s="72">
         <v>1</v>
       </c>
@@ -9480,7 +9047,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:12" s="1" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:12" s="1" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A3" s="73">
         <v>2</v>
       </c>
@@ -9491,7 +9058,7 @@
         <v>22</v>
       </c>
       <c r="D3" s="16" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E3" s="16" t="b">
         <v>1</v>
@@ -9500,9 +9067,9 @@
       <c r="G3" s="2">
         <v>1</v>
       </c>
-      <c r="H3" s="13" t="str">
+      <c r="H3" s="13">
         <f t="shared" ref="H3:H39" si="0">IF(D3=TRUE,G3,IF(F3=TRUE,-2,""))</f>
-        <v/>
+        <v>1</v>
       </c>
       <c r="I3" s="14">
         <f t="shared" ref="I3:I39" si="1">IF(E3=TRUE,G3,IF(F3=TRUE,-2,""))</f>
@@ -9510,10 +9077,10 @@
       </c>
       <c r="J3" s="42">
         <f t="shared" ref="J3:J39" si="2">IF(H3=I3,0,1)</f>
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:12" s="1" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:12" s="1" customFormat="1" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A4" s="73">
         <v>3</v>
       </c>
@@ -9549,7 +9116,7 @@
       </c>
       <c r="L4" s="6"/>
     </row>
-    <row r="5" spans="1:12" s="1" customFormat="1" ht="60" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:12" s="1" customFormat="1" ht="58" x14ac:dyDescent="0.35">
       <c r="A5" s="73">
         <v>4</v>
       </c>
@@ -9585,7 +9152,7 @@
       </c>
       <c r="L5" s="7"/>
     </row>
-    <row r="6" spans="1:12" s="1" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:12" s="1" customFormat="1" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A6" s="73">
         <v>6</v>
       </c>
@@ -9620,7 +9187,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:12" s="1" customFormat="1" ht="25.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:12" s="1" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A7" s="74">
         <v>7</v>
       </c>
@@ -9655,7 +9222,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:12" s="1" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:12" s="1" customFormat="1" ht="29" x14ac:dyDescent="0.35">
       <c r="A8" s="75">
         <v>8</v>
       </c>
@@ -9688,7 +9255,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:12" ht="30" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:12" ht="29" x14ac:dyDescent="0.35">
       <c r="A9" s="73">
         <v>9</v>
       </c>
@@ -9699,7 +9266,7 @@
         <v>34</v>
       </c>
       <c r="D9" s="20" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E9" s="17" t="b">
         <v>1</v>
@@ -9708,9 +9275,9 @@
       <c r="G9" s="2">
         <v>1</v>
       </c>
-      <c r="H9" s="13" t="str">
+      <c r="H9" s="13">
         <f t="shared" si="0"/>
-        <v/>
+        <v>1</v>
       </c>
       <c r="I9" s="14">
         <f t="shared" si="1"/>
@@ -9718,10 +9285,10 @@
       </c>
       <c r="J9" s="42">
         <f t="shared" si="2"/>
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:12" ht="30" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:12" ht="29" x14ac:dyDescent="0.35">
       <c r="A10" s="73">
         <v>10</v>
       </c>
@@ -9732,7 +9299,7 @@
         <v>51</v>
       </c>
       <c r="D10" s="20" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E10" s="17" t="b">
         <v>1</v>
@@ -9745,7 +9312,7 @@
       </c>
       <c r="H10" s="13">
         <f t="shared" si="0"/>
-        <v>-2</v>
+        <v>5</v>
       </c>
       <c r="I10" s="14">
         <f t="shared" si="1"/>
@@ -9753,10 +9320,10 @@
       </c>
       <c r="J10" s="42">
         <f t="shared" si="2"/>
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:12" ht="30" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:12" ht="29" x14ac:dyDescent="0.35">
       <c r="A11" s="73">
         <v>11</v>
       </c>
@@ -9767,7 +9334,7 @@
         <v>41</v>
       </c>
       <c r="D11" s="20" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E11" s="17" t="b">
         <v>1</v>
@@ -9780,7 +9347,7 @@
       </c>
       <c r="H11" s="13">
         <f t="shared" si="0"/>
-        <v>-2</v>
+        <v>5</v>
       </c>
       <c r="I11" s="14">
         <f t="shared" si="1"/>
@@ -9788,10 +9355,10 @@
       </c>
       <c r="J11" s="42">
         <f t="shared" si="2"/>
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:12" ht="30" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:12" ht="29" x14ac:dyDescent="0.35">
       <c r="A12" s="73">
         <v>12</v>
       </c>
@@ -9802,7 +9369,7 @@
         <v>10</v>
       </c>
       <c r="D12" s="20" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E12" s="17" t="b">
         <v>1</v>
@@ -9811,9 +9378,9 @@
       <c r="G12" s="2">
         <v>1</v>
       </c>
-      <c r="H12" s="13" t="str">
+      <c r="H12" s="13">
         <f t="shared" si="0"/>
-        <v/>
+        <v>1</v>
       </c>
       <c r="I12" s="14">
         <f t="shared" si="1"/>
@@ -9821,10 +9388,10 @@
       </c>
       <c r="J12" s="42">
         <f t="shared" si="2"/>
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:12" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:12" ht="29.5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A13" s="73">
         <v>13</v>
       </c>
@@ -9835,7 +9402,7 @@
         <v>71</v>
       </c>
       <c r="D13" s="21" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E13" s="19" t="b">
         <v>1</v>
@@ -9848,7 +9415,7 @@
       </c>
       <c r="H13" s="61">
         <f t="shared" si="0"/>
-        <v>-2</v>
+        <v>5</v>
       </c>
       <c r="I13" s="62">
         <f t="shared" si="1"/>
@@ -9856,10 +9423,10 @@
       </c>
       <c r="J13" s="63">
         <f t="shared" si="2"/>
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:12" ht="60" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:12" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A14" s="73">
         <v>14</v>
       </c>
@@ -9870,7 +9437,7 @@
         <v>74</v>
       </c>
       <c r="D14" s="60" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E14" s="57" t="b">
         <v>1</v>
@@ -9883,7 +9450,7 @@
       </c>
       <c r="H14" s="39">
         <f t="shared" si="0"/>
-        <v>-2</v>
+        <v>5</v>
       </c>
       <c r="I14" s="40">
         <f t="shared" si="1"/>
@@ -9891,10 +9458,10 @@
       </c>
       <c r="J14" s="41">
         <f t="shared" si="2"/>
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:12" ht="30" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:12" ht="29" x14ac:dyDescent="0.35">
       <c r="A15" s="73">
         <v>15</v>
       </c>
@@ -9929,7 +9496,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="16" spans="1:12" ht="45" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:12" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A16" s="73">
         <v>16</v>
       </c>
@@ -9964,7 +9531,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:10" ht="30" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A17" s="73">
         <v>17</v>
       </c>
@@ -9999,7 +9566,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="18" spans="1:10" ht="19.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:10" ht="19.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A18" s="73">
         <v>19</v>
       </c>
@@ -10010,7 +9577,7 @@
         <v>78</v>
       </c>
       <c r="D18" s="20" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E18" s="17" t="b">
         <v>1</v>
@@ -10023,7 +9590,7 @@
       </c>
       <c r="H18" s="13">
         <f t="shared" si="0"/>
-        <v>-2</v>
+        <v>3</v>
       </c>
       <c r="I18" s="14">
         <f t="shared" si="1"/>
@@ -10031,10 +9598,10 @@
       </c>
       <c r="J18" s="42">
         <f t="shared" si="2"/>
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
-    <row r="19" spans="1:10" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:10" ht="19.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A19" s="73">
         <v>21</v>
       </c>
@@ -10045,7 +9612,7 @@
         <v>12</v>
       </c>
       <c r="D19" s="60" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E19" s="57" t="b">
         <v>1</v>
@@ -10054,9 +9621,9 @@
       <c r="G19" s="39">
         <v>1</v>
       </c>
-      <c r="H19" s="39" t="str">
+      <c r="H19" s="39">
         <f t="shared" si="0"/>
-        <v/>
+        <v>1</v>
       </c>
       <c r="I19" s="40">
         <f t="shared" si="1"/>
@@ -10064,10 +9631,10 @@
       </c>
       <c r="J19" s="41">
         <f t="shared" si="2"/>
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
-    <row r="20" spans="1:10" ht="45" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:10" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A20" s="73">
         <v>22</v>
       </c>
@@ -10100,7 +9667,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="21" spans="1:10" ht="30" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:10" ht="29" x14ac:dyDescent="0.35">
       <c r="A21" s="73">
         <v>23</v>
       </c>
@@ -10111,7 +9678,7 @@
         <v>27</v>
       </c>
       <c r="D21" s="20" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E21" s="17" t="b">
         <v>1</v>
@@ -10120,9 +9687,9 @@
       <c r="G21" s="2">
         <v>1</v>
       </c>
-      <c r="H21" s="13" t="str">
+      <c r="H21" s="13">
         <f t="shared" si="0"/>
-        <v/>
+        <v>1</v>
       </c>
       <c r="I21" s="14">
         <f t="shared" si="1"/>
@@ -10130,10 +9697,10 @@
       </c>
       <c r="J21" s="42">
         <f t="shared" si="2"/>
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
-    <row r="22" spans="1:10" ht="45" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:10" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A22" s="73">
         <v>24</v>
       </c>
@@ -10144,7 +9711,7 @@
         <v>28</v>
       </c>
       <c r="D22" s="20" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E22" s="17" t="b">
         <v>1</v>
@@ -10153,9 +9720,9 @@
       <c r="G22" s="2">
         <v>1</v>
       </c>
-      <c r="H22" s="13" t="str">
+      <c r="H22" s="13">
         <f t="shared" si="0"/>
-        <v/>
+        <v>1</v>
       </c>
       <c r="I22" s="14">
         <f t="shared" si="1"/>
@@ -10163,10 +9730,10 @@
       </c>
       <c r="J22" s="42">
         <f t="shared" si="2"/>
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
-    <row r="23" spans="1:10" ht="30" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:10" ht="29" x14ac:dyDescent="0.35">
       <c r="A23" s="73">
         <v>25</v>
       </c>
@@ -10177,7 +9744,7 @@
         <v>13</v>
       </c>
       <c r="D23" s="20" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E23" s="17" t="b">
         <v>1</v>
@@ -10186,9 +9753,9 @@
       <c r="G23" s="2">
         <v>1</v>
       </c>
-      <c r="H23" s="13" t="str">
+      <c r="H23" s="13">
         <f t="shared" si="0"/>
-        <v/>
+        <v>1</v>
       </c>
       <c r="I23" s="14">
         <f t="shared" si="1"/>
@@ -10196,10 +9763,10 @@
       </c>
       <c r="J23" s="42">
         <f t="shared" si="2"/>
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
-    <row r="24" spans="1:10" ht="30" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:10" ht="29" x14ac:dyDescent="0.35">
       <c r="A24" s="73">
         <v>26</v>
       </c>
@@ -10232,7 +9799,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="25" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A25" s="73">
         <v>27</v>
       </c>
@@ -10243,7 +9810,7 @@
         <v>15</v>
       </c>
       <c r="D25" s="20" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E25" s="17" t="b">
         <v>1</v>
@@ -10252,9 +9819,9 @@
       <c r="G25" s="2">
         <v>1</v>
       </c>
-      <c r="H25" s="13" t="str">
+      <c r="H25" s="13">
         <f t="shared" si="0"/>
-        <v/>
+        <v>1</v>
       </c>
       <c r="I25" s="14">
         <f t="shared" si="1"/>
@@ -10262,10 +9829,10 @@
       </c>
       <c r="J25" s="42">
         <f t="shared" si="2"/>
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
-    <row r="26" spans="1:10" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:10" ht="44" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A26" s="76">
         <v>28</v>
       </c>
@@ -10300,7 +9867,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="27" spans="1:10" ht="30" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:10" ht="29" x14ac:dyDescent="0.35">
       <c r="A27" s="72">
         <v>29</v>
       </c>
@@ -10311,7 +9878,7 @@
         <v>72</v>
       </c>
       <c r="D27" s="60" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E27" s="57" t="b">
         <v>1</v>
@@ -10324,7 +9891,7 @@
       </c>
       <c r="H27" s="39">
         <f t="shared" si="0"/>
-        <v>-2</v>
+        <v>4</v>
       </c>
       <c r="I27" s="40">
         <f t="shared" si="1"/>
@@ -10332,10 +9899,10 @@
       </c>
       <c r="J27" s="41">
         <f t="shared" si="2"/>
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
-    <row r="28" spans="1:10" ht="30" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:10" ht="29" x14ac:dyDescent="0.35">
       <c r="A28" s="73">
         <v>30</v>
       </c>
@@ -10346,7 +9913,7 @@
         <v>6</v>
       </c>
       <c r="D28" s="20" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E28" s="17" t="b">
         <v>1</v>
@@ -10355,9 +9922,9 @@
       <c r="G28" s="2">
         <v>1</v>
       </c>
-      <c r="H28" s="13" t="str">
+      <c r="H28" s="13">
         <f t="shared" si="0"/>
-        <v/>
+        <v>1</v>
       </c>
       <c r="I28" s="14">
         <f t="shared" si="1"/>
@@ -10365,10 +9932,10 @@
       </c>
       <c r="J28" s="42">
         <f t="shared" si="2"/>
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
-    <row r="29" spans="1:10" ht="30" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:10" ht="29" x14ac:dyDescent="0.35">
       <c r="A29" s="73">
         <v>31</v>
       </c>
@@ -10379,7 +9946,7 @@
         <v>50</v>
       </c>
       <c r="D29" s="20" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E29" s="17" t="b">
         <v>1</v>
@@ -10388,9 +9955,9 @@
       <c r="G29" s="2">
         <v>1</v>
       </c>
-      <c r="H29" s="13" t="str">
+      <c r="H29" s="13">
         <f t="shared" si="0"/>
-        <v/>
+        <v>1</v>
       </c>
       <c r="I29" s="14">
         <f t="shared" si="1"/>
@@ -10398,10 +9965,10 @@
       </c>
       <c r="J29" s="42">
         <f t="shared" si="2"/>
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
-    <row r="30" spans="1:10" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:10" ht="44" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A30" s="74">
         <v>32</v>
       </c>
@@ -10412,7 +9979,7 @@
         <v>8</v>
       </c>
       <c r="D30" s="59" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E30" s="45" t="b">
         <v>1</v>
@@ -10425,7 +9992,7 @@
       </c>
       <c r="H30" s="47">
         <f t="shared" si="0"/>
-        <v>-2</v>
+        <v>2</v>
       </c>
       <c r="I30" s="48">
         <f t="shared" si="1"/>
@@ -10433,10 +10000,10 @@
       </c>
       <c r="J30" s="49">
         <f t="shared" si="2"/>
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
-    <row r="31" spans="1:10" ht="30" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:10" ht="29" x14ac:dyDescent="0.35">
       <c r="A31" s="72">
         <v>33</v>
       </c>
@@ -10447,7 +10014,7 @@
         <v>43</v>
       </c>
       <c r="D31" s="60" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E31" s="57" t="b">
         <v>1</v>
@@ -10460,7 +10027,7 @@
       </c>
       <c r="H31" s="39">
         <f t="shared" si="0"/>
-        <v>-2</v>
+        <v>2</v>
       </c>
       <c r="I31" s="40">
         <f t="shared" si="1"/>
@@ -10468,10 +10035,10 @@
       </c>
       <c r="J31" s="41">
         <f t="shared" si="2"/>
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
-    <row r="32" spans="1:10" ht="30" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:10" ht="29" x14ac:dyDescent="0.35">
       <c r="A32" s="73">
         <v>34</v>
       </c>
@@ -10504,7 +10071,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="33" spans="1:10" ht="30" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:10" ht="29" x14ac:dyDescent="0.35">
       <c r="A33" s="73">
         <v>35</v>
       </c>
@@ -10515,7 +10082,7 @@
         <v>16</v>
       </c>
       <c r="D33" s="20" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E33" s="17" t="b">
         <v>1</v>
@@ -10528,7 +10095,7 @@
       </c>
       <c r="H33" s="13">
         <f t="shared" si="0"/>
-        <v>-2</v>
+        <v>2</v>
       </c>
       <c r="I33" s="14">
         <f t="shared" si="1"/>
@@ -10536,10 +10103,10 @@
       </c>
       <c r="J33" s="42">
         <f t="shared" si="2"/>
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
-    <row r="34" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A34" s="74">
         <v>36</v>
       </c>
@@ -10550,7 +10117,7 @@
         <v>49</v>
       </c>
       <c r="D34" s="59" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E34" s="45" t="b">
         <v>1</v>
@@ -10559,9 +10126,9 @@
       <c r="G34" s="46">
         <v>2</v>
       </c>
-      <c r="H34" s="47" t="str">
+      <c r="H34" s="47">
         <f t="shared" si="0"/>
-        <v/>
+        <v>2</v>
       </c>
       <c r="I34" s="48">
         <f t="shared" si="1"/>
@@ -10569,10 +10136,10 @@
       </c>
       <c r="J34" s="49">
         <f t="shared" si="2"/>
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
-    <row r="35" spans="1:10" ht="30" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:10" ht="29" x14ac:dyDescent="0.35">
       <c r="A35" s="72">
         <v>37</v>
       </c>
@@ -10607,7 +10174,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="36" spans="1:10" ht="30" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:10" ht="29" x14ac:dyDescent="0.35">
       <c r="A36" s="73">
         <v>38</v>
       </c>
@@ -10642,7 +10209,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="37" spans="1:10" ht="30" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:10" ht="29" x14ac:dyDescent="0.35">
       <c r="A37" s="73">
         <v>39</v>
       </c>
@@ -10677,7 +10244,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="38" spans="1:10" s="1" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:10" s="1" customFormat="1" ht="29" x14ac:dyDescent="0.35">
       <c r="A38" s="73">
         <v>40</v>
       </c>
@@ -10712,7 +10279,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="39" spans="1:10" s="1" customFormat="1" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:10" s="1" customFormat="1" ht="29.5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A39" s="74">
         <v>41</v>
       </c>
@@ -10779,7 +10346,7 @@
                   </from>
                   <to>
                     <xdr:col>4</xdr:col>
-                    <xdr:colOff>104775</xdr:colOff>
+                    <xdr:colOff>107950</xdr:colOff>
                     <xdr:row>1</xdr:row>
                     <xdr:rowOff>209550</xdr:rowOff>
                   </to>
@@ -10801,7 +10368,7 @@
                   </from>
                   <to>
                     <xdr:col>4</xdr:col>
-                    <xdr:colOff>104775</xdr:colOff>
+                    <xdr:colOff>107950</xdr:colOff>
                     <xdr:row>2</xdr:row>
                     <xdr:rowOff>209550</xdr:rowOff>
                   </to>
@@ -10823,7 +10390,7 @@
                   </from>
                   <to>
                     <xdr:col>4</xdr:col>
-                    <xdr:colOff>104775</xdr:colOff>
+                    <xdr:colOff>107950</xdr:colOff>
                     <xdr:row>3</xdr:row>
                     <xdr:rowOff>381000</xdr:rowOff>
                   </to>
@@ -10845,9 +10412,9 @@
                   </from>
                   <to>
                     <xdr:col>4</xdr:col>
-                    <xdr:colOff>104775</xdr:colOff>
+                    <xdr:colOff>107950</xdr:colOff>
                     <xdr:row>4</xdr:row>
-                    <xdr:rowOff>714375</xdr:rowOff>
+                    <xdr:rowOff>717550</xdr:rowOff>
                   </to>
                 </anchor>
               </controlPr>
@@ -10861,7 +10428,7 @@
                 <anchor moveWithCells="1">
                   <from>
                     <xdr:col>3</xdr:col>
-                    <xdr:colOff>28575</xdr:colOff>
+                    <xdr:colOff>31750</xdr:colOff>
                     <xdr:row>5</xdr:row>
                     <xdr:rowOff>19050</xdr:rowOff>
                   </from>
@@ -10889,9 +10456,9 @@
                   </from>
                   <to>
                     <xdr:col>4</xdr:col>
-                    <xdr:colOff>104775</xdr:colOff>
+                    <xdr:colOff>107950</xdr:colOff>
                     <xdr:row>7</xdr:row>
-                    <xdr:rowOff>66675</xdr:rowOff>
+                    <xdr:rowOff>69850</xdr:rowOff>
                   </to>
                 </anchor>
               </controlPr>
@@ -10911,7 +10478,7 @@
                   </from>
                   <to>
                     <xdr:col>4</xdr:col>
-                    <xdr:colOff>104775</xdr:colOff>
+                    <xdr:colOff>107950</xdr:colOff>
                     <xdr:row>7</xdr:row>
                     <xdr:rowOff>209550</xdr:rowOff>
                   </to>
@@ -10933,9 +10500,9 @@
                   </from>
                   <to>
                     <xdr:col>4</xdr:col>
-                    <xdr:colOff>104775</xdr:colOff>
+                    <xdr:colOff>107950</xdr:colOff>
                     <xdr:row>8</xdr:row>
-                    <xdr:rowOff>123825</xdr:rowOff>
+                    <xdr:rowOff>127000</xdr:rowOff>
                   </to>
                 </anchor>
               </controlPr>
@@ -10955,7 +10522,7 @@
                   </from>
                   <to>
                     <xdr:col>4</xdr:col>
-                    <xdr:colOff>104775</xdr:colOff>
+                    <xdr:colOff>107950</xdr:colOff>
                     <xdr:row>10</xdr:row>
                     <xdr:rowOff>0</xdr:rowOff>
                   </to>
@@ -10977,7 +10544,7 @@
                   </from>
                   <to>
                     <xdr:col>4</xdr:col>
-                    <xdr:colOff>104775</xdr:colOff>
+                    <xdr:colOff>107950</xdr:colOff>
                     <xdr:row>11</xdr:row>
                     <xdr:rowOff>0</xdr:rowOff>
                   </to>
@@ -10999,7 +10566,7 @@
                   </from>
                   <to>
                     <xdr:col>4</xdr:col>
-                    <xdr:colOff>104775</xdr:colOff>
+                    <xdr:colOff>107950</xdr:colOff>
                     <xdr:row>11</xdr:row>
                     <xdr:rowOff>209550</xdr:rowOff>
                   </to>
@@ -11021,7 +10588,7 @@
                   </from>
                   <to>
                     <xdr:col>3</xdr:col>
-                    <xdr:colOff>657225</xdr:colOff>
+                    <xdr:colOff>660400</xdr:colOff>
                     <xdr:row>12</xdr:row>
                     <xdr:rowOff>571500</xdr:rowOff>
                   </to>
@@ -11043,7 +10610,7 @@
                   </from>
                   <to>
                     <xdr:col>4</xdr:col>
-                    <xdr:colOff>104775</xdr:colOff>
+                    <xdr:colOff>107950</xdr:colOff>
                     <xdr:row>13</xdr:row>
                     <xdr:rowOff>381000</xdr:rowOff>
                   </to>
@@ -11065,7 +10632,7 @@
                   </from>
                   <to>
                     <xdr:col>4</xdr:col>
-                    <xdr:colOff>104775</xdr:colOff>
+                    <xdr:colOff>107950</xdr:colOff>
                     <xdr:row>14</xdr:row>
                     <xdr:rowOff>209550</xdr:rowOff>
                   </to>
@@ -11087,9 +10654,9 @@
                   </from>
                   <to>
                     <xdr:col>4</xdr:col>
-                    <xdr:colOff>104775</xdr:colOff>
+                    <xdr:colOff>107950</xdr:colOff>
                     <xdr:row>15</xdr:row>
-                    <xdr:rowOff>333375</xdr:rowOff>
+                    <xdr:rowOff>336550</xdr:rowOff>
                   </to>
                 </anchor>
               </controlPr>
@@ -11109,7 +10676,7 @@
                   </from>
                   <to>
                     <xdr:col>4</xdr:col>
-                    <xdr:colOff>104775</xdr:colOff>
+                    <xdr:colOff>107950</xdr:colOff>
                     <xdr:row>17</xdr:row>
                     <xdr:rowOff>0</xdr:rowOff>
                   </to>
@@ -11131,9 +10698,9 @@
                   </from>
                   <to>
                     <xdr:col>4</xdr:col>
-                    <xdr:colOff>104775</xdr:colOff>
+                    <xdr:colOff>107950</xdr:colOff>
                     <xdr:row>17</xdr:row>
-                    <xdr:rowOff>123825</xdr:rowOff>
+                    <xdr:rowOff>127000</xdr:rowOff>
                   </to>
                 </anchor>
               </controlPr>
@@ -11153,7 +10720,7 @@
                   </from>
                   <to>
                     <xdr:col>4</xdr:col>
-                    <xdr:colOff>104775</xdr:colOff>
+                    <xdr:colOff>107950</xdr:colOff>
                     <xdr:row>18</xdr:row>
                     <xdr:rowOff>133350</xdr:rowOff>
                   </to>
@@ -11175,7 +10742,7 @@
                   </from>
                   <to>
                     <xdr:col>4</xdr:col>
-                    <xdr:colOff>104775</xdr:colOff>
+                    <xdr:colOff>107950</xdr:colOff>
                     <xdr:row>20</xdr:row>
                     <xdr:rowOff>0</xdr:rowOff>
                   </to>
@@ -11197,7 +10764,7 @@
                   </from>
                   <to>
                     <xdr:col>4</xdr:col>
-                    <xdr:colOff>104775</xdr:colOff>
+                    <xdr:colOff>107950</xdr:colOff>
                     <xdr:row>20</xdr:row>
                     <xdr:rowOff>209550</xdr:rowOff>
                   </to>
@@ -11219,7 +10786,7 @@
                   </from>
                   <to>
                     <xdr:col>4</xdr:col>
-                    <xdr:colOff>104775</xdr:colOff>
+                    <xdr:colOff>107950</xdr:colOff>
                     <xdr:row>22</xdr:row>
                     <xdr:rowOff>0</xdr:rowOff>
                   </to>
@@ -11241,7 +10808,7 @@
                   </from>
                   <to>
                     <xdr:col>4</xdr:col>
-                    <xdr:colOff>104775</xdr:colOff>
+                    <xdr:colOff>107950</xdr:colOff>
                     <xdr:row>22</xdr:row>
                     <xdr:rowOff>209550</xdr:rowOff>
                   </to>
@@ -11263,7 +10830,7 @@
                   </from>
                   <to>
                     <xdr:col>4</xdr:col>
-                    <xdr:colOff>104775</xdr:colOff>
+                    <xdr:colOff>107950</xdr:colOff>
                     <xdr:row>23</xdr:row>
                     <xdr:rowOff>209550</xdr:rowOff>
                   </to>
@@ -11285,9 +10852,9 @@
                   </from>
                   <to>
                     <xdr:col>4</xdr:col>
-                    <xdr:colOff>104775</xdr:colOff>
+                    <xdr:colOff>107950</xdr:colOff>
                     <xdr:row>24</xdr:row>
-                    <xdr:rowOff>123825</xdr:rowOff>
+                    <xdr:rowOff>127000</xdr:rowOff>
                   </to>
                 </anchor>
               </controlPr>
@@ -11307,7 +10874,7 @@
                   </from>
                   <to>
                     <xdr:col>4</xdr:col>
-                    <xdr:colOff>104775</xdr:colOff>
+                    <xdr:colOff>107950</xdr:colOff>
                     <xdr:row>26</xdr:row>
                     <xdr:rowOff>0</xdr:rowOff>
                   </to>
@@ -11329,7 +10896,7 @@
                   </from>
                   <to>
                     <xdr:col>4</xdr:col>
-                    <xdr:colOff>104775</xdr:colOff>
+                    <xdr:colOff>107950</xdr:colOff>
                     <xdr:row>27</xdr:row>
                     <xdr:rowOff>0</xdr:rowOff>
                   </to>
@@ -11351,7 +10918,7 @@
                   </from>
                   <to>
                     <xdr:col>4</xdr:col>
-                    <xdr:colOff>104775</xdr:colOff>
+                    <xdr:colOff>107950</xdr:colOff>
                     <xdr:row>27</xdr:row>
                     <xdr:rowOff>209550</xdr:rowOff>
                   </to>
@@ -11373,9 +10940,9 @@
                   </from>
                   <to>
                     <xdr:col>4</xdr:col>
-                    <xdr:colOff>104775</xdr:colOff>
+                    <xdr:colOff>107950</xdr:colOff>
                     <xdr:row>28</xdr:row>
-                    <xdr:rowOff>352425</xdr:rowOff>
+                    <xdr:rowOff>355600</xdr:rowOff>
                   </to>
                 </anchor>
               </controlPr>
@@ -11395,7 +10962,7 @@
                   </from>
                   <to>
                     <xdr:col>4</xdr:col>
-                    <xdr:colOff>104775</xdr:colOff>
+                    <xdr:colOff>107950</xdr:colOff>
                     <xdr:row>30</xdr:row>
                     <xdr:rowOff>0</xdr:rowOff>
                   </to>
@@ -11417,7 +10984,7 @@
                   </from>
                   <to>
                     <xdr:col>4</xdr:col>
-                    <xdr:colOff>104775</xdr:colOff>
+                    <xdr:colOff>107950</xdr:colOff>
                     <xdr:row>30</xdr:row>
                     <xdr:rowOff>209550</xdr:rowOff>
                   </to>
@@ -11439,7 +11006,7 @@
                   </from>
                   <to>
                     <xdr:col>4</xdr:col>
-                    <xdr:colOff>104775</xdr:colOff>
+                    <xdr:colOff>107950</xdr:colOff>
                     <xdr:row>32</xdr:row>
                     <xdr:rowOff>0</xdr:rowOff>
                   </to>
@@ -11461,7 +11028,7 @@
                   </from>
                   <to>
                     <xdr:col>4</xdr:col>
-                    <xdr:colOff>104775</xdr:colOff>
+                    <xdr:colOff>107950</xdr:colOff>
                     <xdr:row>32</xdr:row>
                     <xdr:rowOff>209550</xdr:rowOff>
                   </to>
@@ -11483,9 +11050,9 @@
                   </from>
                   <to>
                     <xdr:col>4</xdr:col>
-                    <xdr:colOff>104775</xdr:colOff>
+                    <xdr:colOff>107950</xdr:colOff>
                     <xdr:row>33</xdr:row>
-                    <xdr:rowOff>180975</xdr:rowOff>
+                    <xdr:rowOff>184150</xdr:rowOff>
                   </to>
                 </anchor>
               </controlPr>
@@ -11505,9 +11072,9 @@
                   </from>
                   <to>
                     <xdr:col>4</xdr:col>
-                    <xdr:colOff>104775</xdr:colOff>
+                    <xdr:colOff>107950</xdr:colOff>
                     <xdr:row>35</xdr:row>
-                    <xdr:rowOff>9525</xdr:rowOff>
+                    <xdr:rowOff>12700</xdr:rowOff>
                   </to>
                 </anchor>
               </controlPr>
@@ -11527,7 +11094,7 @@
                   </from>
                   <to>
                     <xdr:col>4</xdr:col>
-                    <xdr:colOff>104775</xdr:colOff>
+                    <xdr:colOff>107950</xdr:colOff>
                     <xdr:row>35</xdr:row>
                     <xdr:rowOff>209550</xdr:rowOff>
                   </to>
@@ -11549,9 +11116,9 @@
                   </from>
                   <to>
                     <xdr:col>4</xdr:col>
-                    <xdr:colOff>104775</xdr:colOff>
+                    <xdr:colOff>107950</xdr:colOff>
                     <xdr:row>36</xdr:row>
-                    <xdr:rowOff>371475</xdr:rowOff>
+                    <xdr:rowOff>374650</xdr:rowOff>
                   </to>
                 </anchor>
               </controlPr>
@@ -11571,7 +11138,7 @@
                   </from>
                   <to>
                     <xdr:col>4</xdr:col>
-                    <xdr:colOff>104775</xdr:colOff>
+                    <xdr:colOff>107950</xdr:colOff>
                     <xdr:row>37</xdr:row>
                     <xdr:rowOff>323850</xdr:rowOff>
                   </to>
@@ -11593,7 +11160,7 @@
                   </from>
                   <to>
                     <xdr:col>4</xdr:col>
-                    <xdr:colOff>104775</xdr:colOff>
+                    <xdr:colOff>107950</xdr:colOff>
                     <xdr:row>38</xdr:row>
                     <xdr:rowOff>381000</xdr:rowOff>
                   </to>
@@ -11683,7 +11250,7 @@
                     <xdr:col>5</xdr:col>
                     <xdr:colOff>152400</xdr:colOff>
                     <xdr:row>4</xdr:row>
-                    <xdr:rowOff>714375</xdr:rowOff>
+                    <xdr:rowOff>717550</xdr:rowOff>
                   </to>
                 </anchor>
               </controlPr>
@@ -11699,7 +11266,7 @@
                     <xdr:col>4</xdr:col>
                     <xdr:colOff>0</xdr:colOff>
                     <xdr:row>5</xdr:row>
-                    <xdr:rowOff>9525</xdr:rowOff>
+                    <xdr:rowOff>12700</xdr:rowOff>
                   </from>
                   <to>
                     <xdr:col>4</xdr:col>
@@ -11727,7 +11294,7 @@
                     <xdr:col>5</xdr:col>
                     <xdr:colOff>152400</xdr:colOff>
                     <xdr:row>7</xdr:row>
-                    <xdr:rowOff>66675</xdr:rowOff>
+                    <xdr:rowOff>69850</xdr:rowOff>
                   </to>
                 </anchor>
               </controlPr>
@@ -11771,7 +11338,7 @@
                     <xdr:col>5</xdr:col>
                     <xdr:colOff>152400</xdr:colOff>
                     <xdr:row>8</xdr:row>
-                    <xdr:rowOff>123825</xdr:rowOff>
+                    <xdr:rowOff>127000</xdr:rowOff>
                   </to>
                 </anchor>
               </controlPr>
@@ -11857,7 +11424,7 @@
                   </from>
                   <to>
                     <xdr:col>4</xdr:col>
-                    <xdr:colOff>695325</xdr:colOff>
+                    <xdr:colOff>698500</xdr:colOff>
                     <xdr:row>12</xdr:row>
                     <xdr:rowOff>571500</xdr:rowOff>
                   </to>
@@ -11925,7 +11492,7 @@
                     <xdr:col>5</xdr:col>
                     <xdr:colOff>152400</xdr:colOff>
                     <xdr:row>15</xdr:row>
-                    <xdr:rowOff>333375</xdr:rowOff>
+                    <xdr:rowOff>336550</xdr:rowOff>
                   </to>
                 </anchor>
               </controlPr>
@@ -11969,7 +11536,7 @@
                     <xdr:col>5</xdr:col>
                     <xdr:colOff>152400</xdr:colOff>
                     <xdr:row>17</xdr:row>
-                    <xdr:rowOff>123825</xdr:rowOff>
+                    <xdr:rowOff>127000</xdr:rowOff>
                   </to>
                 </anchor>
               </controlPr>
@@ -12123,7 +11690,7 @@
                     <xdr:col>5</xdr:col>
                     <xdr:colOff>152400</xdr:colOff>
                     <xdr:row>24</xdr:row>
-                    <xdr:rowOff>123825</xdr:rowOff>
+                    <xdr:rowOff>127000</xdr:rowOff>
                   </to>
                 </anchor>
               </controlPr>
@@ -12321,7 +11888,7 @@
                     <xdr:col>5</xdr:col>
                     <xdr:colOff>152400</xdr:colOff>
                     <xdr:row>34</xdr:row>
-                    <xdr:rowOff>28575</xdr:rowOff>
+                    <xdr:rowOff>31750</xdr:rowOff>
                   </to>
                 </anchor>
               </controlPr>
@@ -12343,7 +11910,7 @@
                     <xdr:col>5</xdr:col>
                     <xdr:colOff>152400</xdr:colOff>
                     <xdr:row>35</xdr:row>
-                    <xdr:rowOff>9525</xdr:rowOff>
+                    <xdr:rowOff>12700</xdr:rowOff>
                   </to>
                 </anchor>
               </controlPr>
@@ -12403,13 +11970,13 @@
                     <xdr:col>4</xdr:col>
                     <xdr:colOff>19050</xdr:colOff>
                     <xdr:row>37</xdr:row>
-                    <xdr:rowOff>85725</xdr:rowOff>
+                    <xdr:rowOff>88900</xdr:rowOff>
                   </from>
                   <to>
                     <xdr:col>5</xdr:col>
                     <xdr:colOff>171450</xdr:colOff>
                     <xdr:row>37</xdr:row>
-                    <xdr:rowOff>295275</xdr:rowOff>
+                    <xdr:rowOff>298450</xdr:rowOff>
                   </to>
                 </anchor>
               </controlPr>
@@ -12445,7 +12012,7 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Munka6"/>
   <dimension ref="A1:H19"/>
   <sheetViews>
@@ -12453,17 +12020,17 @@
       <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="9.140625" style="10"/>
-    <col min="3" max="3" width="11.7109375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="17.7109375" customWidth="1"/>
-    <col min="7" max="7" width="16.42578125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="13.7109375" customWidth="1"/>
-    <col min="13" max="13" width="13.28515625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="9.1796875" style="10"/>
+    <col min="3" max="3" width="11.7265625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="17.7265625" customWidth="1"/>
+    <col min="7" max="7" width="16.453125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="13.7265625" customWidth="1"/>
+    <col min="13" max="13" width="13.26953125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="1" spans="2:8" x14ac:dyDescent="0.35">
       <c r="B1" s="11" t="s">
         <v>31</v>
       </c>
@@ -12476,7 +12043,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="2" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="2" spans="2:8" x14ac:dyDescent="0.35">
       <c r="B2" s="2"/>
       <c r="C2" s="2">
         <v>140</v>
@@ -12489,7 +12056,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="3" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="3" spans="2:8" x14ac:dyDescent="0.35">
       <c r="B3" s="8">
         <v>0.4</v>
       </c>
@@ -12506,7 +12073,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="4" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="4" spans="2:8" x14ac:dyDescent="0.35">
       <c r="B4" s="8">
         <v>0.55000000000000004</v>
       </c>
@@ -12524,7 +12091,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="5" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="5" spans="2:8" x14ac:dyDescent="0.35">
       <c r="B5" s="8">
         <v>0.7</v>
       </c>
@@ -12542,7 +12109,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="6" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="6" spans="2:8" x14ac:dyDescent="0.35">
       <c r="B6" s="8">
         <v>0.85</v>
       </c>
@@ -12560,7 +12127,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="7" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="7" spans="2:8" x14ac:dyDescent="0.35">
       <c r="B7" s="8">
         <v>1</v>
       </c>
@@ -12578,7 +12145,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="8" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="8" spans="2:8" x14ac:dyDescent="0.35">
       <c r="D8" s="5"/>
       <c r="G8">
         <v>12</v>
@@ -12587,7 +12154,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="9" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="9" spans="2:8" x14ac:dyDescent="0.35">
       <c r="G9">
         <v>14</v>
       </c>
@@ -12595,7 +12162,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="10" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="10" spans="2:8" x14ac:dyDescent="0.35">
       <c r="G10">
         <v>16</v>
       </c>
@@ -12603,7 +12170,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="11" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="11" spans="2:8" x14ac:dyDescent="0.35">
       <c r="G11">
         <v>18</v>
       </c>
@@ -12611,7 +12178,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="12" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="12" spans="2:8" x14ac:dyDescent="0.35">
       <c r="G12">
         <v>20</v>
       </c>
@@ -12619,7 +12186,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="19" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B19" s="1"/>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
kisebb javítások css ben
</commit_message>
<xml_diff>
--- a/egyebek/WebprogramozásBeadandóHtmlCssBootstrap.xlsx
+++ b/egyebek/WebprogramozásBeadandóHtmlCssBootstrap.xlsx
@@ -5,11 +5,11 @@
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Latitude\OneDrive\Dokumentumok\Suli\Közgáz\Programozás\Webprogramozás\Beadandó\egyebek\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Hegedűs Gergő\Desktop\beadando\egyebek\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Fedőlap" sheetId="2" r:id="rId1"/>
@@ -20,7 +20,7 @@
     <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">Irányelvek!$A$1:$L$39</definedName>
     <definedName name="nem_modosithato2">Irányelvek!$J:$J,Irányelvek!$I:$I,Irányelvek!$H$1,Irányelvek!$G:$G,Irányelvek!$H:$H,Irányelvek!$F:$F,Irányelvek!$C:$C,Irányelvek!$B:$B,Irányelvek!$A:$A</definedName>
   </definedNames>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="152511"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
@@ -306,7 +306,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="3">
     <numFmt numFmtId="43" formatCode="_-* #,##0.00\ _F_t_-;\-* #,##0.00\ _F_t_-;_-* &quot;-&quot;??\ _F_t_-;_-@_-"/>
     <numFmt numFmtId="164" formatCode=";;;"/>
@@ -1196,6 +1196,12 @@
     <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
     <xf numFmtId="0" fontId="17" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1219,12 +1225,6 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="2" applyBorder="1" applyAlignment="1" applyProtection="1">
       <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="14" fillId="3" borderId="0" xfId="2" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1395,7 +1395,7 @@
 </file>
 
 <file path=xl/ctrlProps/ctrlProp31.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" fmlaLink="D32" lockText="1" noThreeD="1"/>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" checked="Checked" fmlaLink="D32" lockText="1" noThreeD="1"/>
 </file>
 
 <file path=xl/ctrlProps/ctrlProp32.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1519,7 +1519,7 @@
 </file>
 
 <file path=xl/ctrlProps/ctrlProp6.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" fmlaLink="D7" lockText="1" noThreeD="1"/>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" checked="Checked" fmlaLink="D7" lockText="1" noThreeD="1"/>
 </file>
 
 <file path=xl/ctrlProps/ctrlProp60.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1563,7 +1563,7 @@
 </file>
 
 <file path=xl/ctrlProps/ctrlProp7.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" fmlaLink="D8" lockText="1" noThreeD="1"/>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" checked="Checked" fmlaLink="D8" lockText="1" noThreeD="1"/>
 </file>
 
 <file path=xl/ctrlProps/ctrlProp70.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1623,7 +1623,7 @@
           <a:hlinkClick xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-000063370B00}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0100-000063370B00}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1690,7 +1690,7 @@
         </xdr:from>
         <xdr:to>
           <xdr:col>4</xdr:col>
-          <xdr:colOff>107950</xdr:colOff>
+          <xdr:colOff>104775</xdr:colOff>
           <xdr:row>1</xdr:row>
           <xdr:rowOff>209550</xdr:rowOff>
         </xdr:to>
@@ -1702,7 +1702,7 @@
                   <a14:compatExt spid="_x0000_s734509"/>
                 </a:ext>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-00002D350B00}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0100-00002D350B00}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -1741,7 +1741,7 @@
             </a:extLst>
           </xdr:spPr>
           <xdr:txBody>
-            <a:bodyPr vertOverflow="clip" wrap="square" lIns="36576" tIns="22860" rIns="0" bIns="22860" anchor="ctr" upright="1"/>
+            <a:bodyPr vertOverflow="clip" wrap="square" lIns="27432" tIns="18288" rIns="0" bIns="18288" anchor="ctr" upright="1"/>
             <a:lstStyle/>
             <a:p>
               <a:pPr algn="l" rtl="0">
@@ -1777,7 +1777,7 @@
         </xdr:from>
         <xdr:to>
           <xdr:col>4</xdr:col>
-          <xdr:colOff>107950</xdr:colOff>
+          <xdr:colOff>104775</xdr:colOff>
           <xdr:row>2</xdr:row>
           <xdr:rowOff>209550</xdr:rowOff>
         </xdr:to>
@@ -1789,7 +1789,7 @@
                   <a14:compatExt spid="_x0000_s734510"/>
                 </a:ext>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-00002E350B00}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0100-00002E350B00}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -1828,7 +1828,7 @@
             </a:extLst>
           </xdr:spPr>
           <xdr:txBody>
-            <a:bodyPr vertOverflow="clip" wrap="square" lIns="36576" tIns="22860" rIns="0" bIns="22860" anchor="ctr" upright="1"/>
+            <a:bodyPr vertOverflow="clip" wrap="square" lIns="27432" tIns="18288" rIns="0" bIns="18288" anchor="ctr" upright="1"/>
             <a:lstStyle/>
             <a:p>
               <a:pPr algn="l" rtl="0">
@@ -1864,7 +1864,7 @@
         </xdr:from>
         <xdr:to>
           <xdr:col>4</xdr:col>
-          <xdr:colOff>107950</xdr:colOff>
+          <xdr:colOff>104775</xdr:colOff>
           <xdr:row>3</xdr:row>
           <xdr:rowOff>381000</xdr:rowOff>
         </xdr:to>
@@ -1876,7 +1876,7 @@
                   <a14:compatExt spid="_x0000_s734511"/>
                 </a:ext>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-00002F350B00}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0100-00002F350B00}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -1915,7 +1915,7 @@
             </a:extLst>
           </xdr:spPr>
           <xdr:txBody>
-            <a:bodyPr vertOverflow="clip" wrap="square" lIns="36576" tIns="22860" rIns="0" bIns="22860" anchor="ctr" upright="1"/>
+            <a:bodyPr vertOverflow="clip" wrap="square" lIns="27432" tIns="18288" rIns="0" bIns="18288" anchor="ctr" upright="1"/>
             <a:lstStyle/>
             <a:p>
               <a:pPr algn="l" rtl="0">
@@ -1951,9 +1951,9 @@
         </xdr:from>
         <xdr:to>
           <xdr:col>4</xdr:col>
-          <xdr:colOff>107950</xdr:colOff>
+          <xdr:colOff>104775</xdr:colOff>
           <xdr:row>4</xdr:row>
-          <xdr:rowOff>717550</xdr:rowOff>
+          <xdr:rowOff>714375</xdr:rowOff>
         </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
@@ -1963,7 +1963,7 @@
                   <a14:compatExt spid="_x0000_s734512"/>
                 </a:ext>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-000030350B00}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0100-000030350B00}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -2002,7 +2002,7 @@
             </a:extLst>
           </xdr:spPr>
           <xdr:txBody>
-            <a:bodyPr vertOverflow="clip" wrap="square" lIns="36576" tIns="22860" rIns="0" bIns="22860" anchor="ctr" upright="1"/>
+            <a:bodyPr vertOverflow="clip" wrap="square" lIns="27432" tIns="18288" rIns="0" bIns="18288" anchor="ctr" upright="1"/>
             <a:lstStyle/>
             <a:p>
               <a:pPr algn="l" rtl="0">
@@ -2032,7 +2032,7 @@
       <xdr:twoCellAnchor editAs="oneCell">
         <xdr:from>
           <xdr:col>3</xdr:col>
-          <xdr:colOff>31750</xdr:colOff>
+          <xdr:colOff>28575</xdr:colOff>
           <xdr:row>5</xdr:row>
           <xdr:rowOff>19050</xdr:rowOff>
         </xdr:from>
@@ -2050,7 +2050,7 @@
                   <a14:compatExt spid="_x0000_s734516"/>
                 </a:ext>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-000034350B00}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0100-000034350B00}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -2089,7 +2089,7 @@
             </a:extLst>
           </xdr:spPr>
           <xdr:txBody>
-            <a:bodyPr vertOverflow="clip" wrap="square" lIns="36576" tIns="22860" rIns="0" bIns="22860" anchor="ctr" upright="1"/>
+            <a:bodyPr vertOverflow="clip" wrap="square" lIns="27432" tIns="18288" rIns="0" bIns="18288" anchor="ctr" upright="1"/>
             <a:lstStyle/>
             <a:p>
               <a:pPr algn="l" rtl="0">
@@ -2125,9 +2125,9 @@
         </xdr:from>
         <xdr:to>
           <xdr:col>4</xdr:col>
-          <xdr:colOff>107950</xdr:colOff>
+          <xdr:colOff>104775</xdr:colOff>
           <xdr:row>7</xdr:row>
-          <xdr:rowOff>69850</xdr:rowOff>
+          <xdr:rowOff>66675</xdr:rowOff>
         </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
@@ -2137,7 +2137,7 @@
                   <a14:compatExt spid="_x0000_s734517"/>
                 </a:ext>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-000035350B00}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0100-000035350B00}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -2176,7 +2176,7 @@
             </a:extLst>
           </xdr:spPr>
           <xdr:txBody>
-            <a:bodyPr vertOverflow="clip" wrap="square" lIns="36576" tIns="22860" rIns="0" bIns="22860" anchor="ctr" upright="1"/>
+            <a:bodyPr vertOverflow="clip" wrap="square" lIns="27432" tIns="18288" rIns="0" bIns="18288" anchor="ctr" upright="1"/>
             <a:lstStyle/>
             <a:p>
               <a:pPr algn="l" rtl="0">
@@ -2212,7 +2212,7 @@
         </xdr:from>
         <xdr:to>
           <xdr:col>4</xdr:col>
-          <xdr:colOff>107950</xdr:colOff>
+          <xdr:colOff>104775</xdr:colOff>
           <xdr:row>7</xdr:row>
           <xdr:rowOff>209550</xdr:rowOff>
         </xdr:to>
@@ -2224,7 +2224,7 @@
                   <a14:compatExt spid="_x0000_s734518"/>
                 </a:ext>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-000036350B00}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0100-000036350B00}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -2263,7 +2263,7 @@
             </a:extLst>
           </xdr:spPr>
           <xdr:txBody>
-            <a:bodyPr vertOverflow="clip" wrap="square" lIns="36576" tIns="22860" rIns="0" bIns="22860" anchor="ctr" upright="1"/>
+            <a:bodyPr vertOverflow="clip" wrap="square" lIns="27432" tIns="18288" rIns="0" bIns="18288" anchor="ctr" upright="1"/>
             <a:lstStyle/>
             <a:p>
               <a:pPr algn="l" rtl="0">
@@ -2299,9 +2299,9 @@
         </xdr:from>
         <xdr:to>
           <xdr:col>4</xdr:col>
-          <xdr:colOff>107950</xdr:colOff>
+          <xdr:colOff>104775</xdr:colOff>
           <xdr:row>8</xdr:row>
-          <xdr:rowOff>127000</xdr:rowOff>
+          <xdr:rowOff>123825</xdr:rowOff>
         </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
@@ -2311,7 +2311,7 @@
                   <a14:compatExt spid="_x0000_s734519"/>
                 </a:ext>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-000037350B00}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0100-000037350B00}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -2350,7 +2350,7 @@
             </a:extLst>
           </xdr:spPr>
           <xdr:txBody>
-            <a:bodyPr vertOverflow="clip" wrap="square" lIns="36576" tIns="22860" rIns="0" bIns="22860" anchor="ctr" upright="1"/>
+            <a:bodyPr vertOverflow="clip" wrap="square" lIns="27432" tIns="18288" rIns="0" bIns="18288" anchor="ctr" upright="1"/>
             <a:lstStyle/>
             <a:p>
               <a:pPr algn="l" rtl="0">
@@ -2386,7 +2386,7 @@
         </xdr:from>
         <xdr:to>
           <xdr:col>4</xdr:col>
-          <xdr:colOff>107950</xdr:colOff>
+          <xdr:colOff>104775</xdr:colOff>
           <xdr:row>10</xdr:row>
           <xdr:rowOff>0</xdr:rowOff>
         </xdr:to>
@@ -2398,7 +2398,7 @@
                   <a14:compatExt spid="_x0000_s734520"/>
                 </a:ext>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-000038350B00}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0100-000038350B00}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -2437,7 +2437,7 @@
             </a:extLst>
           </xdr:spPr>
           <xdr:txBody>
-            <a:bodyPr vertOverflow="clip" wrap="square" lIns="36576" tIns="22860" rIns="0" bIns="22860" anchor="ctr" upright="1"/>
+            <a:bodyPr vertOverflow="clip" wrap="square" lIns="27432" tIns="18288" rIns="0" bIns="18288" anchor="ctr" upright="1"/>
             <a:lstStyle/>
             <a:p>
               <a:pPr algn="l" rtl="0">
@@ -2473,7 +2473,7 @@
         </xdr:from>
         <xdr:to>
           <xdr:col>4</xdr:col>
-          <xdr:colOff>107950</xdr:colOff>
+          <xdr:colOff>104775</xdr:colOff>
           <xdr:row>11</xdr:row>
           <xdr:rowOff>0</xdr:rowOff>
         </xdr:to>
@@ -2485,7 +2485,7 @@
                   <a14:compatExt spid="_x0000_s734521"/>
                 </a:ext>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-000039350B00}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0100-000039350B00}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -2524,7 +2524,7 @@
             </a:extLst>
           </xdr:spPr>
           <xdr:txBody>
-            <a:bodyPr vertOverflow="clip" wrap="square" lIns="36576" tIns="22860" rIns="0" bIns="22860" anchor="ctr" upright="1"/>
+            <a:bodyPr vertOverflow="clip" wrap="square" lIns="27432" tIns="18288" rIns="0" bIns="18288" anchor="ctr" upright="1"/>
             <a:lstStyle/>
             <a:p>
               <a:pPr algn="l" rtl="0">
@@ -2560,7 +2560,7 @@
         </xdr:from>
         <xdr:to>
           <xdr:col>4</xdr:col>
-          <xdr:colOff>107950</xdr:colOff>
+          <xdr:colOff>104775</xdr:colOff>
           <xdr:row>11</xdr:row>
           <xdr:rowOff>209550</xdr:rowOff>
         </xdr:to>
@@ -2572,7 +2572,7 @@
                   <a14:compatExt spid="_x0000_s734522"/>
                 </a:ext>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-00003A350B00}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0100-00003A350B00}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -2611,7 +2611,7 @@
             </a:extLst>
           </xdr:spPr>
           <xdr:txBody>
-            <a:bodyPr vertOverflow="clip" wrap="square" lIns="36576" tIns="22860" rIns="0" bIns="22860" anchor="ctr" upright="1"/>
+            <a:bodyPr vertOverflow="clip" wrap="square" lIns="27432" tIns="18288" rIns="0" bIns="18288" anchor="ctr" upright="1"/>
             <a:lstStyle/>
             <a:p>
               <a:pPr algn="l" rtl="0">
@@ -2647,7 +2647,7 @@
         </xdr:from>
         <xdr:to>
           <xdr:col>3</xdr:col>
-          <xdr:colOff>660400</xdr:colOff>
+          <xdr:colOff>657225</xdr:colOff>
           <xdr:row>12</xdr:row>
           <xdr:rowOff>571500</xdr:rowOff>
         </xdr:to>
@@ -2659,7 +2659,7 @@
                   <a14:compatExt spid="_x0000_s734523"/>
                 </a:ext>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-00003B350B00}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0100-00003B350B00}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -2698,7 +2698,7 @@
             </a:extLst>
           </xdr:spPr>
           <xdr:txBody>
-            <a:bodyPr vertOverflow="clip" wrap="square" lIns="36576" tIns="22860" rIns="0" bIns="22860" anchor="ctr" upright="1"/>
+            <a:bodyPr vertOverflow="clip" wrap="square" lIns="27432" tIns="18288" rIns="0" bIns="18288" anchor="ctr" upright="1"/>
             <a:lstStyle/>
             <a:p>
               <a:pPr algn="l" rtl="0">
@@ -2734,7 +2734,7 @@
         </xdr:from>
         <xdr:to>
           <xdr:col>4</xdr:col>
-          <xdr:colOff>107950</xdr:colOff>
+          <xdr:colOff>104775</xdr:colOff>
           <xdr:row>13</xdr:row>
           <xdr:rowOff>381000</xdr:rowOff>
         </xdr:to>
@@ -2746,7 +2746,7 @@
                   <a14:compatExt spid="_x0000_s734524"/>
                 </a:ext>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-00003C350B00}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0100-00003C350B00}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -2785,7 +2785,7 @@
             </a:extLst>
           </xdr:spPr>
           <xdr:txBody>
-            <a:bodyPr vertOverflow="clip" wrap="square" lIns="36576" tIns="22860" rIns="0" bIns="22860" anchor="ctr" upright="1"/>
+            <a:bodyPr vertOverflow="clip" wrap="square" lIns="27432" tIns="18288" rIns="0" bIns="18288" anchor="ctr" upright="1"/>
             <a:lstStyle/>
             <a:p>
               <a:pPr algn="l" rtl="0">
@@ -2821,7 +2821,7 @@
         </xdr:from>
         <xdr:to>
           <xdr:col>4</xdr:col>
-          <xdr:colOff>107950</xdr:colOff>
+          <xdr:colOff>104775</xdr:colOff>
           <xdr:row>14</xdr:row>
           <xdr:rowOff>209550</xdr:rowOff>
         </xdr:to>
@@ -2833,7 +2833,7 @@
                   <a14:compatExt spid="_x0000_s734525"/>
                 </a:ext>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-00003D350B00}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0100-00003D350B00}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -2872,7 +2872,7 @@
             </a:extLst>
           </xdr:spPr>
           <xdr:txBody>
-            <a:bodyPr vertOverflow="clip" wrap="square" lIns="36576" tIns="22860" rIns="0" bIns="22860" anchor="ctr" upright="1"/>
+            <a:bodyPr vertOverflow="clip" wrap="square" lIns="27432" tIns="18288" rIns="0" bIns="18288" anchor="ctr" upright="1"/>
             <a:lstStyle/>
             <a:p>
               <a:pPr algn="l" rtl="0">
@@ -2908,9 +2908,9 @@
         </xdr:from>
         <xdr:to>
           <xdr:col>4</xdr:col>
-          <xdr:colOff>107950</xdr:colOff>
+          <xdr:colOff>104775</xdr:colOff>
           <xdr:row>15</xdr:row>
-          <xdr:rowOff>336550</xdr:rowOff>
+          <xdr:rowOff>333375</xdr:rowOff>
         </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
@@ -2920,7 +2920,7 @@
                   <a14:compatExt spid="_x0000_s734526"/>
                 </a:ext>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-00003E350B00}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0100-00003E350B00}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -2959,7 +2959,7 @@
             </a:extLst>
           </xdr:spPr>
           <xdr:txBody>
-            <a:bodyPr vertOverflow="clip" wrap="square" lIns="36576" tIns="22860" rIns="0" bIns="22860" anchor="ctr" upright="1"/>
+            <a:bodyPr vertOverflow="clip" wrap="square" lIns="27432" tIns="18288" rIns="0" bIns="18288" anchor="ctr" upright="1"/>
             <a:lstStyle/>
             <a:p>
               <a:pPr algn="l" rtl="0">
@@ -2995,7 +2995,7 @@
         </xdr:from>
         <xdr:to>
           <xdr:col>4</xdr:col>
-          <xdr:colOff>107950</xdr:colOff>
+          <xdr:colOff>104775</xdr:colOff>
           <xdr:row>17</xdr:row>
           <xdr:rowOff>0</xdr:rowOff>
         </xdr:to>
@@ -3007,7 +3007,7 @@
                   <a14:compatExt spid="_x0000_s734528"/>
                 </a:ext>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-000040350B00}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0100-000040350B00}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -3046,7 +3046,7 @@
             </a:extLst>
           </xdr:spPr>
           <xdr:txBody>
-            <a:bodyPr vertOverflow="clip" wrap="square" lIns="36576" tIns="22860" rIns="0" bIns="22860" anchor="ctr" upright="1"/>
+            <a:bodyPr vertOverflow="clip" wrap="square" lIns="27432" tIns="18288" rIns="0" bIns="18288" anchor="ctr" upright="1"/>
             <a:lstStyle/>
             <a:p>
               <a:pPr algn="l" rtl="0">
@@ -3082,9 +3082,9 @@
         </xdr:from>
         <xdr:to>
           <xdr:col>4</xdr:col>
-          <xdr:colOff>107950</xdr:colOff>
+          <xdr:colOff>104775</xdr:colOff>
           <xdr:row>17</xdr:row>
-          <xdr:rowOff>127000</xdr:rowOff>
+          <xdr:rowOff>123825</xdr:rowOff>
         </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
@@ -3094,7 +3094,7 @@
                   <a14:compatExt spid="_x0000_s734531"/>
                 </a:ext>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-000043350B00}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0100-000043350B00}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -3133,7 +3133,7 @@
             </a:extLst>
           </xdr:spPr>
           <xdr:txBody>
-            <a:bodyPr vertOverflow="clip" wrap="square" lIns="36576" tIns="22860" rIns="0" bIns="22860" anchor="ctr" upright="1"/>
+            <a:bodyPr vertOverflow="clip" wrap="square" lIns="27432" tIns="18288" rIns="0" bIns="18288" anchor="ctr" upright="1"/>
             <a:lstStyle/>
             <a:p>
               <a:pPr algn="l" rtl="0">
@@ -3169,7 +3169,7 @@
         </xdr:from>
         <xdr:to>
           <xdr:col>4</xdr:col>
-          <xdr:colOff>107950</xdr:colOff>
+          <xdr:colOff>104775</xdr:colOff>
           <xdr:row>18</xdr:row>
           <xdr:rowOff>133350</xdr:rowOff>
         </xdr:to>
@@ -3181,7 +3181,7 @@
                   <a14:compatExt spid="_x0000_s734540"/>
                 </a:ext>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-00004C350B00}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0100-00004C350B00}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -3220,7 +3220,7 @@
             </a:extLst>
           </xdr:spPr>
           <xdr:txBody>
-            <a:bodyPr vertOverflow="clip" wrap="square" lIns="36576" tIns="22860" rIns="0" bIns="22860" anchor="ctr" upright="1"/>
+            <a:bodyPr vertOverflow="clip" wrap="square" lIns="27432" tIns="18288" rIns="0" bIns="18288" anchor="ctr" upright="1"/>
             <a:lstStyle/>
             <a:p>
               <a:pPr algn="l" rtl="0">
@@ -3256,7 +3256,7 @@
         </xdr:from>
         <xdr:to>
           <xdr:col>4</xdr:col>
-          <xdr:colOff>107950</xdr:colOff>
+          <xdr:colOff>104775</xdr:colOff>
           <xdr:row>20</xdr:row>
           <xdr:rowOff>0</xdr:rowOff>
         </xdr:to>
@@ -3268,7 +3268,7 @@
                   <a14:compatExt spid="_x0000_s734541"/>
                 </a:ext>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-00004D350B00}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0100-00004D350B00}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -3307,7 +3307,7 @@
             </a:extLst>
           </xdr:spPr>
           <xdr:txBody>
-            <a:bodyPr vertOverflow="clip" wrap="square" lIns="36576" tIns="22860" rIns="0" bIns="22860" anchor="ctr" upright="1"/>
+            <a:bodyPr vertOverflow="clip" wrap="square" lIns="27432" tIns="18288" rIns="0" bIns="18288" anchor="ctr" upright="1"/>
             <a:lstStyle/>
             <a:p>
               <a:pPr algn="l" rtl="0">
@@ -3343,7 +3343,7 @@
         </xdr:from>
         <xdr:to>
           <xdr:col>4</xdr:col>
-          <xdr:colOff>107950</xdr:colOff>
+          <xdr:colOff>104775</xdr:colOff>
           <xdr:row>20</xdr:row>
           <xdr:rowOff>209550</xdr:rowOff>
         </xdr:to>
@@ -3355,7 +3355,7 @@
                   <a14:compatExt spid="_x0000_s734542"/>
                 </a:ext>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-00004E350B00}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0100-00004E350B00}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -3394,7 +3394,7 @@
             </a:extLst>
           </xdr:spPr>
           <xdr:txBody>
-            <a:bodyPr vertOverflow="clip" wrap="square" lIns="36576" tIns="22860" rIns="0" bIns="22860" anchor="ctr" upright="1"/>
+            <a:bodyPr vertOverflow="clip" wrap="square" lIns="27432" tIns="18288" rIns="0" bIns="18288" anchor="ctr" upright="1"/>
             <a:lstStyle/>
             <a:p>
               <a:pPr algn="l" rtl="0">
@@ -3430,7 +3430,7 @@
         </xdr:from>
         <xdr:to>
           <xdr:col>4</xdr:col>
-          <xdr:colOff>107950</xdr:colOff>
+          <xdr:colOff>104775</xdr:colOff>
           <xdr:row>22</xdr:row>
           <xdr:rowOff>0</xdr:rowOff>
         </xdr:to>
@@ -3442,7 +3442,7 @@
                   <a14:compatExt spid="_x0000_s734543"/>
                 </a:ext>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-00004F350B00}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0100-00004F350B00}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -3481,7 +3481,7 @@
             </a:extLst>
           </xdr:spPr>
           <xdr:txBody>
-            <a:bodyPr vertOverflow="clip" wrap="square" lIns="36576" tIns="22860" rIns="0" bIns="22860" anchor="ctr" upright="1"/>
+            <a:bodyPr vertOverflow="clip" wrap="square" lIns="27432" tIns="18288" rIns="0" bIns="18288" anchor="ctr" upright="1"/>
             <a:lstStyle/>
             <a:p>
               <a:pPr algn="l" rtl="0">
@@ -3517,7 +3517,7 @@
         </xdr:from>
         <xdr:to>
           <xdr:col>4</xdr:col>
-          <xdr:colOff>107950</xdr:colOff>
+          <xdr:colOff>104775</xdr:colOff>
           <xdr:row>22</xdr:row>
           <xdr:rowOff>209550</xdr:rowOff>
         </xdr:to>
@@ -3529,7 +3529,7 @@
                   <a14:compatExt spid="_x0000_s734544"/>
                 </a:ext>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-000050350B00}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0100-000050350B00}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -3568,7 +3568,7 @@
             </a:extLst>
           </xdr:spPr>
           <xdr:txBody>
-            <a:bodyPr vertOverflow="clip" wrap="square" lIns="36576" tIns="22860" rIns="0" bIns="22860" anchor="ctr" upright="1"/>
+            <a:bodyPr vertOverflow="clip" wrap="square" lIns="27432" tIns="18288" rIns="0" bIns="18288" anchor="ctr" upright="1"/>
             <a:lstStyle/>
             <a:p>
               <a:pPr algn="l" rtl="0">
@@ -3604,7 +3604,7 @@
         </xdr:from>
         <xdr:to>
           <xdr:col>4</xdr:col>
-          <xdr:colOff>107950</xdr:colOff>
+          <xdr:colOff>104775</xdr:colOff>
           <xdr:row>23</xdr:row>
           <xdr:rowOff>209550</xdr:rowOff>
         </xdr:to>
@@ -3616,7 +3616,7 @@
                   <a14:compatExt spid="_x0000_s734545"/>
                 </a:ext>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-000051350B00}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0100-000051350B00}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -3655,7 +3655,7 @@
             </a:extLst>
           </xdr:spPr>
           <xdr:txBody>
-            <a:bodyPr vertOverflow="clip" wrap="square" lIns="36576" tIns="22860" rIns="0" bIns="22860" anchor="ctr" upright="1"/>
+            <a:bodyPr vertOverflow="clip" wrap="square" lIns="27432" tIns="18288" rIns="0" bIns="18288" anchor="ctr" upright="1"/>
             <a:lstStyle/>
             <a:p>
               <a:pPr algn="l" rtl="0">
@@ -3691,9 +3691,9 @@
         </xdr:from>
         <xdr:to>
           <xdr:col>4</xdr:col>
-          <xdr:colOff>107950</xdr:colOff>
+          <xdr:colOff>104775</xdr:colOff>
           <xdr:row>24</xdr:row>
-          <xdr:rowOff>127000</xdr:rowOff>
+          <xdr:rowOff>123825</xdr:rowOff>
         </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
@@ -3703,7 +3703,7 @@
                   <a14:compatExt spid="_x0000_s734546"/>
                 </a:ext>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-000052350B00}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0100-000052350B00}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -3742,7 +3742,7 @@
             </a:extLst>
           </xdr:spPr>
           <xdr:txBody>
-            <a:bodyPr vertOverflow="clip" wrap="square" lIns="36576" tIns="22860" rIns="0" bIns="22860" anchor="ctr" upright="1"/>
+            <a:bodyPr vertOverflow="clip" wrap="square" lIns="27432" tIns="18288" rIns="0" bIns="18288" anchor="ctr" upright="1"/>
             <a:lstStyle/>
             <a:p>
               <a:pPr algn="l" rtl="0">
@@ -3778,7 +3778,7 @@
         </xdr:from>
         <xdr:to>
           <xdr:col>4</xdr:col>
-          <xdr:colOff>107950</xdr:colOff>
+          <xdr:colOff>104775</xdr:colOff>
           <xdr:row>26</xdr:row>
           <xdr:rowOff>0</xdr:rowOff>
         </xdr:to>
@@ -3790,7 +3790,7 @@
                   <a14:compatExt spid="_x0000_s734549"/>
                 </a:ext>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-000055350B00}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0100-000055350B00}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -3829,7 +3829,7 @@
             </a:extLst>
           </xdr:spPr>
           <xdr:txBody>
-            <a:bodyPr vertOverflow="clip" wrap="square" lIns="36576" tIns="22860" rIns="0" bIns="22860" anchor="ctr" upright="1"/>
+            <a:bodyPr vertOverflow="clip" wrap="square" lIns="27432" tIns="18288" rIns="0" bIns="18288" anchor="ctr" upright="1"/>
             <a:lstStyle/>
             <a:p>
               <a:pPr algn="l" rtl="0">
@@ -3865,7 +3865,7 @@
         </xdr:from>
         <xdr:to>
           <xdr:col>4</xdr:col>
-          <xdr:colOff>107950</xdr:colOff>
+          <xdr:colOff>104775</xdr:colOff>
           <xdr:row>27</xdr:row>
           <xdr:rowOff>0</xdr:rowOff>
         </xdr:to>
@@ -3877,7 +3877,7 @@
                   <a14:compatExt spid="_x0000_s734553"/>
                 </a:ext>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-000059350B00}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0100-000059350B00}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -3916,7 +3916,7 @@
             </a:extLst>
           </xdr:spPr>
           <xdr:txBody>
-            <a:bodyPr vertOverflow="clip" wrap="square" lIns="36576" tIns="22860" rIns="0" bIns="22860" anchor="ctr" upright="1"/>
+            <a:bodyPr vertOverflow="clip" wrap="square" lIns="27432" tIns="18288" rIns="0" bIns="18288" anchor="ctr" upright="1"/>
             <a:lstStyle/>
             <a:p>
               <a:pPr algn="l" rtl="0">
@@ -3952,7 +3952,7 @@
         </xdr:from>
         <xdr:to>
           <xdr:col>4</xdr:col>
-          <xdr:colOff>107950</xdr:colOff>
+          <xdr:colOff>104775</xdr:colOff>
           <xdr:row>27</xdr:row>
           <xdr:rowOff>209550</xdr:rowOff>
         </xdr:to>
@@ -3964,7 +3964,7 @@
                   <a14:compatExt spid="_x0000_s734554"/>
                 </a:ext>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-00005A350B00}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0100-00005A350B00}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -4003,7 +4003,7 @@
             </a:extLst>
           </xdr:spPr>
           <xdr:txBody>
-            <a:bodyPr vertOverflow="clip" wrap="square" lIns="36576" tIns="22860" rIns="0" bIns="22860" anchor="ctr" upright="1"/>
+            <a:bodyPr vertOverflow="clip" wrap="square" lIns="27432" tIns="18288" rIns="0" bIns="18288" anchor="ctr" upright="1"/>
             <a:lstStyle/>
             <a:p>
               <a:pPr algn="l" rtl="0">
@@ -4039,9 +4039,9 @@
         </xdr:from>
         <xdr:to>
           <xdr:col>4</xdr:col>
-          <xdr:colOff>107950</xdr:colOff>
+          <xdr:colOff>104775</xdr:colOff>
           <xdr:row>28</xdr:row>
-          <xdr:rowOff>355600</xdr:rowOff>
+          <xdr:rowOff>352425</xdr:rowOff>
         </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
@@ -4051,7 +4051,7 @@
                   <a14:compatExt spid="_x0000_s734555"/>
                 </a:ext>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-00005B350B00}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0100-00005B350B00}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -4090,7 +4090,7 @@
             </a:extLst>
           </xdr:spPr>
           <xdr:txBody>
-            <a:bodyPr vertOverflow="clip" wrap="square" lIns="36576" tIns="22860" rIns="0" bIns="22860" anchor="ctr" upright="1"/>
+            <a:bodyPr vertOverflow="clip" wrap="square" lIns="27432" tIns="18288" rIns="0" bIns="18288" anchor="ctr" upright="1"/>
             <a:lstStyle/>
             <a:p>
               <a:pPr algn="l" rtl="0">
@@ -4126,7 +4126,7 @@
         </xdr:from>
         <xdr:to>
           <xdr:col>4</xdr:col>
-          <xdr:colOff>107950</xdr:colOff>
+          <xdr:colOff>104775</xdr:colOff>
           <xdr:row>30</xdr:row>
           <xdr:rowOff>0</xdr:rowOff>
         </xdr:to>
@@ -4138,7 +4138,7 @@
                   <a14:compatExt spid="_x0000_s734557"/>
                 </a:ext>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-00005D350B00}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0100-00005D350B00}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -4177,7 +4177,7 @@
             </a:extLst>
           </xdr:spPr>
           <xdr:txBody>
-            <a:bodyPr vertOverflow="clip" wrap="square" lIns="36576" tIns="22860" rIns="0" bIns="22860" anchor="ctr" upright="1"/>
+            <a:bodyPr vertOverflow="clip" wrap="square" lIns="27432" tIns="18288" rIns="0" bIns="18288" anchor="ctr" upright="1"/>
             <a:lstStyle/>
             <a:p>
               <a:pPr algn="l" rtl="0">
@@ -4213,7 +4213,7 @@
         </xdr:from>
         <xdr:to>
           <xdr:col>4</xdr:col>
-          <xdr:colOff>107950</xdr:colOff>
+          <xdr:colOff>104775</xdr:colOff>
           <xdr:row>30</xdr:row>
           <xdr:rowOff>209550</xdr:rowOff>
         </xdr:to>
@@ -4225,7 +4225,7 @@
                   <a14:compatExt spid="_x0000_s734558"/>
                 </a:ext>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-00005E350B00}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0100-00005E350B00}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -4264,7 +4264,7 @@
             </a:extLst>
           </xdr:spPr>
           <xdr:txBody>
-            <a:bodyPr vertOverflow="clip" wrap="square" lIns="36576" tIns="22860" rIns="0" bIns="22860" anchor="ctr" upright="1"/>
+            <a:bodyPr vertOverflow="clip" wrap="square" lIns="27432" tIns="18288" rIns="0" bIns="18288" anchor="ctr" upright="1"/>
             <a:lstStyle/>
             <a:p>
               <a:pPr algn="l" rtl="0">
@@ -4300,7 +4300,7 @@
         </xdr:from>
         <xdr:to>
           <xdr:col>4</xdr:col>
-          <xdr:colOff>107950</xdr:colOff>
+          <xdr:colOff>104775</xdr:colOff>
           <xdr:row>32</xdr:row>
           <xdr:rowOff>0</xdr:rowOff>
         </xdr:to>
@@ -4312,7 +4312,7 @@
                   <a14:compatExt spid="_x0000_s734559"/>
                 </a:ext>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-00005F350B00}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0100-00005F350B00}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -4351,7 +4351,7 @@
             </a:extLst>
           </xdr:spPr>
           <xdr:txBody>
-            <a:bodyPr vertOverflow="clip" wrap="square" lIns="36576" tIns="22860" rIns="0" bIns="22860" anchor="ctr" upright="1"/>
+            <a:bodyPr vertOverflow="clip" wrap="square" lIns="27432" tIns="18288" rIns="0" bIns="18288" anchor="ctr" upright="1"/>
             <a:lstStyle/>
             <a:p>
               <a:pPr algn="l" rtl="0">
@@ -4387,7 +4387,7 @@
         </xdr:from>
         <xdr:to>
           <xdr:col>4</xdr:col>
-          <xdr:colOff>107950</xdr:colOff>
+          <xdr:colOff>104775</xdr:colOff>
           <xdr:row>32</xdr:row>
           <xdr:rowOff>209550</xdr:rowOff>
         </xdr:to>
@@ -4399,7 +4399,7 @@
                   <a14:compatExt spid="_x0000_s734560"/>
                 </a:ext>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-000060350B00}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0100-000060350B00}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -4438,7 +4438,7 @@
             </a:extLst>
           </xdr:spPr>
           <xdr:txBody>
-            <a:bodyPr vertOverflow="clip" wrap="square" lIns="36576" tIns="22860" rIns="0" bIns="22860" anchor="ctr" upright="1"/>
+            <a:bodyPr vertOverflow="clip" wrap="square" lIns="27432" tIns="18288" rIns="0" bIns="18288" anchor="ctr" upright="1"/>
             <a:lstStyle/>
             <a:p>
               <a:pPr algn="l" rtl="0">
@@ -4474,9 +4474,9 @@
         </xdr:from>
         <xdr:to>
           <xdr:col>4</xdr:col>
-          <xdr:colOff>107950</xdr:colOff>
+          <xdr:colOff>104775</xdr:colOff>
           <xdr:row>33</xdr:row>
-          <xdr:rowOff>184150</xdr:rowOff>
+          <xdr:rowOff>180975</xdr:rowOff>
         </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
@@ -4486,7 +4486,7 @@
                   <a14:compatExt spid="_x0000_s734565"/>
                 </a:ext>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-000065350B00}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0100-000065350B00}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -4525,7 +4525,7 @@
             </a:extLst>
           </xdr:spPr>
           <xdr:txBody>
-            <a:bodyPr vertOverflow="clip" wrap="square" lIns="36576" tIns="22860" rIns="0" bIns="22860" anchor="ctr" upright="1"/>
+            <a:bodyPr vertOverflow="clip" wrap="square" lIns="27432" tIns="18288" rIns="0" bIns="18288" anchor="ctr" upright="1"/>
             <a:lstStyle/>
             <a:p>
               <a:pPr algn="l" rtl="0">
@@ -4561,9 +4561,9 @@
         </xdr:from>
         <xdr:to>
           <xdr:col>4</xdr:col>
-          <xdr:colOff>107950</xdr:colOff>
+          <xdr:colOff>104775</xdr:colOff>
           <xdr:row>35</xdr:row>
-          <xdr:rowOff>12700</xdr:rowOff>
+          <xdr:rowOff>9525</xdr:rowOff>
         </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
@@ -4573,7 +4573,7 @@
                   <a14:compatExt spid="_x0000_s734566"/>
                 </a:ext>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-000066350B00}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0100-000066350B00}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -4612,7 +4612,7 @@
             </a:extLst>
           </xdr:spPr>
           <xdr:txBody>
-            <a:bodyPr vertOverflow="clip" wrap="square" lIns="36576" tIns="22860" rIns="0" bIns="22860" anchor="ctr" upright="1"/>
+            <a:bodyPr vertOverflow="clip" wrap="square" lIns="27432" tIns="18288" rIns="0" bIns="18288" anchor="ctr" upright="1"/>
             <a:lstStyle/>
             <a:p>
               <a:pPr algn="l" rtl="0">
@@ -4648,7 +4648,7 @@
         </xdr:from>
         <xdr:to>
           <xdr:col>4</xdr:col>
-          <xdr:colOff>107950</xdr:colOff>
+          <xdr:colOff>104775</xdr:colOff>
           <xdr:row>35</xdr:row>
           <xdr:rowOff>209550</xdr:rowOff>
         </xdr:to>
@@ -4660,7 +4660,7 @@
                   <a14:compatExt spid="_x0000_s734567"/>
                 </a:ext>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-000067350B00}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0100-000067350B00}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -4699,7 +4699,7 @@
             </a:extLst>
           </xdr:spPr>
           <xdr:txBody>
-            <a:bodyPr vertOverflow="clip" wrap="square" lIns="36576" tIns="22860" rIns="0" bIns="22860" anchor="ctr" upright="1"/>
+            <a:bodyPr vertOverflow="clip" wrap="square" lIns="27432" tIns="18288" rIns="0" bIns="18288" anchor="ctr" upright="1"/>
             <a:lstStyle/>
             <a:p>
               <a:pPr algn="l" rtl="0">
@@ -4735,9 +4735,9 @@
         </xdr:from>
         <xdr:to>
           <xdr:col>4</xdr:col>
-          <xdr:colOff>107950</xdr:colOff>
+          <xdr:colOff>104775</xdr:colOff>
           <xdr:row>36</xdr:row>
-          <xdr:rowOff>374650</xdr:rowOff>
+          <xdr:rowOff>371475</xdr:rowOff>
         </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
@@ -4747,7 +4747,7 @@
                   <a14:compatExt spid="_x0000_s734568"/>
                 </a:ext>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-000068350B00}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0100-000068350B00}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -4786,7 +4786,7 @@
             </a:extLst>
           </xdr:spPr>
           <xdr:txBody>
-            <a:bodyPr vertOverflow="clip" wrap="square" lIns="36576" tIns="22860" rIns="0" bIns="22860" anchor="ctr" upright="1"/>
+            <a:bodyPr vertOverflow="clip" wrap="square" lIns="27432" tIns="18288" rIns="0" bIns="18288" anchor="ctr" upright="1"/>
             <a:lstStyle/>
             <a:p>
               <a:pPr algn="l" rtl="0">
@@ -4822,7 +4822,7 @@
         </xdr:from>
         <xdr:to>
           <xdr:col>4</xdr:col>
-          <xdr:colOff>107950</xdr:colOff>
+          <xdr:colOff>104775</xdr:colOff>
           <xdr:row>37</xdr:row>
           <xdr:rowOff>323850</xdr:rowOff>
         </xdr:to>
@@ -4834,7 +4834,7 @@
                   <a14:compatExt spid="_x0000_s734572"/>
                 </a:ext>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-00006C350B00}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0100-00006C350B00}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -4873,7 +4873,7 @@
             </a:extLst>
           </xdr:spPr>
           <xdr:txBody>
-            <a:bodyPr vertOverflow="clip" wrap="square" lIns="36576" tIns="22860" rIns="0" bIns="22860" anchor="ctr" upright="1"/>
+            <a:bodyPr vertOverflow="clip" wrap="square" lIns="27432" tIns="18288" rIns="0" bIns="18288" anchor="ctr" upright="1"/>
             <a:lstStyle/>
             <a:p>
               <a:pPr algn="l" rtl="0">
@@ -4909,7 +4909,7 @@
         </xdr:from>
         <xdr:to>
           <xdr:col>4</xdr:col>
-          <xdr:colOff>107950</xdr:colOff>
+          <xdr:colOff>104775</xdr:colOff>
           <xdr:row>38</xdr:row>
           <xdr:rowOff>381000</xdr:rowOff>
         </xdr:to>
@@ -4921,7 +4921,7 @@
                   <a14:compatExt spid="_x0000_s734573"/>
                 </a:ext>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-00006D350B00}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0100-00006D350B00}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -4960,7 +4960,7 @@
             </a:extLst>
           </xdr:spPr>
           <xdr:txBody>
-            <a:bodyPr vertOverflow="clip" wrap="square" lIns="36576" tIns="22860" rIns="0" bIns="22860" anchor="ctr" upright="1"/>
+            <a:bodyPr vertOverflow="clip" wrap="square" lIns="27432" tIns="18288" rIns="0" bIns="18288" anchor="ctr" upright="1"/>
             <a:lstStyle/>
             <a:p>
               <a:pPr algn="l" rtl="0">
@@ -5008,7 +5008,7 @@
                   <a14:compatExt spid="_x0000_s734574"/>
                 </a:ext>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-00006E350B00}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0100-00006E350B00}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -5047,7 +5047,7 @@
             </a:extLst>
           </xdr:spPr>
           <xdr:txBody>
-            <a:bodyPr vertOverflow="clip" wrap="square" lIns="36576" tIns="22860" rIns="0" bIns="22860" anchor="ctr" upright="1"/>
+            <a:bodyPr vertOverflow="clip" wrap="square" lIns="27432" tIns="18288" rIns="0" bIns="18288" anchor="ctr" upright="1"/>
             <a:lstStyle/>
             <a:p>
               <a:pPr algn="l" rtl="0">
@@ -5095,7 +5095,7 @@
                   <a14:compatExt spid="_x0000_s734575"/>
                 </a:ext>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-00006F350B00}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0100-00006F350B00}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -5134,7 +5134,7 @@
             </a:extLst>
           </xdr:spPr>
           <xdr:txBody>
-            <a:bodyPr vertOverflow="clip" wrap="square" lIns="36576" tIns="22860" rIns="0" bIns="22860" anchor="ctr" upright="1"/>
+            <a:bodyPr vertOverflow="clip" wrap="square" lIns="27432" tIns="18288" rIns="0" bIns="18288" anchor="ctr" upright="1"/>
             <a:lstStyle/>
             <a:p>
               <a:pPr algn="l" rtl="0">
@@ -5182,7 +5182,7 @@
                   <a14:compatExt spid="_x0000_s734576"/>
                 </a:ext>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-000070350B00}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0100-000070350B00}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -5221,7 +5221,7 @@
             </a:extLst>
           </xdr:spPr>
           <xdr:txBody>
-            <a:bodyPr vertOverflow="clip" wrap="square" lIns="36576" tIns="22860" rIns="0" bIns="22860" anchor="ctr" upright="1"/>
+            <a:bodyPr vertOverflow="clip" wrap="square" lIns="27432" tIns="18288" rIns="0" bIns="18288" anchor="ctr" upright="1"/>
             <a:lstStyle/>
             <a:p>
               <a:pPr algn="l" rtl="0">
@@ -5259,7 +5259,7 @@
           <xdr:col>5</xdr:col>
           <xdr:colOff>152400</xdr:colOff>
           <xdr:row>4</xdr:row>
-          <xdr:rowOff>717550</xdr:rowOff>
+          <xdr:rowOff>714375</xdr:rowOff>
         </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
@@ -5269,7 +5269,7 @@
                   <a14:compatExt spid="_x0000_s734577"/>
                 </a:ext>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-000071350B00}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0100-000071350B00}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -5308,7 +5308,7 @@
             </a:extLst>
           </xdr:spPr>
           <xdr:txBody>
-            <a:bodyPr vertOverflow="clip" wrap="square" lIns="36576" tIns="22860" rIns="0" bIns="22860" anchor="ctr" upright="1"/>
+            <a:bodyPr vertOverflow="clip" wrap="square" lIns="27432" tIns="18288" rIns="0" bIns="18288" anchor="ctr" upright="1"/>
             <a:lstStyle/>
             <a:p>
               <a:pPr algn="l" rtl="0">
@@ -5340,7 +5340,7 @@
           <xdr:col>4</xdr:col>
           <xdr:colOff>0</xdr:colOff>
           <xdr:row>5</xdr:row>
-          <xdr:rowOff>12700</xdr:rowOff>
+          <xdr:rowOff>9525</xdr:rowOff>
         </xdr:from>
         <xdr:to>
           <xdr:col>4</xdr:col>
@@ -5356,7 +5356,7 @@
                   <a14:compatExt spid="_x0000_s734581"/>
                 </a:ext>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-000075350B00}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0100-000075350B00}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -5395,7 +5395,7 @@
             </a:extLst>
           </xdr:spPr>
           <xdr:txBody>
-            <a:bodyPr vertOverflow="clip" wrap="square" lIns="36576" tIns="22860" rIns="0" bIns="22860" anchor="ctr" upright="1"/>
+            <a:bodyPr vertOverflow="clip" wrap="square" lIns="27432" tIns="18288" rIns="0" bIns="18288" anchor="ctr" upright="1"/>
             <a:lstStyle/>
             <a:p>
               <a:pPr algn="l" rtl="0">
@@ -5433,7 +5433,7 @@
           <xdr:col>5</xdr:col>
           <xdr:colOff>152400</xdr:colOff>
           <xdr:row>7</xdr:row>
-          <xdr:rowOff>69850</xdr:rowOff>
+          <xdr:rowOff>66675</xdr:rowOff>
         </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
@@ -5443,7 +5443,7 @@
                   <a14:compatExt spid="_x0000_s734582"/>
                 </a:ext>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-000076350B00}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0100-000076350B00}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -5482,7 +5482,7 @@
             </a:extLst>
           </xdr:spPr>
           <xdr:txBody>
-            <a:bodyPr vertOverflow="clip" wrap="square" lIns="36576" tIns="22860" rIns="0" bIns="22860" anchor="ctr" upright="1"/>
+            <a:bodyPr vertOverflow="clip" wrap="square" lIns="27432" tIns="18288" rIns="0" bIns="18288" anchor="ctr" upright="1"/>
             <a:lstStyle/>
             <a:p>
               <a:pPr algn="l" rtl="0">
@@ -5530,7 +5530,7 @@
                   <a14:compatExt spid="_x0000_s734583"/>
                 </a:ext>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-000077350B00}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0100-000077350B00}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -5569,7 +5569,7 @@
             </a:extLst>
           </xdr:spPr>
           <xdr:txBody>
-            <a:bodyPr vertOverflow="clip" wrap="square" lIns="36576" tIns="22860" rIns="0" bIns="22860" anchor="ctr" upright="1"/>
+            <a:bodyPr vertOverflow="clip" wrap="square" lIns="27432" tIns="18288" rIns="0" bIns="18288" anchor="ctr" upright="1"/>
             <a:lstStyle/>
             <a:p>
               <a:pPr algn="l" rtl="0">
@@ -5607,7 +5607,7 @@
           <xdr:col>5</xdr:col>
           <xdr:colOff>152400</xdr:colOff>
           <xdr:row>8</xdr:row>
-          <xdr:rowOff>127000</xdr:rowOff>
+          <xdr:rowOff>123825</xdr:rowOff>
         </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
@@ -5617,7 +5617,7 @@
                   <a14:compatExt spid="_x0000_s734584"/>
                 </a:ext>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-000078350B00}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0100-000078350B00}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -5656,7 +5656,7 @@
             </a:extLst>
           </xdr:spPr>
           <xdr:txBody>
-            <a:bodyPr vertOverflow="clip" wrap="square" lIns="36576" tIns="22860" rIns="0" bIns="22860" anchor="ctr" upright="1"/>
+            <a:bodyPr vertOverflow="clip" wrap="square" lIns="27432" tIns="18288" rIns="0" bIns="18288" anchor="ctr" upright="1"/>
             <a:lstStyle/>
             <a:p>
               <a:pPr algn="l" rtl="0">
@@ -5704,7 +5704,7 @@
                   <a14:compatExt spid="_x0000_s734585"/>
                 </a:ext>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-000079350B00}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0100-000079350B00}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -5743,7 +5743,7 @@
             </a:extLst>
           </xdr:spPr>
           <xdr:txBody>
-            <a:bodyPr vertOverflow="clip" wrap="square" lIns="36576" tIns="22860" rIns="0" bIns="22860" anchor="ctr" upright="1"/>
+            <a:bodyPr vertOverflow="clip" wrap="square" lIns="27432" tIns="18288" rIns="0" bIns="18288" anchor="ctr" upright="1"/>
             <a:lstStyle/>
             <a:p>
               <a:pPr algn="l" rtl="0">
@@ -5791,7 +5791,7 @@
                   <a14:compatExt spid="_x0000_s734586"/>
                 </a:ext>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-00007A350B00}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0100-00007A350B00}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -5830,7 +5830,7 @@
             </a:extLst>
           </xdr:spPr>
           <xdr:txBody>
-            <a:bodyPr vertOverflow="clip" wrap="square" lIns="36576" tIns="22860" rIns="0" bIns="22860" anchor="ctr" upright="1"/>
+            <a:bodyPr vertOverflow="clip" wrap="square" lIns="27432" tIns="18288" rIns="0" bIns="18288" anchor="ctr" upright="1"/>
             <a:lstStyle/>
             <a:p>
               <a:pPr algn="l" rtl="0">
@@ -5878,7 +5878,7 @@
                   <a14:compatExt spid="_x0000_s734587"/>
                 </a:ext>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-00007B350B00}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0100-00007B350B00}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -5917,7 +5917,7 @@
             </a:extLst>
           </xdr:spPr>
           <xdr:txBody>
-            <a:bodyPr vertOverflow="clip" wrap="square" lIns="36576" tIns="22860" rIns="0" bIns="22860" anchor="ctr" upright="1"/>
+            <a:bodyPr vertOverflow="clip" wrap="square" lIns="27432" tIns="18288" rIns="0" bIns="18288" anchor="ctr" upright="1"/>
             <a:lstStyle/>
             <a:p>
               <a:pPr algn="l" rtl="0">
@@ -5953,7 +5953,7 @@
         </xdr:from>
         <xdr:to>
           <xdr:col>4</xdr:col>
-          <xdr:colOff>698500</xdr:colOff>
+          <xdr:colOff>695325</xdr:colOff>
           <xdr:row>12</xdr:row>
           <xdr:rowOff>571500</xdr:rowOff>
         </xdr:to>
@@ -5965,7 +5965,7 @@
                   <a14:compatExt spid="_x0000_s734588"/>
                 </a:ext>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-00007C350B00}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0100-00007C350B00}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -6004,7 +6004,7 @@
             </a:extLst>
           </xdr:spPr>
           <xdr:txBody>
-            <a:bodyPr vertOverflow="clip" wrap="square" lIns="36576" tIns="22860" rIns="0" bIns="22860" anchor="ctr" upright="1"/>
+            <a:bodyPr vertOverflow="clip" wrap="square" lIns="27432" tIns="18288" rIns="0" bIns="18288" anchor="ctr" upright="1"/>
             <a:lstStyle/>
             <a:p>
               <a:pPr algn="l" rtl="0">
@@ -6052,7 +6052,7 @@
                   <a14:compatExt spid="_x0000_s734589"/>
                 </a:ext>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-00007D350B00}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0100-00007D350B00}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -6091,7 +6091,7 @@
             </a:extLst>
           </xdr:spPr>
           <xdr:txBody>
-            <a:bodyPr vertOverflow="clip" wrap="square" lIns="36576" tIns="22860" rIns="0" bIns="22860" anchor="ctr" upright="1"/>
+            <a:bodyPr vertOverflow="clip" wrap="square" lIns="27432" tIns="18288" rIns="0" bIns="18288" anchor="ctr" upright="1"/>
             <a:lstStyle/>
             <a:p>
               <a:pPr algn="l" rtl="0">
@@ -6139,7 +6139,7 @@
                   <a14:compatExt spid="_x0000_s734590"/>
                 </a:ext>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-00007E350B00}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0100-00007E350B00}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -6178,7 +6178,7 @@
             </a:extLst>
           </xdr:spPr>
           <xdr:txBody>
-            <a:bodyPr vertOverflow="clip" wrap="square" lIns="36576" tIns="22860" rIns="0" bIns="22860" anchor="ctr" upright="1"/>
+            <a:bodyPr vertOverflow="clip" wrap="square" lIns="27432" tIns="18288" rIns="0" bIns="18288" anchor="ctr" upright="1"/>
             <a:lstStyle/>
             <a:p>
               <a:pPr algn="l" rtl="0">
@@ -6216,7 +6216,7 @@
           <xdr:col>5</xdr:col>
           <xdr:colOff>152400</xdr:colOff>
           <xdr:row>15</xdr:row>
-          <xdr:rowOff>336550</xdr:rowOff>
+          <xdr:rowOff>333375</xdr:rowOff>
         </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
@@ -6226,7 +6226,7 @@
                   <a14:compatExt spid="_x0000_s734591"/>
                 </a:ext>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-00007F350B00}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0100-00007F350B00}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -6265,7 +6265,7 @@
             </a:extLst>
           </xdr:spPr>
           <xdr:txBody>
-            <a:bodyPr vertOverflow="clip" wrap="square" lIns="36576" tIns="22860" rIns="0" bIns="22860" anchor="ctr" upright="1"/>
+            <a:bodyPr vertOverflow="clip" wrap="square" lIns="27432" tIns="18288" rIns="0" bIns="18288" anchor="ctr" upright="1"/>
             <a:lstStyle/>
             <a:p>
               <a:pPr algn="l" rtl="0">
@@ -6313,7 +6313,7 @@
                   <a14:compatExt spid="_x0000_s734593"/>
                 </a:ext>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-000081350B00}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0100-000081350B00}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -6352,7 +6352,7 @@
             </a:extLst>
           </xdr:spPr>
           <xdr:txBody>
-            <a:bodyPr vertOverflow="clip" wrap="square" lIns="36576" tIns="22860" rIns="0" bIns="22860" anchor="ctr" upright="1"/>
+            <a:bodyPr vertOverflow="clip" wrap="square" lIns="27432" tIns="18288" rIns="0" bIns="18288" anchor="ctr" upright="1"/>
             <a:lstStyle/>
             <a:p>
               <a:pPr algn="l" rtl="0">
@@ -6390,7 +6390,7 @@
           <xdr:col>5</xdr:col>
           <xdr:colOff>152400</xdr:colOff>
           <xdr:row>17</xdr:row>
-          <xdr:rowOff>127000</xdr:rowOff>
+          <xdr:rowOff>123825</xdr:rowOff>
         </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
@@ -6400,7 +6400,7 @@
                   <a14:compatExt spid="_x0000_s734596"/>
                 </a:ext>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-000084350B00}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0100-000084350B00}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -6439,7 +6439,7 @@
             </a:extLst>
           </xdr:spPr>
           <xdr:txBody>
-            <a:bodyPr vertOverflow="clip" wrap="square" lIns="36576" tIns="22860" rIns="0" bIns="22860" anchor="ctr" upright="1"/>
+            <a:bodyPr vertOverflow="clip" wrap="square" lIns="27432" tIns="18288" rIns="0" bIns="18288" anchor="ctr" upright="1"/>
             <a:lstStyle/>
             <a:p>
               <a:pPr algn="l" rtl="0">
@@ -6487,7 +6487,7 @@
                   <a14:compatExt spid="_x0000_s734605"/>
                 </a:ext>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-00008D350B00}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0100-00008D350B00}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -6526,7 +6526,7 @@
             </a:extLst>
           </xdr:spPr>
           <xdr:txBody>
-            <a:bodyPr vertOverflow="clip" wrap="square" lIns="36576" tIns="22860" rIns="0" bIns="22860" anchor="ctr" upright="1"/>
+            <a:bodyPr vertOverflow="clip" wrap="square" lIns="27432" tIns="18288" rIns="0" bIns="18288" anchor="ctr" upright="1"/>
             <a:lstStyle/>
             <a:p>
               <a:pPr algn="l" rtl="0">
@@ -6574,7 +6574,7 @@
                   <a14:compatExt spid="_x0000_s734606"/>
                 </a:ext>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-00008E350B00}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0100-00008E350B00}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -6613,7 +6613,7 @@
             </a:extLst>
           </xdr:spPr>
           <xdr:txBody>
-            <a:bodyPr vertOverflow="clip" wrap="square" lIns="36576" tIns="22860" rIns="0" bIns="22860" anchor="ctr" upright="1"/>
+            <a:bodyPr vertOverflow="clip" wrap="square" lIns="27432" tIns="18288" rIns="0" bIns="18288" anchor="ctr" upright="1"/>
             <a:lstStyle/>
             <a:p>
               <a:pPr algn="l" rtl="0">
@@ -6661,7 +6661,7 @@
                   <a14:compatExt spid="_x0000_s734607"/>
                 </a:ext>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-00008F350B00}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0100-00008F350B00}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -6700,7 +6700,7 @@
             </a:extLst>
           </xdr:spPr>
           <xdr:txBody>
-            <a:bodyPr vertOverflow="clip" wrap="square" lIns="36576" tIns="22860" rIns="0" bIns="22860" anchor="ctr" upright="1"/>
+            <a:bodyPr vertOverflow="clip" wrap="square" lIns="27432" tIns="18288" rIns="0" bIns="18288" anchor="ctr" upright="1"/>
             <a:lstStyle/>
             <a:p>
               <a:pPr algn="l" rtl="0">
@@ -6748,7 +6748,7 @@
                   <a14:compatExt spid="_x0000_s734608"/>
                 </a:ext>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-000090350B00}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0100-000090350B00}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -6787,7 +6787,7 @@
             </a:extLst>
           </xdr:spPr>
           <xdr:txBody>
-            <a:bodyPr vertOverflow="clip" wrap="square" lIns="36576" tIns="22860" rIns="0" bIns="22860" anchor="ctr" upright="1"/>
+            <a:bodyPr vertOverflow="clip" wrap="square" lIns="27432" tIns="18288" rIns="0" bIns="18288" anchor="ctr" upright="1"/>
             <a:lstStyle/>
             <a:p>
               <a:pPr algn="l" rtl="0">
@@ -6835,7 +6835,7 @@
                   <a14:compatExt spid="_x0000_s734609"/>
                 </a:ext>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-000091350B00}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0100-000091350B00}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -6874,7 +6874,7 @@
             </a:extLst>
           </xdr:spPr>
           <xdr:txBody>
-            <a:bodyPr vertOverflow="clip" wrap="square" lIns="36576" tIns="22860" rIns="0" bIns="22860" anchor="ctr" upright="1"/>
+            <a:bodyPr vertOverflow="clip" wrap="square" lIns="27432" tIns="18288" rIns="0" bIns="18288" anchor="ctr" upright="1"/>
             <a:lstStyle/>
             <a:p>
               <a:pPr algn="l" rtl="0">
@@ -6922,7 +6922,7 @@
                   <a14:compatExt spid="_x0000_s734610"/>
                 </a:ext>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-000092350B00}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0100-000092350B00}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -6961,7 +6961,7 @@
             </a:extLst>
           </xdr:spPr>
           <xdr:txBody>
-            <a:bodyPr vertOverflow="clip" wrap="square" lIns="36576" tIns="22860" rIns="0" bIns="22860" anchor="ctr" upright="1"/>
+            <a:bodyPr vertOverflow="clip" wrap="square" lIns="27432" tIns="18288" rIns="0" bIns="18288" anchor="ctr" upright="1"/>
             <a:lstStyle/>
             <a:p>
               <a:pPr algn="l" rtl="0">
@@ -6999,7 +6999,7 @@
           <xdr:col>5</xdr:col>
           <xdr:colOff>152400</xdr:colOff>
           <xdr:row>24</xdr:row>
-          <xdr:rowOff>127000</xdr:rowOff>
+          <xdr:rowOff>123825</xdr:rowOff>
         </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
@@ -7009,7 +7009,7 @@
                   <a14:compatExt spid="_x0000_s734611"/>
                 </a:ext>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-000093350B00}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0100-000093350B00}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -7048,7 +7048,7 @@
             </a:extLst>
           </xdr:spPr>
           <xdr:txBody>
-            <a:bodyPr vertOverflow="clip" wrap="square" lIns="36576" tIns="22860" rIns="0" bIns="22860" anchor="ctr" upright="1"/>
+            <a:bodyPr vertOverflow="clip" wrap="square" lIns="27432" tIns="18288" rIns="0" bIns="18288" anchor="ctr" upright="1"/>
             <a:lstStyle/>
             <a:p>
               <a:pPr algn="l" rtl="0">
@@ -7096,7 +7096,7 @@
                   <a14:compatExt spid="_x0000_s734614"/>
                 </a:ext>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-000096350B00}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0100-000096350B00}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -7135,7 +7135,7 @@
             </a:extLst>
           </xdr:spPr>
           <xdr:txBody>
-            <a:bodyPr vertOverflow="clip" wrap="square" lIns="36576" tIns="22860" rIns="0" bIns="22860" anchor="ctr" upright="1"/>
+            <a:bodyPr vertOverflow="clip" wrap="square" lIns="27432" tIns="18288" rIns="0" bIns="18288" anchor="ctr" upright="1"/>
             <a:lstStyle/>
             <a:p>
               <a:pPr algn="l" rtl="0">
@@ -7183,7 +7183,7 @@
                   <a14:compatExt spid="_x0000_s734618"/>
                 </a:ext>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-00009A350B00}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0100-00009A350B00}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -7222,7 +7222,7 @@
             </a:extLst>
           </xdr:spPr>
           <xdr:txBody>
-            <a:bodyPr vertOverflow="clip" wrap="square" lIns="36576" tIns="22860" rIns="0" bIns="22860" anchor="ctr" upright="1"/>
+            <a:bodyPr vertOverflow="clip" wrap="square" lIns="27432" tIns="18288" rIns="0" bIns="18288" anchor="ctr" upright="1"/>
             <a:lstStyle/>
             <a:p>
               <a:pPr algn="l" rtl="0">
@@ -7270,7 +7270,7 @@
                   <a14:compatExt spid="_x0000_s734619"/>
                 </a:ext>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-00009B350B00}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0100-00009B350B00}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -7309,7 +7309,7 @@
             </a:extLst>
           </xdr:spPr>
           <xdr:txBody>
-            <a:bodyPr vertOverflow="clip" wrap="square" lIns="36576" tIns="22860" rIns="0" bIns="22860" anchor="ctr" upright="1"/>
+            <a:bodyPr vertOverflow="clip" wrap="square" lIns="27432" tIns="18288" rIns="0" bIns="18288" anchor="ctr" upright="1"/>
             <a:lstStyle/>
             <a:p>
               <a:pPr algn="l" rtl="0">
@@ -7357,7 +7357,7 @@
                   <a14:compatExt spid="_x0000_s734620"/>
                 </a:ext>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-00009C350B00}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0100-00009C350B00}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -7396,7 +7396,7 @@
             </a:extLst>
           </xdr:spPr>
           <xdr:txBody>
-            <a:bodyPr vertOverflow="clip" wrap="square" lIns="36576" tIns="22860" rIns="0" bIns="22860" anchor="ctr" upright="1"/>
+            <a:bodyPr vertOverflow="clip" wrap="square" lIns="27432" tIns="18288" rIns="0" bIns="18288" anchor="ctr" upright="1"/>
             <a:lstStyle/>
             <a:p>
               <a:pPr algn="l" rtl="0">
@@ -7444,7 +7444,7 @@
                   <a14:compatExt spid="_x0000_s734622"/>
                 </a:ext>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-00009E350B00}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0100-00009E350B00}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -7483,7 +7483,7 @@
             </a:extLst>
           </xdr:spPr>
           <xdr:txBody>
-            <a:bodyPr vertOverflow="clip" wrap="square" lIns="36576" tIns="22860" rIns="0" bIns="22860" anchor="ctr" upright="1"/>
+            <a:bodyPr vertOverflow="clip" wrap="square" lIns="27432" tIns="18288" rIns="0" bIns="18288" anchor="ctr" upright="1"/>
             <a:lstStyle/>
             <a:p>
               <a:pPr algn="l" rtl="0">
@@ -7531,7 +7531,7 @@
                   <a14:compatExt spid="_x0000_s734623"/>
                 </a:ext>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-00009F350B00}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0100-00009F350B00}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -7570,7 +7570,7 @@
             </a:extLst>
           </xdr:spPr>
           <xdr:txBody>
-            <a:bodyPr vertOverflow="clip" wrap="square" lIns="36576" tIns="22860" rIns="0" bIns="22860" anchor="ctr" upright="1"/>
+            <a:bodyPr vertOverflow="clip" wrap="square" lIns="27432" tIns="18288" rIns="0" bIns="18288" anchor="ctr" upright="1"/>
             <a:lstStyle/>
             <a:p>
               <a:pPr algn="l" rtl="0">
@@ -7618,7 +7618,7 @@
                   <a14:compatExt spid="_x0000_s734624"/>
                 </a:ext>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-0000A0350B00}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0100-0000A0350B00}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -7657,7 +7657,7 @@
             </a:extLst>
           </xdr:spPr>
           <xdr:txBody>
-            <a:bodyPr vertOverflow="clip" wrap="square" lIns="36576" tIns="22860" rIns="0" bIns="22860" anchor="ctr" upright="1"/>
+            <a:bodyPr vertOverflow="clip" wrap="square" lIns="27432" tIns="18288" rIns="0" bIns="18288" anchor="ctr" upright="1"/>
             <a:lstStyle/>
             <a:p>
               <a:pPr algn="l" rtl="0">
@@ -7705,7 +7705,7 @@
                   <a14:compatExt spid="_x0000_s734625"/>
                 </a:ext>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-0000A1350B00}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0100-0000A1350B00}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -7744,7 +7744,7 @@
             </a:extLst>
           </xdr:spPr>
           <xdr:txBody>
-            <a:bodyPr vertOverflow="clip" wrap="square" lIns="36576" tIns="22860" rIns="0" bIns="22860" anchor="ctr" upright="1"/>
+            <a:bodyPr vertOverflow="clip" wrap="square" lIns="27432" tIns="18288" rIns="0" bIns="18288" anchor="ctr" upright="1"/>
             <a:lstStyle/>
             <a:p>
               <a:pPr algn="l" rtl="0">
@@ -7782,7 +7782,7 @@
           <xdr:col>5</xdr:col>
           <xdr:colOff>152400</xdr:colOff>
           <xdr:row>34</xdr:row>
-          <xdr:rowOff>31750</xdr:rowOff>
+          <xdr:rowOff>28575</xdr:rowOff>
         </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
@@ -7792,7 +7792,7 @@
                   <a14:compatExt spid="_x0000_s734630"/>
                 </a:ext>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-0000A6350B00}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0100-0000A6350B00}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -7831,7 +7831,7 @@
             </a:extLst>
           </xdr:spPr>
           <xdr:txBody>
-            <a:bodyPr vertOverflow="clip" wrap="square" lIns="36576" tIns="22860" rIns="0" bIns="22860" anchor="ctr" upright="1"/>
+            <a:bodyPr vertOverflow="clip" wrap="square" lIns="27432" tIns="18288" rIns="0" bIns="18288" anchor="ctr" upright="1"/>
             <a:lstStyle/>
             <a:p>
               <a:pPr algn="l" rtl="0">
@@ -7869,7 +7869,7 @@
           <xdr:col>5</xdr:col>
           <xdr:colOff>152400</xdr:colOff>
           <xdr:row>35</xdr:row>
-          <xdr:rowOff>12700</xdr:rowOff>
+          <xdr:rowOff>9525</xdr:rowOff>
         </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
@@ -7879,7 +7879,7 @@
                   <a14:compatExt spid="_x0000_s734631"/>
                 </a:ext>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-0000A7350B00}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0100-0000A7350B00}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -7918,7 +7918,7 @@
             </a:extLst>
           </xdr:spPr>
           <xdr:txBody>
-            <a:bodyPr vertOverflow="clip" wrap="square" lIns="36576" tIns="22860" rIns="0" bIns="22860" anchor="ctr" upright="1"/>
+            <a:bodyPr vertOverflow="clip" wrap="square" lIns="27432" tIns="18288" rIns="0" bIns="18288" anchor="ctr" upright="1"/>
             <a:lstStyle/>
             <a:p>
               <a:pPr algn="l" rtl="0">
@@ -7966,7 +7966,7 @@
                   <a14:compatExt spid="_x0000_s734632"/>
                 </a:ext>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-0000A8350B00}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0100-0000A8350B00}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -8005,7 +8005,7 @@
             </a:extLst>
           </xdr:spPr>
           <xdr:txBody>
-            <a:bodyPr vertOverflow="clip" wrap="square" lIns="36576" tIns="22860" rIns="0" bIns="22860" anchor="ctr" upright="1"/>
+            <a:bodyPr vertOverflow="clip" wrap="square" lIns="27432" tIns="18288" rIns="0" bIns="18288" anchor="ctr" upright="1"/>
             <a:lstStyle/>
             <a:p>
               <a:pPr algn="l" rtl="0">
@@ -8053,7 +8053,7 @@
                   <a14:compatExt spid="_x0000_s734633"/>
                 </a:ext>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-0000A9350B00}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0100-0000A9350B00}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -8092,7 +8092,7 @@
             </a:extLst>
           </xdr:spPr>
           <xdr:txBody>
-            <a:bodyPr vertOverflow="clip" wrap="square" lIns="36576" tIns="22860" rIns="0" bIns="22860" anchor="ctr" upright="1"/>
+            <a:bodyPr vertOverflow="clip" wrap="square" lIns="27432" tIns="18288" rIns="0" bIns="18288" anchor="ctr" upright="1"/>
             <a:lstStyle/>
             <a:p>
               <a:pPr algn="l" rtl="0">
@@ -8124,13 +8124,13 @@
           <xdr:col>4</xdr:col>
           <xdr:colOff>19050</xdr:colOff>
           <xdr:row>37</xdr:row>
-          <xdr:rowOff>88900</xdr:rowOff>
+          <xdr:rowOff>85725</xdr:rowOff>
         </xdr:from>
         <xdr:to>
           <xdr:col>5</xdr:col>
           <xdr:colOff>171450</xdr:colOff>
           <xdr:row>37</xdr:row>
-          <xdr:rowOff>298450</xdr:rowOff>
+          <xdr:rowOff>295275</xdr:rowOff>
         </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
@@ -8140,7 +8140,7 @@
                   <a14:compatExt spid="_x0000_s734637"/>
                 </a:ext>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-0000AD350B00}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0100-0000AD350B00}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -8179,7 +8179,7 @@
             </a:extLst>
           </xdr:spPr>
           <xdr:txBody>
-            <a:bodyPr vertOverflow="clip" wrap="square" lIns="36576" tIns="22860" rIns="0" bIns="22860" anchor="ctr" upright="1"/>
+            <a:bodyPr vertOverflow="clip" wrap="square" lIns="27432" tIns="18288" rIns="0" bIns="18288" anchor="ctr" upright="1"/>
             <a:lstStyle/>
             <a:p>
               <a:pPr algn="l" rtl="0">
@@ -8227,7 +8227,7 @@
                   <a14:compatExt spid="_x0000_s734638"/>
                 </a:ext>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-0000AE350B00}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0100-0000AE350B00}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -8266,7 +8266,7 @@
             </a:extLst>
           </xdr:spPr>
           <xdr:txBody>
-            <a:bodyPr vertOverflow="clip" wrap="square" lIns="36576" tIns="22860" rIns="0" bIns="22860" anchor="ctr" upright="1"/>
+            <a:bodyPr vertOverflow="clip" wrap="square" lIns="27432" tIns="18288" rIns="0" bIns="18288" anchor="ctr" upright="1"/>
             <a:lstStyle/>
             <a:p>
               <a:pPr algn="l" rtl="0">
@@ -8588,68 +8588,68 @@
       <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="4.26953125" customWidth="1"/>
-    <col min="2" max="2" width="26.81640625" customWidth="1"/>
-    <col min="3" max="3" width="39.81640625" customWidth="1"/>
-    <col min="4" max="4" width="14.81640625" customWidth="1"/>
-    <col min="5" max="5" width="4.1796875" customWidth="1"/>
-    <col min="6" max="6" width="40.7265625" customWidth="1"/>
-    <col min="8" max="8" width="6.1796875" customWidth="1"/>
-    <col min="9" max="9" width="2.453125" customWidth="1"/>
-    <col min="10" max="10" width="2.7265625" customWidth="1"/>
-    <col min="13" max="13" width="15.26953125" customWidth="1"/>
+    <col min="1" max="1" width="4.28515625" customWidth="1"/>
+    <col min="2" max="2" width="26.85546875" customWidth="1"/>
+    <col min="3" max="3" width="39.85546875" customWidth="1"/>
+    <col min="4" max="4" width="14.85546875" customWidth="1"/>
+    <col min="5" max="5" width="4.140625" customWidth="1"/>
+    <col min="6" max="6" width="40.7109375" customWidth="1"/>
+    <col min="8" max="8" width="6.140625" customWidth="1"/>
+    <col min="9" max="9" width="2.42578125" customWidth="1"/>
+    <col min="10" max="10" width="2.7109375" customWidth="1"/>
+    <col min="13" max="13" width="15.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="32.25" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:10" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="31"/>
-      <c r="B1" s="81" t="s">
+      <c r="B1" s="83" t="s">
         <v>45</v>
       </c>
-      <c r="C1" s="82"/>
-      <c r="D1" s="82"/>
-      <c r="E1" s="82"/>
-      <c r="F1" s="82"/>
-      <c r="G1" s="82"/>
-      <c r="H1" s="82"/>
+      <c r="C1" s="84"/>
+      <c r="D1" s="84"/>
+      <c r="E1" s="84"/>
+      <c r="F1" s="84"/>
+      <c r="G1" s="84"/>
+      <c r="H1" s="84"/>
       <c r="I1" s="31"/>
       <c r="J1" s="31"/>
     </row>
-    <row r="2" spans="1:10" ht="23.5" x14ac:dyDescent="0.55000000000000004">
+    <row r="2" spans="1:10" ht="23.25" x14ac:dyDescent="0.35">
       <c r="A2" s="31"/>
       <c r="B2" s="34" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="86"/>
-      <c r="D2" s="87"/>
-      <c r="E2" s="87"/>
-      <c r="F2" s="87"/>
-      <c r="G2" s="87"/>
-      <c r="H2" s="87"/>
+      <c r="C2" s="88"/>
+      <c r="D2" s="89"/>
+      <c r="E2" s="89"/>
+      <c r="F2" s="89"/>
+      <c r="G2" s="89"/>
+      <c r="H2" s="89"/>
       <c r="I2" s="31"/>
       <c r="J2" s="31"/>
     </row>
-    <row r="3" spans="1:10" ht="23.5" x14ac:dyDescent="0.55000000000000004">
+    <row r="3" spans="1:10" ht="23.25" x14ac:dyDescent="0.35">
       <c r="A3" s="31"/>
       <c r="B3" s="34" t="s">
         <v>1</v>
       </c>
-      <c r="C3" s="88"/>
-      <c r="D3" s="87"/>
-      <c r="E3" s="87"/>
-      <c r="F3" s="87"/>
-      <c r="G3" s="87"/>
-      <c r="H3" s="87"/>
+      <c r="C3" s="90"/>
+      <c r="D3" s="89"/>
+      <c r="E3" s="89"/>
+      <c r="F3" s="89"/>
+      <c r="G3" s="89"/>
+      <c r="H3" s="89"/>
       <c r="I3" s="31"/>
       <c r="J3" s="31"/>
     </row>
-    <row r="4" spans="1:10" ht="22.5" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:10" ht="23.25" x14ac:dyDescent="0.35">
       <c r="A4" s="31"/>
       <c r="B4" s="34" t="s">
         <v>3</v>
       </c>
-      <c r="C4" s="86"/>
+      <c r="C4" s="88"/>
       <c r="D4" s="92"/>
       <c r="E4" s="92"/>
       <c r="F4" s="92"/>
@@ -8658,7 +8658,7 @@
       <c r="I4" s="31"/>
       <c r="J4" s="31"/>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A5" s="31"/>
       <c r="B5" s="31"/>
       <c r="C5" s="31"/>
@@ -8670,7 +8670,7 @@
       <c r="I5" s="31"/>
       <c r="J5" s="31"/>
     </row>
-    <row r="6" spans="1:10" ht="49.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:10" ht="49.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="31"/>
       <c r="B6" s="91" t="s">
         <v>2</v>
@@ -8684,7 +8684,7 @@
       <c r="I6" s="31"/>
       <c r="J6" s="31"/>
     </row>
-    <row r="7" spans="1:10" ht="37.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:10" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="31"/>
       <c r="B7" s="94" t="str">
         <f>CONCATENATE("Az irányelvek között vannak kiemelt (sárga háttérszínnel és félkövér kiemeléssel jelölt) elvek , amelyek betartására kiemelten figyelni kell! Az elégséges szinthez legalább ",D11," pontot el kell érni. A tanulói és tanári értékelés tekintetében, maximum 10 darab irányelvben lehet eltérés.")</f>
@@ -8699,7 +8699,7 @@
       <c r="I7" s="31"/>
       <c r="J7" s="31"/>
     </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A8" s="31"/>
       <c r="B8" s="31"/>
       <c r="C8" s="31"/>
@@ -8711,7 +8711,7 @@
       <c r="I8" s="31"/>
       <c r="J8" s="31"/>
     </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A9" s="31"/>
       <c r="B9" s="32" t="s">
         <v>33</v>
@@ -8725,12 +8725,12 @@
       <c r="I9" s="31"/>
       <c r="J9" s="31"/>
     </row>
-    <row r="10" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="31"/>
-      <c r="B10" s="89" t="s">
+      <c r="B10" s="81" t="s">
         <v>30</v>
       </c>
-      <c r="C10" s="90"/>
+      <c r="C10" s="82"/>
       <c r="D10" s="78">
         <f>SUM(Irányelvek!G:G)</f>
         <v>80</v>
@@ -8744,12 +8744,12 @@
       <c r="I10" s="31"/>
       <c r="J10" s="31"/>
     </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A11" s="31"/>
-      <c r="B11" s="83" t="s">
+      <c r="B11" s="85" t="s">
         <v>36</v>
       </c>
-      <c r="C11" s="84"/>
+      <c r="C11" s="86"/>
       <c r="D11" s="79">
         <v>20</v>
       </c>
@@ -8760,12 +8760,12 @@
       <c r="I11" s="31"/>
       <c r="J11" s="31"/>
     </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A12" s="31"/>
-      <c r="B12" s="89" t="s">
+      <c r="B12" s="81" t="s">
         <v>58</v>
       </c>
-      <c r="C12" s="90"/>
+      <c r="C12" s="82"/>
       <c r="D12" s="78">
         <v>20</v>
       </c>
@@ -8776,12 +8776,12 @@
       <c r="I12" s="31"/>
       <c r="J12" s="31"/>
     </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A13" s="31"/>
-      <c r="B13" s="89" t="s">
+      <c r="B13" s="81" t="s">
         <v>59</v>
       </c>
-      <c r="C13" s="90"/>
+      <c r="C13" s="82"/>
       <c r="D13" s="78">
         <v>40</v>
       </c>
@@ -8792,7 +8792,7 @@
       <c r="I13" s="31"/>
       <c r="J13" s="31"/>
     </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A14" s="31"/>
       <c r="B14" s="31"/>
       <c r="C14" s="31"/>
@@ -8804,7 +8804,7 @@
       <c r="I14" s="31"/>
       <c r="J14" s="31"/>
     </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A15" s="31"/>
       <c r="B15" s="32" t="s">
         <v>57</v>
@@ -8818,12 +8818,12 @@
       <c r="I15" s="31"/>
       <c r="J15" s="31"/>
     </row>
-    <row r="16" spans="1:10" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:10" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="31"/>
-      <c r="B16" s="89" t="s">
+      <c r="B16" s="81" t="s">
         <v>39</v>
       </c>
-      <c r="C16" s="90"/>
+      <c r="C16" s="82"/>
       <c r="D16" s="30" t="b">
         <f t="array" ref="D16">IF(COUNTIFS(Irányelvek!D2:D39,"=hamis",Irányelvek!F2:F39,"=Igaz")=0,TRUE,FALSE)</f>
         <v>0</v>
@@ -8835,15 +8835,15 @@
       <c r="I16" s="31"/>
       <c r="J16" s="31"/>
     </row>
-    <row r="17" spans="1:10" ht="31.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:10" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="31"/>
-      <c r="B17" s="89" t="s">
+      <c r="B17" s="81" t="s">
         <v>32</v>
       </c>
-      <c r="C17" s="90"/>
+      <c r="C17" s="82"/>
       <c r="D17" s="33">
         <f>SUM(Irányelvek!H2:H39)</f>
-        <v>22</v>
+        <v>28</v>
       </c>
       <c r="E17" s="31"/>
       <c r="F17" s="97" t="str">
@@ -8855,7 +8855,7 @@
       <c r="I17" s="31"/>
       <c r="J17" s="31"/>
     </row>
-    <row r="18" spans="1:10" ht="31.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:10" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="31"/>
       <c r="B18" s="95" t="s">
         <v>60</v>
@@ -8863,7 +8863,7 @@
       <c r="C18" s="96"/>
       <c r="D18" s="36">
         <f>IF(D17&gt;D11,VLOOKUP(SUM(Irányelvek!J2:J39),Ponthatárok!G2:H12,2,TRUE),0)</f>
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="E18" s="31"/>
       <c r="F18" s="97"/>
@@ -8872,12 +8872,12 @@
       <c r="I18" s="31"/>
       <c r="J18" s="31"/>
     </row>
-    <row r="19" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A19" s="31"/>
-      <c r="B19" s="89" t="s">
+      <c r="B19" s="81" t="s">
         <v>61</v>
       </c>
-      <c r="C19" s="90"/>
+      <c r="C19" s="82"/>
       <c r="D19" s="80">
         <v>40</v>
       </c>
@@ -8888,27 +8888,27 @@
       <c r="I19" s="31"/>
       <c r="J19" s="31"/>
     </row>
-    <row r="20" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A20" s="31"/>
-      <c r="B20" s="89" t="s">
+      <c r="B20" s="81" t="s">
         <v>62</v>
       </c>
-      <c r="C20" s="90"/>
+      <c r="C20" s="82"/>
       <c r="D20" s="33">
         <f>SUM(D17:D19)</f>
-        <v>66</v>
+        <v>74</v>
       </c>
       <c r="E20" s="31"/>
-      <c r="F20" s="85" t="str">
+      <c r="F20" s="87" t="str">
         <f>CONCATENATE("Az önértékelés alapján ",VLOOKUP(D20,Ponthatárok!$C$3:$D$7,2,TRUE), "  érdemjegyet kapnál rá.")</f>
         <v>Az önértékelés alapján Elégséges (2)  érdemjegyet kapnál rá.</v>
       </c>
-      <c r="G20" s="85"/>
-      <c r="H20" s="85"/>
+      <c r="G20" s="87"/>
+      <c r="H20" s="87"/>
       <c r="I20" s="31"/>
       <c r="J20" s="31"/>
     </row>
-    <row r="21" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A21" s="31"/>
       <c r="B21" s="35"/>
       <c r="C21" s="35"/>
@@ -8923,6 +8923,8 @@
   </sheetData>
   <sheetProtection algorithmName="SHA-512" hashValue="Pt2r10NfCQvSDRx8qMjGYxYpEYBoOyIK56jWLg5u88pMtB0yZv+L45h/PZkvP5rgD0XQukcG0FY9SUv/PUWVng==" saltValue="OS0FMTO/1nXUT8EsxtE52w==" spinCount="100000" sheet="1" objects="1" scenarios="1"/>
   <mergeCells count="18">
+    <mergeCell ref="F17:H19"/>
+    <mergeCell ref="F10:H14"/>
     <mergeCell ref="B10:C10"/>
     <mergeCell ref="B16:C16"/>
     <mergeCell ref="B1:H1"/>
@@ -8939,8 +8941,6 @@
     <mergeCell ref="B12:C12"/>
     <mergeCell ref="B13:C13"/>
     <mergeCell ref="B18:C18"/>
-    <mergeCell ref="F17:H19"/>
-    <mergeCell ref="F10:H14"/>
   </mergeCells>
   <conditionalFormatting sqref="D17:D20">
     <cfRule type="expression" dxfId="2" priority="1" stopIfTrue="1">
@@ -8961,27 +8961,27 @@
   <sheetPr codeName="Munka2"/>
   <dimension ref="A1:L39"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A32" activePane="bottomLeft" state="frozen"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="C36" sqref="C36"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="3.1796875" customWidth="1"/>
-    <col min="2" max="2" width="15.81640625" style="28" customWidth="1"/>
-    <col min="3" max="3" width="54.1796875" style="29" customWidth="1"/>
-    <col min="4" max="4" width="10.54296875" style="22" customWidth="1"/>
-    <col min="5" max="5" width="10.54296875" style="23" customWidth="1"/>
-    <col min="6" max="6" width="9.81640625" customWidth="1"/>
+    <col min="1" max="1" width="3.140625" customWidth="1"/>
+    <col min="2" max="2" width="15.85546875" style="28" customWidth="1"/>
+    <col min="3" max="3" width="54.140625" style="29" customWidth="1"/>
+    <col min="4" max="4" width="10.5703125" style="22" customWidth="1"/>
+    <col min="5" max="5" width="10.5703125" style="23" customWidth="1"/>
+    <col min="6" max="6" width="9.85546875" customWidth="1"/>
     <col min="8" max="8" width="13" customWidth="1"/>
     <col min="9" max="9" width="16" customWidth="1"/>
-    <col min="10" max="10" width="10.81640625" customWidth="1"/>
-    <col min="11" max="11" width="11.7265625" customWidth="1"/>
-    <col min="12" max="12" width="9.7265625" customWidth="1"/>
+    <col min="10" max="10" width="10.85546875" customWidth="1"/>
+    <col min="11" max="11" width="11.7109375" customWidth="1"/>
+    <col min="12" max="12" width="9.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" s="3" customFormat="1" ht="39.5" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:12" s="3" customFormat="1" ht="39" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A1" s="71"/>
       <c r="B1" s="64" t="s">
         <v>5</v>
@@ -9012,7 +9012,7 @@
       </c>
       <c r="L1" s="4"/>
     </row>
-    <row r="2" spans="1:12" s="1" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:12" s="1" customFormat="1" ht="24.75" x14ac:dyDescent="0.25">
       <c r="A2" s="72">
         <v>1</v>
       </c>
@@ -9047,7 +9047,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:12" s="1" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:12" s="1" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A3" s="73">
         <v>2</v>
       </c>
@@ -9080,7 +9080,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:12" s="1" customFormat="1" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:12" s="1" customFormat="1" ht="45" x14ac:dyDescent="0.25">
       <c r="A4" s="73">
         <v>3</v>
       </c>
@@ -9116,7 +9116,7 @@
       </c>
       <c r="L4" s="6"/>
     </row>
-    <row r="5" spans="1:12" s="1" customFormat="1" ht="58" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:12" s="1" customFormat="1" ht="60" x14ac:dyDescent="0.25">
       <c r="A5" s="73">
         <v>4</v>
       </c>
@@ -9152,7 +9152,7 @@
       </c>
       <c r="L5" s="7"/>
     </row>
-    <row r="6" spans="1:12" s="1" customFormat="1" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:12" s="1" customFormat="1" ht="45" x14ac:dyDescent="0.25">
       <c r="A6" s="73">
         <v>6</v>
       </c>
@@ -9187,7 +9187,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:12" s="1" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="7" spans="1:12" s="1" customFormat="1" ht="25.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A7" s="74">
         <v>7</v>
       </c>
@@ -9198,7 +9198,7 @@
         <v>70</v>
       </c>
       <c r="D7" s="44" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E7" s="45" t="b">
         <v>1</v>
@@ -9211,7 +9211,7 @@
       </c>
       <c r="H7" s="47">
         <f t="shared" si="0"/>
-        <v>-2</v>
+        <v>2</v>
       </c>
       <c r="I7" s="48">
         <f t="shared" si="1"/>
@@ -9219,10 +9219,10 @@
       </c>
       <c r="J7" s="49">
         <f t="shared" si="2"/>
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:12" s="1" customFormat="1" ht="29" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:12" s="1" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A8" s="75">
         <v>8</v>
       </c>
@@ -9233,7 +9233,7 @@
         <v>26</v>
       </c>
       <c r="D8" s="56" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E8" s="57" t="b">
         <v>1</v>
@@ -9242,9 +9242,9 @@
       <c r="G8" s="39">
         <v>1</v>
       </c>
-      <c r="H8" s="39" t="str">
+      <c r="H8" s="39">
         <f t="shared" si="0"/>
-        <v/>
+        <v>1</v>
       </c>
       <c r="I8" s="40">
         <f t="shared" si="1"/>
@@ -9252,10 +9252,10 @@
       </c>
       <c r="J8" s="41">
         <f t="shared" si="2"/>
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:12" ht="29" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:12" ht="30" x14ac:dyDescent="0.25">
       <c r="A9" s="73">
         <v>9</v>
       </c>
@@ -9288,7 +9288,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:12" ht="29" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:12" ht="30" x14ac:dyDescent="0.25">
       <c r="A10" s="73">
         <v>10</v>
       </c>
@@ -9323,7 +9323,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:12" ht="29" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:12" ht="30" x14ac:dyDescent="0.25">
       <c r="A11" s="73">
         <v>11</v>
       </c>
@@ -9358,7 +9358,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:12" ht="29" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:12" ht="30" x14ac:dyDescent="0.25">
       <c r="A12" s="73">
         <v>12</v>
       </c>
@@ -9391,7 +9391,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:12" ht="29.5" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="13" spans="1:12" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A13" s="73">
         <v>13</v>
       </c>
@@ -9426,7 +9426,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:12" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:12" ht="60" x14ac:dyDescent="0.25">
       <c r="A14" s="73">
         <v>14</v>
       </c>
@@ -9461,7 +9461,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:12" ht="29" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:12" ht="30" x14ac:dyDescent="0.25">
       <c r="A15" s="73">
         <v>15</v>
       </c>
@@ -9496,7 +9496,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="16" spans="1:12" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:12" ht="45" x14ac:dyDescent="0.25">
       <c r="A16" s="73">
         <v>16</v>
       </c>
@@ -9531,7 +9531,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:10" ht="30" x14ac:dyDescent="0.25">
       <c r="A17" s="73">
         <v>17</v>
       </c>
@@ -9566,7 +9566,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="18" spans="1:10" ht="19.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="18" spans="1:10" ht="19.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A18" s="73">
         <v>19</v>
       </c>
@@ -9601,7 +9601,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="1:10" ht="19.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:10" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="73">
         <v>21</v>
       </c>
@@ -9634,7 +9634,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="1:10" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:10" ht="45" x14ac:dyDescent="0.25">
       <c r="A20" s="73">
         <v>22</v>
       </c>
@@ -9667,7 +9667,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="21" spans="1:10" ht="29" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:10" ht="30" x14ac:dyDescent="0.25">
       <c r="A21" s="73">
         <v>23</v>
       </c>
@@ -9700,7 +9700,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="22" spans="1:10" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:10" ht="45" x14ac:dyDescent="0.25">
       <c r="A22" s="73">
         <v>24</v>
       </c>
@@ -9733,7 +9733,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="1:10" ht="29" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:10" ht="30" x14ac:dyDescent="0.25">
       <c r="A23" s="73">
         <v>25</v>
       </c>
@@ -9766,7 +9766,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="24" spans="1:10" ht="29" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:10" ht="30" x14ac:dyDescent="0.25">
       <c r="A24" s="73">
         <v>26</v>
       </c>
@@ -9799,7 +9799,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="25" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A25" s="73">
         <v>27</v>
       </c>
@@ -9832,7 +9832,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="26" spans="1:10" ht="44" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="26" spans="1:10" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A26" s="76">
         <v>28</v>
       </c>
@@ -9867,7 +9867,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="27" spans="1:10" ht="29" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:10" ht="30" x14ac:dyDescent="0.25">
       <c r="A27" s="72">
         <v>29</v>
       </c>
@@ -9902,7 +9902,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="28" spans="1:10" ht="29" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:10" ht="30" x14ac:dyDescent="0.25">
       <c r="A28" s="73">
         <v>30</v>
       </c>
@@ -9935,7 +9935,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="29" spans="1:10" ht="29" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:10" ht="30" x14ac:dyDescent="0.25">
       <c r="A29" s="73">
         <v>31</v>
       </c>
@@ -9968,7 +9968,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="30" spans="1:10" ht="44" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="30" spans="1:10" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A30" s="74">
         <v>32</v>
       </c>
@@ -10003,7 +10003,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="31" spans="1:10" ht="29" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:10" ht="30" x14ac:dyDescent="0.25">
       <c r="A31" s="72">
         <v>33</v>
       </c>
@@ -10038,7 +10038,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="32" spans="1:10" ht="29" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:10" ht="30" x14ac:dyDescent="0.25">
       <c r="A32" s="73">
         <v>34</v>
       </c>
@@ -10049,7 +10049,7 @@
         <v>44</v>
       </c>
       <c r="D32" s="20" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E32" s="17" t="b">
         <v>1</v>
@@ -10058,9 +10058,9 @@
       <c r="G32" s="2">
         <v>1</v>
       </c>
-      <c r="H32" s="13" t="str">
+      <c r="H32" s="13">
         <f t="shared" si="0"/>
-        <v/>
+        <v>1</v>
       </c>
       <c r="I32" s="14">
         <f t="shared" si="1"/>
@@ -10068,10 +10068,10 @@
       </c>
       <c r="J32" s="42">
         <f t="shared" si="2"/>
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
-    <row r="33" spans="1:10" ht="29" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:10" ht="30" x14ac:dyDescent="0.25">
       <c r="A33" s="73">
         <v>35</v>
       </c>
@@ -10106,7 +10106,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="34" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="34" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A34" s="74">
         <v>36</v>
       </c>
@@ -10139,7 +10139,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="35" spans="1:10" ht="29" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:10" ht="30" x14ac:dyDescent="0.25">
       <c r="A35" s="72">
         <v>37</v>
       </c>
@@ -10174,7 +10174,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="36" spans="1:10" ht="29" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:10" ht="30" x14ac:dyDescent="0.25">
       <c r="A36" s="73">
         <v>38</v>
       </c>
@@ -10209,7 +10209,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="37" spans="1:10" ht="29" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:10" ht="30" x14ac:dyDescent="0.25">
       <c r="A37" s="73">
         <v>39</v>
       </c>
@@ -10244,7 +10244,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="38" spans="1:10" s="1" customFormat="1" ht="29" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:10" s="1" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A38" s="73">
         <v>40</v>
       </c>
@@ -10279,7 +10279,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="39" spans="1:10" s="1" customFormat="1" ht="29.5" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="39" spans="1:10" s="1" customFormat="1" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A39" s="74">
         <v>41</v>
       </c>
@@ -10346,7 +10346,7 @@
                   </from>
                   <to>
                     <xdr:col>4</xdr:col>
-                    <xdr:colOff>107950</xdr:colOff>
+                    <xdr:colOff>104775</xdr:colOff>
                     <xdr:row>1</xdr:row>
                     <xdr:rowOff>209550</xdr:rowOff>
                   </to>
@@ -10368,7 +10368,7 @@
                   </from>
                   <to>
                     <xdr:col>4</xdr:col>
-                    <xdr:colOff>107950</xdr:colOff>
+                    <xdr:colOff>104775</xdr:colOff>
                     <xdr:row>2</xdr:row>
                     <xdr:rowOff>209550</xdr:rowOff>
                   </to>
@@ -10390,7 +10390,7 @@
                   </from>
                   <to>
                     <xdr:col>4</xdr:col>
-                    <xdr:colOff>107950</xdr:colOff>
+                    <xdr:colOff>104775</xdr:colOff>
                     <xdr:row>3</xdr:row>
                     <xdr:rowOff>381000</xdr:rowOff>
                   </to>
@@ -10412,9 +10412,9 @@
                   </from>
                   <to>
                     <xdr:col>4</xdr:col>
-                    <xdr:colOff>107950</xdr:colOff>
+                    <xdr:colOff>104775</xdr:colOff>
                     <xdr:row>4</xdr:row>
-                    <xdr:rowOff>717550</xdr:rowOff>
+                    <xdr:rowOff>714375</xdr:rowOff>
                   </to>
                 </anchor>
               </controlPr>
@@ -10428,7 +10428,7 @@
                 <anchor moveWithCells="1">
                   <from>
                     <xdr:col>3</xdr:col>
-                    <xdr:colOff>31750</xdr:colOff>
+                    <xdr:colOff>28575</xdr:colOff>
                     <xdr:row>5</xdr:row>
                     <xdr:rowOff>19050</xdr:rowOff>
                   </from>
@@ -10456,9 +10456,9 @@
                   </from>
                   <to>
                     <xdr:col>4</xdr:col>
-                    <xdr:colOff>107950</xdr:colOff>
+                    <xdr:colOff>104775</xdr:colOff>
                     <xdr:row>7</xdr:row>
-                    <xdr:rowOff>69850</xdr:rowOff>
+                    <xdr:rowOff>66675</xdr:rowOff>
                   </to>
                 </anchor>
               </controlPr>
@@ -10478,7 +10478,7 @@
                   </from>
                   <to>
                     <xdr:col>4</xdr:col>
-                    <xdr:colOff>107950</xdr:colOff>
+                    <xdr:colOff>104775</xdr:colOff>
                     <xdr:row>7</xdr:row>
                     <xdr:rowOff>209550</xdr:rowOff>
                   </to>
@@ -10500,9 +10500,9 @@
                   </from>
                   <to>
                     <xdr:col>4</xdr:col>
-                    <xdr:colOff>107950</xdr:colOff>
+                    <xdr:colOff>104775</xdr:colOff>
                     <xdr:row>8</xdr:row>
-                    <xdr:rowOff>127000</xdr:rowOff>
+                    <xdr:rowOff>123825</xdr:rowOff>
                   </to>
                 </anchor>
               </controlPr>
@@ -10522,7 +10522,7 @@
                   </from>
                   <to>
                     <xdr:col>4</xdr:col>
-                    <xdr:colOff>107950</xdr:colOff>
+                    <xdr:colOff>104775</xdr:colOff>
                     <xdr:row>10</xdr:row>
                     <xdr:rowOff>0</xdr:rowOff>
                   </to>
@@ -10544,7 +10544,7 @@
                   </from>
                   <to>
                     <xdr:col>4</xdr:col>
-                    <xdr:colOff>107950</xdr:colOff>
+                    <xdr:colOff>104775</xdr:colOff>
                     <xdr:row>11</xdr:row>
                     <xdr:rowOff>0</xdr:rowOff>
                   </to>
@@ -10566,7 +10566,7 @@
                   </from>
                   <to>
                     <xdr:col>4</xdr:col>
-                    <xdr:colOff>107950</xdr:colOff>
+                    <xdr:colOff>104775</xdr:colOff>
                     <xdr:row>11</xdr:row>
                     <xdr:rowOff>209550</xdr:rowOff>
                   </to>
@@ -10588,7 +10588,7 @@
                   </from>
                   <to>
                     <xdr:col>3</xdr:col>
-                    <xdr:colOff>660400</xdr:colOff>
+                    <xdr:colOff>657225</xdr:colOff>
                     <xdr:row>12</xdr:row>
                     <xdr:rowOff>571500</xdr:rowOff>
                   </to>
@@ -10610,7 +10610,7 @@
                   </from>
                   <to>
                     <xdr:col>4</xdr:col>
-                    <xdr:colOff>107950</xdr:colOff>
+                    <xdr:colOff>104775</xdr:colOff>
                     <xdr:row>13</xdr:row>
                     <xdr:rowOff>381000</xdr:rowOff>
                   </to>
@@ -10632,7 +10632,7 @@
                   </from>
                   <to>
                     <xdr:col>4</xdr:col>
-                    <xdr:colOff>107950</xdr:colOff>
+                    <xdr:colOff>104775</xdr:colOff>
                     <xdr:row>14</xdr:row>
                     <xdr:rowOff>209550</xdr:rowOff>
                   </to>
@@ -10654,9 +10654,9 @@
                   </from>
                   <to>
                     <xdr:col>4</xdr:col>
-                    <xdr:colOff>107950</xdr:colOff>
+                    <xdr:colOff>104775</xdr:colOff>
                     <xdr:row>15</xdr:row>
-                    <xdr:rowOff>336550</xdr:rowOff>
+                    <xdr:rowOff>333375</xdr:rowOff>
                   </to>
                 </anchor>
               </controlPr>
@@ -10676,7 +10676,7 @@
                   </from>
                   <to>
                     <xdr:col>4</xdr:col>
-                    <xdr:colOff>107950</xdr:colOff>
+                    <xdr:colOff>104775</xdr:colOff>
                     <xdr:row>17</xdr:row>
                     <xdr:rowOff>0</xdr:rowOff>
                   </to>
@@ -10698,9 +10698,9 @@
                   </from>
                   <to>
                     <xdr:col>4</xdr:col>
-                    <xdr:colOff>107950</xdr:colOff>
+                    <xdr:colOff>104775</xdr:colOff>
                     <xdr:row>17</xdr:row>
-                    <xdr:rowOff>127000</xdr:rowOff>
+                    <xdr:rowOff>123825</xdr:rowOff>
                   </to>
                 </anchor>
               </controlPr>
@@ -10720,7 +10720,7 @@
                   </from>
                   <to>
                     <xdr:col>4</xdr:col>
-                    <xdr:colOff>107950</xdr:colOff>
+                    <xdr:colOff>104775</xdr:colOff>
                     <xdr:row>18</xdr:row>
                     <xdr:rowOff>133350</xdr:rowOff>
                   </to>
@@ -10742,7 +10742,7 @@
                   </from>
                   <to>
                     <xdr:col>4</xdr:col>
-                    <xdr:colOff>107950</xdr:colOff>
+                    <xdr:colOff>104775</xdr:colOff>
                     <xdr:row>20</xdr:row>
                     <xdr:rowOff>0</xdr:rowOff>
                   </to>
@@ -10764,7 +10764,7 @@
                   </from>
                   <to>
                     <xdr:col>4</xdr:col>
-                    <xdr:colOff>107950</xdr:colOff>
+                    <xdr:colOff>104775</xdr:colOff>
                     <xdr:row>20</xdr:row>
                     <xdr:rowOff>209550</xdr:rowOff>
                   </to>
@@ -10786,7 +10786,7 @@
                   </from>
                   <to>
                     <xdr:col>4</xdr:col>
-                    <xdr:colOff>107950</xdr:colOff>
+                    <xdr:colOff>104775</xdr:colOff>
                     <xdr:row>22</xdr:row>
                     <xdr:rowOff>0</xdr:rowOff>
                   </to>
@@ -10808,7 +10808,7 @@
                   </from>
                   <to>
                     <xdr:col>4</xdr:col>
-                    <xdr:colOff>107950</xdr:colOff>
+                    <xdr:colOff>104775</xdr:colOff>
                     <xdr:row>22</xdr:row>
                     <xdr:rowOff>209550</xdr:rowOff>
                   </to>
@@ -10830,7 +10830,7 @@
                   </from>
                   <to>
                     <xdr:col>4</xdr:col>
-                    <xdr:colOff>107950</xdr:colOff>
+                    <xdr:colOff>104775</xdr:colOff>
                     <xdr:row>23</xdr:row>
                     <xdr:rowOff>209550</xdr:rowOff>
                   </to>
@@ -10852,9 +10852,9 @@
                   </from>
                   <to>
                     <xdr:col>4</xdr:col>
-                    <xdr:colOff>107950</xdr:colOff>
+                    <xdr:colOff>104775</xdr:colOff>
                     <xdr:row>24</xdr:row>
-                    <xdr:rowOff>127000</xdr:rowOff>
+                    <xdr:rowOff>123825</xdr:rowOff>
                   </to>
                 </anchor>
               </controlPr>
@@ -10874,7 +10874,7 @@
                   </from>
                   <to>
                     <xdr:col>4</xdr:col>
-                    <xdr:colOff>107950</xdr:colOff>
+                    <xdr:colOff>104775</xdr:colOff>
                     <xdr:row>26</xdr:row>
                     <xdr:rowOff>0</xdr:rowOff>
                   </to>
@@ -10896,7 +10896,7 @@
                   </from>
                   <to>
                     <xdr:col>4</xdr:col>
-                    <xdr:colOff>107950</xdr:colOff>
+                    <xdr:colOff>104775</xdr:colOff>
                     <xdr:row>27</xdr:row>
                     <xdr:rowOff>0</xdr:rowOff>
                   </to>
@@ -10918,7 +10918,7 @@
                   </from>
                   <to>
                     <xdr:col>4</xdr:col>
-                    <xdr:colOff>107950</xdr:colOff>
+                    <xdr:colOff>104775</xdr:colOff>
                     <xdr:row>27</xdr:row>
                     <xdr:rowOff>209550</xdr:rowOff>
                   </to>
@@ -10940,9 +10940,9 @@
                   </from>
                   <to>
                     <xdr:col>4</xdr:col>
-                    <xdr:colOff>107950</xdr:colOff>
+                    <xdr:colOff>104775</xdr:colOff>
                     <xdr:row>28</xdr:row>
-                    <xdr:rowOff>355600</xdr:rowOff>
+                    <xdr:rowOff>352425</xdr:rowOff>
                   </to>
                 </anchor>
               </controlPr>
@@ -10962,7 +10962,7 @@
                   </from>
                   <to>
                     <xdr:col>4</xdr:col>
-                    <xdr:colOff>107950</xdr:colOff>
+                    <xdr:colOff>104775</xdr:colOff>
                     <xdr:row>30</xdr:row>
                     <xdr:rowOff>0</xdr:rowOff>
                   </to>
@@ -10984,7 +10984,7 @@
                   </from>
                   <to>
                     <xdr:col>4</xdr:col>
-                    <xdr:colOff>107950</xdr:colOff>
+                    <xdr:colOff>104775</xdr:colOff>
                     <xdr:row>30</xdr:row>
                     <xdr:rowOff>209550</xdr:rowOff>
                   </to>
@@ -11006,7 +11006,7 @@
                   </from>
                   <to>
                     <xdr:col>4</xdr:col>
-                    <xdr:colOff>107950</xdr:colOff>
+                    <xdr:colOff>104775</xdr:colOff>
                     <xdr:row>32</xdr:row>
                     <xdr:rowOff>0</xdr:rowOff>
                   </to>
@@ -11028,7 +11028,7 @@
                   </from>
                   <to>
                     <xdr:col>4</xdr:col>
-                    <xdr:colOff>107950</xdr:colOff>
+                    <xdr:colOff>104775</xdr:colOff>
                     <xdr:row>32</xdr:row>
                     <xdr:rowOff>209550</xdr:rowOff>
                   </to>
@@ -11050,9 +11050,9 @@
                   </from>
                   <to>
                     <xdr:col>4</xdr:col>
-                    <xdr:colOff>107950</xdr:colOff>
+                    <xdr:colOff>104775</xdr:colOff>
                     <xdr:row>33</xdr:row>
-                    <xdr:rowOff>184150</xdr:rowOff>
+                    <xdr:rowOff>180975</xdr:rowOff>
                   </to>
                 </anchor>
               </controlPr>
@@ -11072,9 +11072,9 @@
                   </from>
                   <to>
                     <xdr:col>4</xdr:col>
-                    <xdr:colOff>107950</xdr:colOff>
+                    <xdr:colOff>104775</xdr:colOff>
                     <xdr:row>35</xdr:row>
-                    <xdr:rowOff>12700</xdr:rowOff>
+                    <xdr:rowOff>9525</xdr:rowOff>
                   </to>
                 </anchor>
               </controlPr>
@@ -11094,7 +11094,7 @@
                   </from>
                   <to>
                     <xdr:col>4</xdr:col>
-                    <xdr:colOff>107950</xdr:colOff>
+                    <xdr:colOff>104775</xdr:colOff>
                     <xdr:row>35</xdr:row>
                     <xdr:rowOff>209550</xdr:rowOff>
                   </to>
@@ -11116,9 +11116,9 @@
                   </from>
                   <to>
                     <xdr:col>4</xdr:col>
-                    <xdr:colOff>107950</xdr:colOff>
+                    <xdr:colOff>104775</xdr:colOff>
                     <xdr:row>36</xdr:row>
-                    <xdr:rowOff>374650</xdr:rowOff>
+                    <xdr:rowOff>371475</xdr:rowOff>
                   </to>
                 </anchor>
               </controlPr>
@@ -11138,7 +11138,7 @@
                   </from>
                   <to>
                     <xdr:col>4</xdr:col>
-                    <xdr:colOff>107950</xdr:colOff>
+                    <xdr:colOff>104775</xdr:colOff>
                     <xdr:row>37</xdr:row>
                     <xdr:rowOff>323850</xdr:rowOff>
                   </to>
@@ -11160,7 +11160,7 @@
                   </from>
                   <to>
                     <xdr:col>4</xdr:col>
-                    <xdr:colOff>107950</xdr:colOff>
+                    <xdr:colOff>104775</xdr:colOff>
                     <xdr:row>38</xdr:row>
                     <xdr:rowOff>381000</xdr:rowOff>
                   </to>
@@ -11250,7 +11250,7 @@
                     <xdr:col>5</xdr:col>
                     <xdr:colOff>152400</xdr:colOff>
                     <xdr:row>4</xdr:row>
-                    <xdr:rowOff>717550</xdr:rowOff>
+                    <xdr:rowOff>714375</xdr:rowOff>
                   </to>
                 </anchor>
               </controlPr>
@@ -11266,7 +11266,7 @@
                     <xdr:col>4</xdr:col>
                     <xdr:colOff>0</xdr:colOff>
                     <xdr:row>5</xdr:row>
-                    <xdr:rowOff>12700</xdr:rowOff>
+                    <xdr:rowOff>9525</xdr:rowOff>
                   </from>
                   <to>
                     <xdr:col>4</xdr:col>
@@ -11294,7 +11294,7 @@
                     <xdr:col>5</xdr:col>
                     <xdr:colOff>152400</xdr:colOff>
                     <xdr:row>7</xdr:row>
-                    <xdr:rowOff>69850</xdr:rowOff>
+                    <xdr:rowOff>66675</xdr:rowOff>
                   </to>
                 </anchor>
               </controlPr>
@@ -11338,7 +11338,7 @@
                     <xdr:col>5</xdr:col>
                     <xdr:colOff>152400</xdr:colOff>
                     <xdr:row>8</xdr:row>
-                    <xdr:rowOff>127000</xdr:rowOff>
+                    <xdr:rowOff>123825</xdr:rowOff>
                   </to>
                 </anchor>
               </controlPr>
@@ -11424,7 +11424,7 @@
                   </from>
                   <to>
                     <xdr:col>4</xdr:col>
-                    <xdr:colOff>698500</xdr:colOff>
+                    <xdr:colOff>695325</xdr:colOff>
                     <xdr:row>12</xdr:row>
                     <xdr:rowOff>571500</xdr:rowOff>
                   </to>
@@ -11492,7 +11492,7 @@
                     <xdr:col>5</xdr:col>
                     <xdr:colOff>152400</xdr:colOff>
                     <xdr:row>15</xdr:row>
-                    <xdr:rowOff>336550</xdr:rowOff>
+                    <xdr:rowOff>333375</xdr:rowOff>
                   </to>
                 </anchor>
               </controlPr>
@@ -11536,7 +11536,7 @@
                     <xdr:col>5</xdr:col>
                     <xdr:colOff>152400</xdr:colOff>
                     <xdr:row>17</xdr:row>
-                    <xdr:rowOff>127000</xdr:rowOff>
+                    <xdr:rowOff>123825</xdr:rowOff>
                   </to>
                 </anchor>
               </controlPr>
@@ -11690,7 +11690,7 @@
                     <xdr:col>5</xdr:col>
                     <xdr:colOff>152400</xdr:colOff>
                     <xdr:row>24</xdr:row>
-                    <xdr:rowOff>127000</xdr:rowOff>
+                    <xdr:rowOff>123825</xdr:rowOff>
                   </to>
                 </anchor>
               </controlPr>
@@ -11888,7 +11888,7 @@
                     <xdr:col>5</xdr:col>
                     <xdr:colOff>152400</xdr:colOff>
                     <xdr:row>34</xdr:row>
-                    <xdr:rowOff>31750</xdr:rowOff>
+                    <xdr:rowOff>28575</xdr:rowOff>
                   </to>
                 </anchor>
               </controlPr>
@@ -11910,7 +11910,7 @@
                     <xdr:col>5</xdr:col>
                     <xdr:colOff>152400</xdr:colOff>
                     <xdr:row>35</xdr:row>
-                    <xdr:rowOff>12700</xdr:rowOff>
+                    <xdr:rowOff>9525</xdr:rowOff>
                   </to>
                 </anchor>
               </controlPr>
@@ -11970,13 +11970,13 @@
                     <xdr:col>4</xdr:col>
                     <xdr:colOff>19050</xdr:colOff>
                     <xdr:row>37</xdr:row>
-                    <xdr:rowOff>88900</xdr:rowOff>
+                    <xdr:rowOff>85725</xdr:rowOff>
                   </from>
                   <to>
                     <xdr:col>5</xdr:col>
                     <xdr:colOff>171450</xdr:colOff>
                     <xdr:row>37</xdr:row>
-                    <xdr:rowOff>298450</xdr:rowOff>
+                    <xdr:rowOff>295275</xdr:rowOff>
                   </to>
                 </anchor>
               </controlPr>
@@ -12016,21 +12016,21 @@
   <sheetPr codeName="Munka6"/>
   <dimension ref="A1:H19"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="9.1796875" style="10"/>
-    <col min="3" max="3" width="11.7265625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="17.7265625" customWidth="1"/>
-    <col min="7" max="7" width="16.453125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="13.7265625" customWidth="1"/>
-    <col min="13" max="13" width="13.26953125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="9.140625" style="10"/>
+    <col min="3" max="3" width="11.7109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="17.7109375" customWidth="1"/>
+    <col min="7" max="7" width="16.42578125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="13.7109375" customWidth="1"/>
+    <col min="13" max="13" width="13.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:8" x14ac:dyDescent="0.35">
+    <row r="1" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B1" s="11" t="s">
         <v>31</v>
       </c>
@@ -12043,7 +12043,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="2" spans="2:8" x14ac:dyDescent="0.35">
+    <row r="2" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B2" s="2"/>
       <c r="C2" s="2">
         <v>140</v>
@@ -12056,7 +12056,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="3" spans="2:8" x14ac:dyDescent="0.35">
+    <row r="3" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B3" s="8">
         <v>0.4</v>
       </c>
@@ -12073,7 +12073,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="4" spans="2:8" x14ac:dyDescent="0.35">
+    <row r="4" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B4" s="8">
         <v>0.55000000000000004</v>
       </c>
@@ -12091,7 +12091,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="5" spans="2:8" x14ac:dyDescent="0.35">
+    <row r="5" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B5" s="8">
         <v>0.7</v>
       </c>
@@ -12109,7 +12109,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="6" spans="2:8" x14ac:dyDescent="0.35">
+    <row r="6" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B6" s="8">
         <v>0.85</v>
       </c>
@@ -12127,7 +12127,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="7" spans="2:8" x14ac:dyDescent="0.35">
+    <row r="7" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B7" s="8">
         <v>1</v>
       </c>
@@ -12145,7 +12145,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="8" spans="2:8" x14ac:dyDescent="0.35">
+    <row r="8" spans="2:8" x14ac:dyDescent="0.25">
       <c r="D8" s="5"/>
       <c r="G8">
         <v>12</v>
@@ -12154,7 +12154,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="9" spans="2:8" x14ac:dyDescent="0.35">
+    <row r="9" spans="2:8" x14ac:dyDescent="0.25">
       <c r="G9">
         <v>14</v>
       </c>
@@ -12162,7 +12162,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="10" spans="2:8" x14ac:dyDescent="0.35">
+    <row r="10" spans="2:8" x14ac:dyDescent="0.25">
       <c r="G10">
         <v>16</v>
       </c>
@@ -12170,7 +12170,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="11" spans="2:8" x14ac:dyDescent="0.35">
+    <row r="11" spans="2:8" x14ac:dyDescent="0.25">
       <c r="G11">
         <v>18</v>
       </c>
@@ -12178,7 +12178,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="12" spans="2:8" x14ac:dyDescent="0.35">
+    <row r="12" spans="2:8" x14ac:dyDescent="0.25">
       <c r="G12">
         <v>20</v>
       </c>
@@ -12186,7 +12186,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="2:2" x14ac:dyDescent="0.35">
+    <row r="19" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B19" s="1"/>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
oldal publikálása, kisebb hibajavítások
</commit_message>
<xml_diff>
--- a/egyebek/WebprogramozásBeadandóHtmlCssBootstrap.xlsx
+++ b/egyebek/WebprogramozásBeadandóHtmlCssBootstrap.xlsx
@@ -5,11 +5,11 @@
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Latitude\OneDrive\Dokumentumok\Suli\Közgáz\Programozás\Webprogramozás\Beadandó\egyebek\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Latitude\OneDrive\Dokumentumok\Suli\Közgáz\9.osztály\Programozás\Webprogramozás\Beadandó\egyebek\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="6350"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="14380" windowHeight="3520"/>
   </bookViews>
   <sheets>
     <sheet name="Fedőlap" sheetId="2" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="110" uniqueCount="79">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="113" uniqueCount="82">
   <si>
     <t>Neved:</t>
   </si>
@@ -301,6 +301,15 @@
   </si>
   <si>
     <t>Minden értékre (szín, méret) használj változókat.</t>
+  </si>
+  <si>
+    <t>Bekker Barnabás, Hegedűs Gergő</t>
+  </si>
+  <si>
+    <t>bekker.barnabas@ckik.hu hegedus.gergo@ckik.hu</t>
+  </si>
+  <si>
+    <t>https://sparkly-hamster-15669d.netlify.app/alap</t>
   </si>
 </sst>
 </file>
@@ -1196,6 +1205,12 @@
     <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
     <xf numFmtId="0" fontId="17" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1219,12 +1234,6 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="2" applyBorder="1" applyAlignment="1" applyProtection="1">
       <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="14" fillId="3" borderId="0" xfId="2" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1311,7 +1320,7 @@
 </file>
 
 <file path=xl/ctrlProps/ctrlProp12.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" checked="Checked" fmlaLink="D13" lockText="1" noThreeD="1"/>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" fmlaLink="D13" lockText="1" noThreeD="1"/>
 </file>
 
 <file path=xl/ctrlProps/ctrlProp13.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1335,7 +1344,7 @@
 </file>
 
 <file path=xl/ctrlProps/ctrlProp18.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" checked="Checked" fmlaLink="D19" lockText="1" noThreeD="1"/>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" fmlaLink="D19" lockText="1" noThreeD="1"/>
 </file>
 
 <file path=xl/ctrlProps/ctrlProp19.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1599,7 +1608,7 @@
 </file>
 
 <file path=xl/ctrlProps/ctrlProp9.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" checked="Checked" fmlaLink="D10" lockText="1" noThreeD="1"/>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" fmlaLink="D10" lockText="1" noThreeD="1"/>
 </file>
 
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -8584,7 +8593,7 @@
   <sheetPr codeName="Munka1"/>
   <dimension ref="A1:J21"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" zoomScaleNormal="100" workbookViewId="0"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
@@ -8602,15 +8611,15 @@
   <sheetData>
     <row r="1" spans="1:10" ht="32.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A1" s="31"/>
-      <c r="B1" s="81" t="s">
+      <c r="B1" s="83" t="s">
         <v>45</v>
       </c>
-      <c r="C1" s="82"/>
-      <c r="D1" s="82"/>
-      <c r="E1" s="82"/>
-      <c r="F1" s="82"/>
-      <c r="G1" s="82"/>
-      <c r="H1" s="82"/>
+      <c r="C1" s="84"/>
+      <c r="D1" s="84"/>
+      <c r="E1" s="84"/>
+      <c r="F1" s="84"/>
+      <c r="G1" s="84"/>
+      <c r="H1" s="84"/>
       <c r="I1" s="31"/>
       <c r="J1" s="31"/>
     </row>
@@ -8619,12 +8628,14 @@
       <c r="B2" s="34" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="86"/>
-      <c r="D2" s="87"/>
-      <c r="E2" s="87"/>
-      <c r="F2" s="87"/>
-      <c r="G2" s="87"/>
-      <c r="H2" s="87"/>
+      <c r="C2" s="88" t="s">
+        <v>79</v>
+      </c>
+      <c r="D2" s="89"/>
+      <c r="E2" s="89"/>
+      <c r="F2" s="89"/>
+      <c r="G2" s="89"/>
+      <c r="H2" s="89"/>
       <c r="I2" s="31"/>
       <c r="J2" s="31"/>
     </row>
@@ -8633,12 +8644,14 @@
       <c r="B3" s="34" t="s">
         <v>1</v>
       </c>
-      <c r="C3" s="88"/>
-      <c r="D3" s="87"/>
-      <c r="E3" s="87"/>
-      <c r="F3" s="87"/>
-      <c r="G3" s="87"/>
-      <c r="H3" s="87"/>
+      <c r="C3" s="90" t="s">
+        <v>80</v>
+      </c>
+      <c r="D3" s="89"/>
+      <c r="E3" s="89"/>
+      <c r="F3" s="89"/>
+      <c r="G3" s="89"/>
+      <c r="H3" s="89"/>
       <c r="I3" s="31"/>
       <c r="J3" s="31"/>
     </row>
@@ -8647,7 +8660,9 @@
       <c r="B4" s="34" t="s">
         <v>3</v>
       </c>
-      <c r="C4" s="86"/>
+      <c r="C4" s="88" t="s">
+        <v>81</v>
+      </c>
       <c r="D4" s="92"/>
       <c r="E4" s="92"/>
       <c r="F4" s="92"/>
@@ -8725,10 +8740,10 @@
     </row>
     <row r="10" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A10" s="31"/>
-      <c r="B10" s="89" t="s">
+      <c r="B10" s="81" t="s">
         <v>30</v>
       </c>
-      <c r="C10" s="90"/>
+      <c r="C10" s="82"/>
       <c r="D10" s="78">
         <f>SUM(Irányelvek!G:G)</f>
         <v>80</v>
@@ -8744,10 +8759,10 @@
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A11" s="31"/>
-      <c r="B11" s="83" t="s">
+      <c r="B11" s="85" t="s">
         <v>36</v>
       </c>
-      <c r="C11" s="84"/>
+      <c r="C11" s="86"/>
       <c r="D11" s="79">
         <v>20</v>
       </c>
@@ -8760,10 +8775,10 @@
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A12" s="31"/>
-      <c r="B12" s="89" t="s">
+      <c r="B12" s="81" t="s">
         <v>58</v>
       </c>
-      <c r="C12" s="90"/>
+      <c r="C12" s="82"/>
       <c r="D12" s="78">
         <v>20</v>
       </c>
@@ -8776,10 +8791,10 @@
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A13" s="31"/>
-      <c r="B13" s="89" t="s">
+      <c r="B13" s="81" t="s">
         <v>59</v>
       </c>
-      <c r="C13" s="90"/>
+      <c r="C13" s="82"/>
       <c r="D13" s="78">
         <v>40</v>
       </c>
@@ -8818,13 +8833,13 @@
     </row>
     <row r="16" spans="1:10" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A16" s="31"/>
-      <c r="B16" s="89" t="s">
+      <c r="B16" s="81" t="s">
         <v>39</v>
       </c>
-      <c r="C16" s="90"/>
+      <c r="C16" s="82"/>
       <c r="D16" s="30" t="b">
         <f t="array" ref="D16">IF(COUNTIFS(Irányelvek!D2:D39,"=hamis",Irányelvek!F2:F39,"=Igaz")=0,TRUE,FALSE)</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E16" s="31"/>
       <c r="F16" s="31"/>
@@ -8835,13 +8850,13 @@
     </row>
     <row r="17" spans="1:10" ht="31.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A17" s="31"/>
-      <c r="B17" s="89" t="s">
+      <c r="B17" s="81" t="s">
         <v>32</v>
       </c>
-      <c r="C17" s="90"/>
+      <c r="C17" s="82"/>
       <c r="D17" s="33">
         <f>SUM(Irányelvek!H2:H39)</f>
-        <v>79</v>
+        <v>64</v>
       </c>
       <c r="E17" s="31"/>
       <c r="F17" s="97" t="str">
@@ -8861,7 +8876,7 @@
       <c r="C18" s="96"/>
       <c r="D18" s="36">
         <f>IF(D17&gt;D11,VLOOKUP(SUM(Irányelvek!J2:J39),Ponthatárok!G2:H12,2,TRUE),0)</f>
-        <v>20</v>
+        <v>16</v>
       </c>
       <c r="E18" s="31"/>
       <c r="F18" s="97"/>
@@ -8872,10 +8887,10 @@
     </row>
     <row r="19" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A19" s="31"/>
-      <c r="B19" s="89" t="s">
+      <c r="B19" s="81" t="s">
         <v>61</v>
       </c>
-      <c r="C19" s="90"/>
+      <c r="C19" s="82"/>
       <c r="D19" s="80">
         <v>40</v>
       </c>
@@ -8888,21 +8903,21 @@
     </row>
     <row r="20" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A20" s="31"/>
-      <c r="B20" s="89" t="s">
+      <c r="B20" s="81" t="s">
         <v>62</v>
       </c>
-      <c r="C20" s="90"/>
+      <c r="C20" s="82"/>
       <c r="D20" s="33">
         <f>SUM(D17:D19)</f>
-        <v>139</v>
+        <v>120</v>
       </c>
       <c r="E20" s="31"/>
-      <c r="F20" s="85" t="str">
+      <c r="F20" s="87" t="str">
         <f>CONCATENATE("Az önértékelés alapján ",VLOOKUP(D20,Ponthatárok!$C$3:$D$7,2,TRUE), "  érdemjegyet kapnál rá.")</f>
         <v>Az önértékelés alapján Jeles (5)  érdemjegyet kapnál rá.</v>
       </c>
-      <c r="G20" s="85"/>
-      <c r="H20" s="85"/>
+      <c r="G20" s="87"/>
+      <c r="H20" s="87"/>
       <c r="I20" s="31"/>
       <c r="J20" s="31"/>
     </row>
@@ -8921,6 +8936,8 @@
   </sheetData>
   <sheetProtection algorithmName="SHA-512" hashValue="Pt2r10NfCQvSDRx8qMjGYxYpEYBoOyIK56jWLg5u88pMtB0yZv+L45h/PZkvP5rgD0XQukcG0FY9SUv/PUWVng==" saltValue="OS0FMTO/1nXUT8EsxtE52w==" spinCount="100000" sheet="1" objects="1" scenarios="1"/>
   <mergeCells count="18">
+    <mergeCell ref="F17:H19"/>
+    <mergeCell ref="F10:H14"/>
     <mergeCell ref="B10:C10"/>
     <mergeCell ref="B16:C16"/>
     <mergeCell ref="B1:H1"/>
@@ -8937,8 +8954,6 @@
     <mergeCell ref="B12:C12"/>
     <mergeCell ref="B13:C13"/>
     <mergeCell ref="B18:C18"/>
-    <mergeCell ref="F17:H19"/>
-    <mergeCell ref="F10:H14"/>
   </mergeCells>
   <conditionalFormatting sqref="D17:D20">
     <cfRule type="expression" dxfId="2" priority="1" stopIfTrue="1">
@@ -8960,8 +8975,8 @@
   <dimension ref="A1:L39"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A35" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D19" sqref="D19"/>
+      <pane ySplit="1" topLeftCell="A21" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -9297,7 +9312,7 @@
         <v>51</v>
       </c>
       <c r="D10" s="20" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E10" s="17" t="b">
         <v>1</v>
@@ -9310,7 +9325,7 @@
       </c>
       <c r="H10" s="13">
         <f t="shared" si="0"/>
-        <v>5</v>
+        <v>-2</v>
       </c>
       <c r="I10" s="14">
         <f t="shared" si="1"/>
@@ -9318,7 +9333,7 @@
       </c>
       <c r="J10" s="42">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="11" spans="1:12" ht="29" x14ac:dyDescent="0.35">
@@ -9400,7 +9415,7 @@
         <v>71</v>
       </c>
       <c r="D13" s="21" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E13" s="19" t="b">
         <v>1</v>
@@ -9413,7 +9428,7 @@
       </c>
       <c r="H13" s="61">
         <f t="shared" si="0"/>
-        <v>5</v>
+        <v>-2</v>
       </c>
       <c r="I13" s="62">
         <f t="shared" si="1"/>
@@ -9421,7 +9436,7 @@
       </c>
       <c r="J13" s="63">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="14" spans="1:12" ht="43.5" x14ac:dyDescent="0.35">
@@ -9610,7 +9625,7 @@
         <v>12</v>
       </c>
       <c r="D19" s="60" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E19" s="57" t="b">
         <v>1</v>
@@ -9619,9 +9634,9 @@
       <c r="G19" s="39">
         <v>1</v>
       </c>
-      <c r="H19" s="39">
+      <c r="H19" s="39" t="str">
         <f t="shared" si="0"/>
-        <v>1</v>
+        <v/>
       </c>
       <c r="I19" s="40">
         <f t="shared" si="1"/>
@@ -9629,7 +9644,7 @@
       </c>
       <c r="J19" s="41">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="20" spans="1:10" ht="43.5" x14ac:dyDescent="0.35">

</xml_diff>